<commit_message>
Added setScreen() functionality (WIP)
</commit_message>
<xml_diff>
--- a/LCD User Interface.xlsx
+++ b/LCD User Interface.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Stromvy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9BD853-4838-4395-A510-77ACA2E49E95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46976388-7E1A-4FD2-8B1A-363CC4544458}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="88">
   <si>
     <t>x</t>
   </si>
@@ -225,15 +226,9 @@
     <t>l</t>
   </si>
   <si>
-    <t>Ton/ff</t>
-  </si>
-  <si>
     <t>deg</t>
   </si>
   <si>
-    <t>CUP/V/I</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -261,9 +256,6 @@
     <t>d</t>
   </si>
   <si>
-    <t>=</t>
-  </si>
-  <si>
     <t>SCREEN_LOG</t>
   </si>
   <si>
@@ -286,6 +278,18 @@
   </si>
   <si>
     <t>SCREEN_CAL</t>
+  </si>
+  <si>
+    <t>ON/OFF</t>
+  </si>
+  <si>
+    <t>Ton/Toff</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>)</t>
   </si>
 </sst>
 </file>
@@ -438,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -473,28 +477,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -508,6 +494,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -792,7 +805,7 @@
   <dimension ref="A1:AK150"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="Q46" sqref="Q46"/>
+      <selection activeCell="X35" sqref="X35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -803,75 +816,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
+      <c r="B1" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>0</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="G3" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="H3" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>61</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
         <v>4</v>
@@ -892,20 +909,20 @@
         <v>65</v>
       </c>
       <c r="Q3" s="1"/>
-      <c r="R3" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="S3" s="15"/>
-      <c r="T3" s="1"/>
+      <c r="R3" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="S3" s="22"/>
+      <c r="T3" s="21"/>
       <c r="U3" s="1"/>
-      <c r="W3" s="21"/>
-      <c r="X3" s="21"/>
-      <c r="Y3" s="21"/>
-      <c r="Z3" s="21"/>
-      <c r="AA3" s="21"/>
-      <c r="AB3" s="21"/>
-      <c r="AC3" s="21"/>
-      <c r="AD3" s="21"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="15"/>
+      <c r="AA3" s="15"/>
+      <c r="AB3" s="15"/>
+      <c r="AC3" s="15"/>
+      <c r="AD3" s="15"/>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
@@ -957,26 +974,20 @@
         <v>2</v>
       </c>
       <c r="Q4" s="1"/>
-      <c r="R4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="W4" s="21"/>
-      <c r="X4" s="21"/>
-      <c r="Y4" s="21"/>
-      <c r="Z4" s="21"/>
-      <c r="AA4" s="21"/>
-      <c r="AB4" s="21"/>
-      <c r="AC4" s="21"/>
-      <c r="AD4" s="21"/>
+      <c r="R4" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="S4" s="21"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="15"/>
+      <c r="AB4" s="15"/>
+      <c r="AC4" s="15"/>
+      <c r="AD4" s="15"/>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
@@ -1028,20 +1039,26 @@
         <v>4</v>
       </c>
       <c r="Q5" s="1"/>
-      <c r="R5" s="15" t="s">
+      <c r="R5" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="T5" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="W5" s="21"/>
-      <c r="X5" s="21"/>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="21"/>
-      <c r="AA5" s="21"/>
-      <c r="AB5" s="21"/>
-      <c r="AC5" s="21"/>
-      <c r="AD5" s="21"/>
+      <c r="U5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="15"/>
+      <c r="AD5" s="15"/>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
@@ -1075,7 +1092,7 @@
         <v>8</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>58</v>
@@ -1084,25 +1101,25 @@
         <v>12</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="1"/>
-      <c r="W6" s="21"/>
-      <c r="X6" s="21"/>
-      <c r="Y6" s="21"/>
-      <c r="Z6" s="21"/>
-      <c r="AA6" s="21"/>
-      <c r="AB6" s="21"/>
-      <c r="AC6" s="21"/>
-      <c r="AD6" s="21"/>
+      <c r="R6" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="S6" s="22"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="12"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="15"/>
+      <c r="AD6" s="15"/>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B7" s="11">
@@ -1165,86 +1182,86 @@
       <c r="U7" s="11">
         <v>19</v>
       </c>
-      <c r="W7" s="21"/>
-      <c r="X7" s="21"/>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="21"/>
-      <c r="AA7" s="21"/>
-      <c r="AB7" s="21"/>
-      <c r="AC7" s="21"/>
-      <c r="AD7" s="21"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="15"/>
+      <c r="AB7" s="15"/>
+      <c r="AC7" s="15"/>
+      <c r="AD7" s="15"/>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="W8" s="21"/>
-      <c r="X8" s="21"/>
-      <c r="Y8" s="21"/>
-      <c r="Z8" s="21"/>
-      <c r="AA8" s="21"/>
-      <c r="AB8" s="21"/>
-      <c r="AC8" s="21"/>
-      <c r="AD8" s="21"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
+      <c r="AA8" s="15"/>
+      <c r="AB8" s="15"/>
+      <c r="AC8" s="15"/>
+      <c r="AD8" s="15"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="12"/>
-      <c r="U9" s="12"/>
-      <c r="W9" s="21"/>
-      <c r="X9" s="21"/>
-      <c r="Y9" s="21"/>
-      <c r="Z9" s="21"/>
-      <c r="AA9" s="21"/>
-      <c r="AB9" s="21"/>
-      <c r="AC9" s="21"/>
-      <c r="AD9" s="21"/>
+      <c r="B9" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="18"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="15"/>
+      <c r="AB9" s="15"/>
+      <c r="AC9" s="15"/>
+      <c r="AD9" s="15"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
-      <c r="W10" s="21"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="21"/>
-      <c r="Z10" s="21"/>
-      <c r="AA10" s="21"/>
-      <c r="AB10" s="21"/>
-      <c r="AC10" s="21"/>
-      <c r="AD10" s="21"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
+      <c r="AA10" s="15"/>
+      <c r="AB10" s="15"/>
+      <c r="AC10" s="15"/>
+      <c r="AD10" s="15"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
@@ -1254,7 +1271,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>17</v>
@@ -1300,14 +1317,14 @@
       <c r="U11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W11" s="21"/>
-      <c r="X11" s="21"/>
-      <c r="Y11" s="21"/>
-      <c r="Z11" s="21"/>
-      <c r="AA11" s="21"/>
-      <c r="AB11" s="21"/>
-      <c r="AC11" s="21"/>
-      <c r="AD11" s="21"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="15"/>
+      <c r="AB11" s="15"/>
+      <c r="AC11" s="15"/>
+      <c r="AD11" s="15"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
@@ -1342,10 +1359,10 @@
         <v>19</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -1363,14 +1380,14 @@
       <c r="U12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="W12" s="21"/>
-      <c r="X12" s="21"/>
-      <c r="Y12" s="21"/>
-      <c r="Z12" s="21"/>
-      <c r="AA12" s="21"/>
-      <c r="AB12" s="21"/>
-      <c r="AC12" s="21"/>
-      <c r="AD12" s="21"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="15"/>
+      <c r="Y12" s="15"/>
+      <c r="Z12" s="15"/>
+      <c r="AA12" s="15"/>
+      <c r="AB12" s="15"/>
+      <c r="AC12" s="15"/>
+      <c r="AD12" s="15"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
@@ -1391,37 +1408,37 @@
       <c r="F13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="13" t="s">
         <v>14</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>0</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="I13" s="13"/>
       <c r="J13" s="7" t="s">
         <v>0</v>
       </c>
       <c r="K13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="L13" s="7" t="s">
-        <v>0</v>
-      </c>
       <c r="M13" s="7" t="s">
         <v>0</v>
       </c>
       <c r="N13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O13" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="P13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Q13" s="4"/>
+      <c r="Q13" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="R13" s="5" t="s">
         <v>8</v>
       </c>
@@ -1434,14 +1451,14 @@
       <c r="U13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="W13" s="21"/>
-      <c r="X13" s="21"/>
-      <c r="Y13" s="21"/>
-      <c r="Z13" s="21"/>
-      <c r="AA13" s="21"/>
-      <c r="AB13" s="21"/>
-      <c r="AC13" s="21"/>
-      <c r="AD13" s="21"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="15"/>
+      <c r="AD13" s="15"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
@@ -1451,7 +1468,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>17</v>
@@ -1467,7 +1484,7 @@
         <v>25</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>23</v>
@@ -1491,14 +1508,14 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
-      <c r="W14" s="21"/>
-      <c r="X14" s="21"/>
-      <c r="Y14" s="21"/>
-      <c r="Z14" s="21"/>
-      <c r="AA14" s="21"/>
-      <c r="AB14" s="21"/>
-      <c r="AC14" s="21"/>
-      <c r="AD14" s="21"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="15"/>
+      <c r="Z14" s="15"/>
+      <c r="AA14" s="15"/>
+      <c r="AB14" s="15"/>
+      <c r="AC14" s="15"/>
+      <c r="AD14" s="15"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B15" s="11">
@@ -1561,129 +1578,129 @@
       <c r="U15" s="11">
         <v>19</v>
       </c>
-      <c r="W15" s="21"/>
-      <c r="X15" s="21"/>
-      <c r="Y15" s="21"/>
-      <c r="Z15" s="21"/>
-      <c r="AA15" s="21"/>
-      <c r="AB15" s="21"/>
-      <c r="AC15" s="21"/>
-      <c r="AD15" s="21"/>
+      <c r="W15" s="15"/>
+      <c r="X15" s="15"/>
+      <c r="Y15" s="15"/>
+      <c r="Z15" s="15"/>
+      <c r="AA15" s="15"/>
+      <c r="AB15" s="15"/>
+      <c r="AC15" s="15"/>
+      <c r="AD15" s="15"/>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="22"/>
-      <c r="S16" s="22"/>
-      <c r="T16" s="22"/>
-      <c r="U16" s="22"/>
-      <c r="V16" s="22"/>
-      <c r="W16" s="22"/>
-      <c r="X16" s="22"/>
-      <c r="Y16" s="22"/>
-      <c r="Z16" s="22"/>
-      <c r="AA16" s="22"/>
-      <c r="AB16" s="22"/>
-      <c r="AC16" s="22"/>
-      <c r="AD16" s="22"/>
-      <c r="AE16" s="22"/>
-      <c r="AF16" s="22"/>
-      <c r="AG16" s="22"/>
-      <c r="AH16" s="22"/>
-      <c r="AI16" s="22"/>
-      <c r="AJ16" s="22"/>
-      <c r="AK16" s="22"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="16"/>
+      <c r="W16" s="16"/>
+      <c r="X16" s="16"/>
+      <c r="Y16" s="16"/>
+      <c r="Z16" s="16"/>
+      <c r="AA16" s="16"/>
+      <c r="AB16" s="16"/>
+      <c r="AC16" s="16"/>
+      <c r="AD16" s="16"/>
+      <c r="AE16" s="16"/>
+      <c r="AF16" s="16"/>
+      <c r="AG16" s="16"/>
+      <c r="AH16" s="16"/>
+      <c r="AI16" s="16"/>
+      <c r="AJ16" s="16"/>
+      <c r="AK16" s="16"/>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
-      <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
-      <c r="U17" s="12"/>
-      <c r="W17" s="21"/>
-      <c r="X17" s="21"/>
-      <c r="Y17" s="21"/>
-      <c r="Z17" s="21"/>
-      <c r="AA17" s="21"/>
-      <c r="AB17" s="21"/>
-      <c r="AC17" s="21"/>
-      <c r="AD17" s="22"/>
-      <c r="AE17" s="22"/>
-      <c r="AF17" s="22"/>
-      <c r="AG17" s="22"/>
-      <c r="AH17" s="22"/>
-      <c r="AI17" s="22"/>
-      <c r="AJ17" s="22"/>
-      <c r="AK17" s="22"/>
+      <c r="B17" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18"/>
+      <c r="S17" s="18"/>
+      <c r="T17" s="18"/>
+      <c r="U17" s="18"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="15"/>
+      <c r="AC17" s="15"/>
+      <c r="AD17" s="16"/>
+      <c r="AE17" s="16"/>
+      <c r="AF17" s="16"/>
+      <c r="AG17" s="16"/>
+      <c r="AH17" s="16"/>
+      <c r="AI17" s="16"/>
+      <c r="AJ17" s="16"/>
+      <c r="AK17" s="16"/>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
-      <c r="W18" s="21"/>
-      <c r="X18" s="21"/>
-      <c r="Y18" s="21"/>
-      <c r="Z18" s="21"/>
-      <c r="AA18" s="21"/>
-      <c r="AB18" s="21"/>
-      <c r="AC18" s="21"/>
-      <c r="AD18" s="22"/>
-      <c r="AE18" s="22"/>
-      <c r="AF18" s="22"/>
-      <c r="AG18" s="22"/>
-      <c r="AH18" s="22"/>
-      <c r="AI18" s="22"/>
-      <c r="AJ18" s="22"/>
-      <c r="AK18" s="22"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="19"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="15"/>
+      <c r="Z18" s="15"/>
+      <c r="AA18" s="15"/>
+      <c r="AB18" s="15"/>
+      <c r="AC18" s="15"/>
+      <c r="AD18" s="16"/>
+      <c r="AE18" s="16"/>
+      <c r="AF18" s="16"/>
+      <c r="AG18" s="16"/>
+      <c r="AH18" s="16"/>
+      <c r="AI18" s="16"/>
+      <c r="AJ18" s="16"/>
+      <c r="AK18" s="16"/>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
@@ -1711,55 +1728,57 @@
         <v>0</v>
       </c>
       <c r="I19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="K19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="L19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L19" s="2"/>
-      <c r="M19" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="N19" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="O19" s="7" t="s">
+      <c r="M19" s="4"/>
+      <c r="N19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="P19" s="7" t="s">
-        <v>0</v>
-      </c>
       <c r="Q19" s="7" t="s">
         <v>0</v>
       </c>
       <c r="R19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="S19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="S19" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="T19" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="U19" s="2"/>
-      <c r="W19" s="21"/>
-      <c r="X19" s="21"/>
-      <c r="Y19" s="21"/>
-      <c r="Z19" s="21"/>
-      <c r="AA19" s="21"/>
-      <c r="AB19" s="21"/>
-      <c r="AC19" s="21"/>
-      <c r="AD19" s="22"/>
-      <c r="AE19" s="22"/>
-      <c r="AF19" s="22"/>
-      <c r="AG19" s="22"/>
-      <c r="AH19" s="22"/>
-      <c r="AI19" s="22"/>
-      <c r="AJ19" s="22"/>
-      <c r="AK19" s="22"/>
+      <c r="U19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="W19" s="15"/>
+      <c r="X19" s="15"/>
+      <c r="Y19" s="15"/>
+      <c r="Z19" s="15"/>
+      <c r="AA19" s="15"/>
+      <c r="AB19" s="15"/>
+      <c r="AC19" s="15"/>
+      <c r="AD19" s="16"/>
+      <c r="AE19" s="16"/>
+      <c r="AF19" s="16"/>
+      <c r="AG19" s="16"/>
+      <c r="AH19" s="16"/>
+      <c r="AI19" s="16"/>
+      <c r="AJ19" s="16"/>
+      <c r="AK19" s="16"/>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
@@ -1787,15 +1806,17 @@
         <v>0</v>
       </c>
       <c r="I20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="K20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="L20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L20" s="2"/>
       <c r="M20" s="4"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -1805,21 +1826,21 @@
       <c r="S20" s="7"/>
       <c r="T20" s="7"/>
       <c r="U20" s="7"/>
-      <c r="W20" s="21"/>
-      <c r="X20" s="21"/>
-      <c r="Y20" s="21"/>
-      <c r="Z20" s="21"/>
-      <c r="AA20" s="21"/>
-      <c r="AB20" s="21"/>
-      <c r="AC20" s="21"/>
-      <c r="AD20" s="22"/>
-      <c r="AE20" s="22"/>
-      <c r="AF20" s="22"/>
-      <c r="AG20" s="22"/>
-      <c r="AH20" s="22"/>
-      <c r="AI20" s="22"/>
-      <c r="AJ20" s="22"/>
-      <c r="AK20" s="22"/>
+      <c r="W20" s="15"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="15"/>
+      <c r="Z20" s="15"/>
+      <c r="AA20" s="15"/>
+      <c r="AB20" s="15"/>
+      <c r="AC20" s="15"/>
+      <c r="AD20" s="16"/>
+      <c r="AE20" s="16"/>
+      <c r="AF20" s="16"/>
+      <c r="AG20" s="16"/>
+      <c r="AH20" s="16"/>
+      <c r="AI20" s="16"/>
+      <c r="AJ20" s="16"/>
+      <c r="AK20" s="16"/>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
@@ -1828,7 +1849,7 @@
       <c r="B21" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D21" s="7" t="s">
@@ -1854,13 +1875,13 @@
         <v>16</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>14</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
@@ -1869,21 +1890,21 @@
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
-      <c r="W21" s="21"/>
-      <c r="X21" s="21"/>
-      <c r="Y21" s="21"/>
-      <c r="Z21" s="21"/>
-      <c r="AA21" s="21"/>
-      <c r="AB21" s="21"/>
-      <c r="AC21" s="21"/>
-      <c r="AD21" s="22"/>
-      <c r="AE21" s="22"/>
-      <c r="AF21" s="22"/>
-      <c r="AG21" s="22"/>
-      <c r="AH21" s="22"/>
-      <c r="AI21" s="22"/>
-      <c r="AJ21" s="22"/>
-      <c r="AK21" s="22"/>
+      <c r="W21" s="15"/>
+      <c r="X21" s="15"/>
+      <c r="Y21" s="15"/>
+      <c r="Z21" s="15"/>
+      <c r="AA21" s="15"/>
+      <c r="AB21" s="15"/>
+      <c r="AC21" s="15"/>
+      <c r="AD21" s="16"/>
+      <c r="AE21" s="16"/>
+      <c r="AF21" s="16"/>
+      <c r="AG21" s="16"/>
+      <c r="AH21" s="16"/>
+      <c r="AI21" s="16"/>
+      <c r="AJ21" s="16"/>
+      <c r="AK21" s="16"/>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
@@ -1919,21 +1940,21 @@
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
-      <c r="W22" s="21"/>
-      <c r="X22" s="21"/>
-      <c r="Y22" s="21"/>
-      <c r="Z22" s="21"/>
-      <c r="AA22" s="21"/>
-      <c r="AB22" s="21"/>
-      <c r="AC22" s="21"/>
-      <c r="AD22" s="22"/>
-      <c r="AE22" s="22"/>
-      <c r="AF22" s="22"/>
-      <c r="AG22" s="22"/>
-      <c r="AH22" s="22"/>
-      <c r="AI22" s="22"/>
-      <c r="AJ22" s="22"/>
-      <c r="AK22" s="22"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
+      <c r="Z22" s="15"/>
+      <c r="AA22" s="15"/>
+      <c r="AB22" s="15"/>
+      <c r="AC22" s="15"/>
+      <c r="AD22" s="16"/>
+      <c r="AE22" s="16"/>
+      <c r="AF22" s="16"/>
+      <c r="AG22" s="16"/>
+      <c r="AH22" s="16"/>
+      <c r="AI22" s="16"/>
+      <c r="AJ22" s="16"/>
+      <c r="AK22" s="16"/>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B23" s="11">
@@ -1996,98 +2017,98 @@
       <c r="U23" s="11">
         <v>19</v>
       </c>
-      <c r="W23" s="21"/>
-      <c r="X23" s="21"/>
-      <c r="Y23" s="21"/>
-      <c r="Z23" s="21"/>
-      <c r="AA23" s="21"/>
-      <c r="AB23" s="21"/>
-      <c r="AC23" s="21"/>
-      <c r="AD23" s="22"/>
-      <c r="AE23" s="22"/>
-      <c r="AF23" s="22"/>
-      <c r="AG23" s="22"/>
-      <c r="AH23" s="22"/>
-      <c r="AI23" s="22"/>
-      <c r="AJ23" s="22"/>
-      <c r="AK23" s="22"/>
+      <c r="W23" s="15"/>
+      <c r="X23" s="15"/>
+      <c r="Y23" s="15"/>
+      <c r="Z23" s="15"/>
+      <c r="AA23" s="15"/>
+      <c r="AB23" s="15"/>
+      <c r="AC23" s="15"/>
+      <c r="AD23" s="16"/>
+      <c r="AE23" s="16"/>
+      <c r="AF23" s="16"/>
+      <c r="AG23" s="16"/>
+      <c r="AH23" s="16"/>
+      <c r="AI23" s="16"/>
+      <c r="AJ23" s="16"/>
+      <c r="AK23" s="16"/>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="AD24" s="22"/>
-      <c r="AE24" s="22"/>
-      <c r="AF24" s="22"/>
-      <c r="AG24" s="22"/>
-      <c r="AH24" s="22"/>
-      <c r="AI24" s="22"/>
-      <c r="AJ24" s="22"/>
-      <c r="AK24" s="22"/>
+      <c r="AD24" s="16"/>
+      <c r="AE24" s="16"/>
+      <c r="AF24" s="16"/>
+      <c r="AG24" s="16"/>
+      <c r="AH24" s="16"/>
+      <c r="AI24" s="16"/>
+      <c r="AJ24" s="16"/>
+      <c r="AK24" s="16"/>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B25" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="12"/>
-      <c r="Q25" s="12"/>
-      <c r="R25" s="12"/>
-      <c r="S25" s="12"/>
-      <c r="T25" s="12"/>
-      <c r="U25" s="12"/>
-      <c r="AE25" s="22"/>
-      <c r="AF25" s="22"/>
-      <c r="AG25" s="22"/>
-      <c r="AH25" s="22"/>
-      <c r="AI25" s="22"/>
-      <c r="AJ25" s="22"/>
-      <c r="AK25" s="22"/>
+      <c r="B25" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
+      <c r="S25" s="18"/>
+      <c r="T25" s="18"/>
+      <c r="U25" s="18"/>
+      <c r="AE25" s="16"/>
+      <c r="AF25" s="16"/>
+      <c r="AG25" s="16"/>
+      <c r="AH25" s="16"/>
+      <c r="AI25" s="16"/>
+      <c r="AJ25" s="16"/>
+      <c r="AK25" s="16"/>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
-      <c r="T26" s="13"/>
-      <c r="U26" s="13"/>
-      <c r="AE26" s="22"/>
-      <c r="AF26" s="22"/>
-      <c r="AG26" s="22"/>
-      <c r="AH26" s="22"/>
-      <c r="AI26" s="22"/>
-      <c r="AJ26" s="22"/>
-      <c r="AK26" s="22"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
+      <c r="AE26" s="16"/>
+      <c r="AF26" s="16"/>
+      <c r="AG26" s="16"/>
+      <c r="AH26" s="16"/>
+      <c r="AI26" s="16"/>
+      <c r="AJ26" s="16"/>
+      <c r="AK26" s="16"/>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>0</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>4</v>
@@ -2106,10 +2127,10 @@
         <v>9</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>11</v>
@@ -2118,34 +2139,38 @@
         <v>12</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="N27" s="4"/>
       <c r="O27" s="4" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="P27" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q27" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="Q27" s="4" t="s">
+      <c r="R27" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="R27" s="4" t="s">
+      <c r="S27" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S27" s="4"/>
-      <c r="T27" s="4"/>
+      <c r="T27" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="U27" s="4"/>
-      <c r="W27" s="21"/>
-      <c r="X27" s="21"/>
-      <c r="Y27" s="21"/>
-      <c r="AE27" s="22"/>
-      <c r="AF27" s="22"/>
-      <c r="AG27" s="22"/>
-      <c r="AH27" s="22"/>
-      <c r="AI27" s="22"/>
-      <c r="AJ27" s="22"/>
-      <c r="AK27" s="22"/>
+      <c r="W27" s="15"/>
+      <c r="X27" s="15"/>
+      <c r="Y27" s="15"/>
+      <c r="AE27" s="16"/>
+      <c r="AF27" s="16"/>
+      <c r="AG27" s="16"/>
+      <c r="AH27" s="16"/>
+      <c r="AI27" s="16"/>
+      <c r="AJ27" s="16"/>
+      <c r="AK27" s="16"/>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
@@ -2154,16 +2179,16 @@
       <c r="B28" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="19"/>
+      <c r="C28" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="26"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
@@ -2175,16 +2200,16 @@
       <c r="S28" s="4"/>
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
-      <c r="W28" s="21"/>
-      <c r="X28" s="21"/>
-      <c r="Y28" s="21"/>
-      <c r="AE28" s="22"/>
-      <c r="AF28" s="22"/>
-      <c r="AG28" s="22"/>
-      <c r="AH28" s="22"/>
-      <c r="AI28" s="22"/>
-      <c r="AJ28" s="22"/>
-      <c r="AK28" s="22"/>
+      <c r="W28" s="15"/>
+      <c r="X28" s="15"/>
+      <c r="Y28" s="15"/>
+      <c r="AE28" s="16"/>
+      <c r="AF28" s="16"/>
+      <c r="AG28" s="16"/>
+      <c r="AH28" s="16"/>
+      <c r="AI28" s="16"/>
+      <c r="AJ28" s="16"/>
+      <c r="AK28" s="16"/>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
@@ -2209,7 +2234,7 @@
         <v>14</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>17</v>
@@ -2244,16 +2269,16 @@
       <c r="S29" s="4"/>
       <c r="T29" s="4"/>
       <c r="U29" s="4"/>
-      <c r="W29" s="21"/>
-      <c r="X29" s="21"/>
-      <c r="Y29" s="21"/>
-      <c r="AE29" s="22"/>
-      <c r="AF29" s="22"/>
-      <c r="AG29" s="22"/>
-      <c r="AH29" s="22"/>
-      <c r="AI29" s="22"/>
-      <c r="AJ29" s="22"/>
-      <c r="AK29" s="22"/>
+      <c r="W29" s="15"/>
+      <c r="X29" s="15"/>
+      <c r="Y29" s="15"/>
+      <c r="AE29" s="16"/>
+      <c r="AF29" s="16"/>
+      <c r="AG29" s="16"/>
+      <c r="AH29" s="16"/>
+      <c r="AI29" s="16"/>
+      <c r="AJ29" s="16"/>
+      <c r="AK29" s="16"/>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
@@ -2289,16 +2314,16 @@
       <c r="S30" s="4"/>
       <c r="T30" s="4"/>
       <c r="U30" s="4"/>
-      <c r="W30" s="21"/>
-      <c r="X30" s="21"/>
-      <c r="Y30" s="21"/>
-      <c r="AE30" s="22"/>
-      <c r="AF30" s="22"/>
-      <c r="AG30" s="22"/>
-      <c r="AH30" s="22"/>
-      <c r="AI30" s="22"/>
-      <c r="AJ30" s="22"/>
-      <c r="AK30" s="22"/>
+      <c r="W30" s="15"/>
+      <c r="X30" s="15"/>
+      <c r="Y30" s="15"/>
+      <c r="AE30" s="16"/>
+      <c r="AF30" s="16"/>
+      <c r="AG30" s="16"/>
+      <c r="AH30" s="16"/>
+      <c r="AI30" s="16"/>
+      <c r="AJ30" s="16"/>
+      <c r="AK30" s="16"/>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B31" s="11">
@@ -2361,16 +2386,16 @@
       <c r="U31" s="11">
         <v>19</v>
       </c>
-      <c r="W31" s="21"/>
-      <c r="X31" s="21"/>
-      <c r="Y31" s="21"/>
-      <c r="AE31" s="22"/>
-      <c r="AF31" s="22"/>
-      <c r="AG31" s="22"/>
-      <c r="AH31" s="22"/>
-      <c r="AI31" s="22"/>
-      <c r="AJ31" s="22"/>
-      <c r="AK31" s="22"/>
+      <c r="W31" s="15"/>
+      <c r="X31" s="15"/>
+      <c r="Y31" s="15"/>
+      <c r="AE31" s="16"/>
+      <c r="AF31" s="16"/>
+      <c r="AG31" s="16"/>
+      <c r="AH31" s="16"/>
+      <c r="AI31" s="16"/>
+      <c r="AJ31" s="16"/>
+      <c r="AK31" s="16"/>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
@@ -2401,72 +2426,72 @@
       <c r="Z32" s="10"/>
       <c r="AA32" s="10"/>
       <c r="AB32" s="10"/>
-      <c r="AD32" s="22"/>
-      <c r="AE32" s="22"/>
-      <c r="AF32" s="22"/>
-      <c r="AG32" s="22"/>
-      <c r="AH32" s="22"/>
-      <c r="AI32" s="22"/>
-      <c r="AJ32" s="22"/>
-      <c r="AK32" s="22"/>
+      <c r="AD32" s="16"/>
+      <c r="AE32" s="16"/>
+      <c r="AF32" s="16"/>
+      <c r="AG32" s="16"/>
+      <c r="AH32" s="16"/>
+      <c r="AI32" s="16"/>
+      <c r="AJ32" s="16"/>
+      <c r="AK32" s="16"/>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B33" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="12"/>
-      <c r="M33" s="12"/>
-      <c r="N33" s="12"/>
-      <c r="O33" s="12"/>
-      <c r="P33" s="12"/>
-      <c r="Q33" s="12"/>
-      <c r="R33" s="12"/>
-      <c r="S33" s="12"/>
-      <c r="T33" s="12"/>
-      <c r="U33" s="12"/>
-      <c r="AF33" s="22"/>
-      <c r="AG33" s="22"/>
-      <c r="AH33" s="22"/>
-      <c r="AI33" s="22"/>
-      <c r="AJ33" s="22"/>
-      <c r="AK33" s="22"/>
+      <c r="B33" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="18"/>
+      <c r="T33" s="18"/>
+      <c r="U33" s="18"/>
+      <c r="AF33" s="16"/>
+      <c r="AG33" s="16"/>
+      <c r="AH33" s="16"/>
+      <c r="AI33" s="16"/>
+      <c r="AJ33" s="16"/>
+      <c r="AK33" s="16"/>
     </row>
     <row r="34" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="13"/>
-      <c r="P34" s="13"/>
-      <c r="Q34" s="13"/>
-      <c r="R34" s="13"/>
-      <c r="S34" s="13"/>
-      <c r="T34" s="13"/>
-      <c r="U34" s="13"/>
-      <c r="AF34" s="22"/>
-      <c r="AG34" s="22"/>
-      <c r="AH34" s="22"/>
-      <c r="AI34" s="22"/>
-      <c r="AJ34" s="22"/>
-      <c r="AK34" s="22"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+      <c r="AF34" s="16"/>
+      <c r="AG34" s="16"/>
+      <c r="AH34" s="16"/>
+      <c r="AI34" s="16"/>
+      <c r="AJ34" s="16"/>
+      <c r="AK34" s="16"/>
     </row>
     <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
@@ -2476,7 +2501,7 @@
         <v>8</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>22</v>
@@ -2500,13 +2525,13 @@
         <v>0</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L35" s="3" t="s">
         <v>8</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>17</v>
@@ -2527,20 +2552,20 @@
         <v>0</v>
       </c>
       <c r="T35" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="W35" s="21"/>
-      <c r="X35" s="21"/>
-      <c r="Y35" s="21"/>
-      <c r="AF35" s="22"/>
-      <c r="AG35" s="22"/>
-      <c r="AH35" s="22"/>
-      <c r="AI35" s="22"/>
-      <c r="AJ35" s="22"/>
-      <c r="AK35" s="22"/>
+      <c r="W35" s="15"/>
+      <c r="X35" s="15"/>
+      <c r="Y35" s="15"/>
+      <c r="AF35" s="16"/>
+      <c r="AG35" s="16"/>
+      <c r="AH35" s="16"/>
+      <c r="AI35" s="16"/>
+      <c r="AJ35" s="16"/>
+      <c r="AK35" s="16"/>
     </row>
     <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
@@ -2550,7 +2575,7 @@
         <v>8</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>22</v>
@@ -2574,13 +2599,13 @@
         <v>0</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L36" s="3" t="s">
         <v>8</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>22</v>
@@ -2601,22 +2626,22 @@
         <v>0</v>
       </c>
       <c r="T36" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U36" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="W36" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="X36" s="21"/>
-      <c r="Y36" s="21"/>
-      <c r="AF36" s="22"/>
-      <c r="AG36" s="22"/>
-      <c r="AH36" s="22"/>
-      <c r="AI36" s="22"/>
-      <c r="AJ36" s="22"/>
-      <c r="AK36" s="22"/>
+      <c r="W36" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="X36" s="15"/>
+      <c r="Y36" s="15"/>
+      <c r="AF36" s="16"/>
+      <c r="AG36" s="16"/>
+      <c r="AH36" s="16"/>
+      <c r="AI36" s="16"/>
+      <c r="AJ36" s="16"/>
+      <c r="AK36" s="16"/>
     </row>
     <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
@@ -2626,7 +2651,7 @@
         <v>8</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>17</v>
@@ -2653,36 +2678,36 @@
         <v>0</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="M37" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="M37" s="4"/>
+      <c r="N37" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N37" s="4" t="s">
+      <c r="O37" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="O37" s="4" t="s">
+      <c r="P37" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="P37" s="4" t="s">
+      <c r="Q37" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Q37" s="4" t="s">
+      <c r="R37" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="R37" s="4"/>
       <c r="S37" s="4"/>
       <c r="T37" s="4"/>
       <c r="U37" s="4"/>
-      <c r="W37" s="21"/>
-      <c r="X37" s="21"/>
-      <c r="Y37" s="21"/>
-      <c r="AF37" s="22"/>
-      <c r="AG37" s="22"/>
-      <c r="AH37" s="22"/>
-      <c r="AI37" s="22"/>
-      <c r="AJ37" s="22"/>
-      <c r="AK37" s="22"/>
+      <c r="W37" s="15"/>
+      <c r="X37" s="15"/>
+      <c r="Y37" s="15"/>
+      <c r="AF37" s="16"/>
+      <c r="AG37" s="16"/>
+      <c r="AH37" s="16"/>
+      <c r="AI37" s="16"/>
+      <c r="AJ37" s="16"/>
+      <c r="AK37" s="16"/>
     </row>
     <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
@@ -2692,7 +2717,7 @@
         <v>8</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>17</v>
@@ -2707,7 +2732,7 @@
         <v>2</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I38" s="4" t="s">
         <v>0</v>
@@ -2719,7 +2744,7 @@
         <v>0</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
@@ -2730,15 +2755,15 @@
       <c r="S38" s="4"/>
       <c r="T38" s="4"/>
       <c r="U38" s="4"/>
-      <c r="W38" s="21"/>
-      <c r="X38" s="21"/>
-      <c r="Y38" s="21"/>
-      <c r="AF38" s="22"/>
-      <c r="AG38" s="22"/>
-      <c r="AH38" s="22"/>
-      <c r="AI38" s="22"/>
-      <c r="AJ38" s="22"/>
-      <c r="AK38" s="22"/>
+      <c r="W38" s="15"/>
+      <c r="X38" s="15"/>
+      <c r="Y38" s="15"/>
+      <c r="AF38" s="16"/>
+      <c r="AG38" s="16"/>
+      <c r="AH38" s="16"/>
+      <c r="AI38" s="16"/>
+      <c r="AJ38" s="16"/>
+      <c r="AK38" s="16"/>
     </row>
     <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B39" s="11">
@@ -2801,93 +2826,93 @@
       <c r="U39" s="11">
         <v>19</v>
       </c>
-      <c r="W39" s="21"/>
-      <c r="X39" s="21"/>
-      <c r="Y39" s="21"/>
-      <c r="AF39" s="22"/>
-      <c r="AG39" s="22"/>
-      <c r="AH39" s="22"/>
-      <c r="AI39" s="22"/>
-      <c r="AJ39" s="22"/>
-      <c r="AK39" s="22"/>
+      <c r="W39" s="15"/>
+      <c r="X39" s="15"/>
+      <c r="Y39" s="15"/>
+      <c r="AF39" s="16"/>
+      <c r="AG39" s="16"/>
+      <c r="AH39" s="16"/>
+      <c r="AI39" s="16"/>
+      <c r="AJ39" s="16"/>
+      <c r="AK39" s="16"/>
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="AD40" s="22"/>
-      <c r="AE40" s="22"/>
-      <c r="AF40" s="22"/>
-      <c r="AG40" s="22"/>
-      <c r="AH40" s="22"/>
-      <c r="AI40" s="22"/>
-      <c r="AJ40" s="22"/>
-      <c r="AK40" s="22"/>
+      <c r="AD40" s="16"/>
+      <c r="AE40" s="16"/>
+      <c r="AF40" s="16"/>
+      <c r="AG40" s="16"/>
+      <c r="AH40" s="16"/>
+      <c r="AI40" s="16"/>
+      <c r="AJ40" s="16"/>
+      <c r="AK40" s="16"/>
     </row>
     <row r="41" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B41" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="12"/>
-      <c r="M41" s="12"/>
-      <c r="N41" s="12"/>
-      <c r="O41" s="12"/>
-      <c r="P41" s="12"/>
-      <c r="Q41" s="12"/>
-      <c r="R41" s="12"/>
-      <c r="S41" s="12"/>
-      <c r="T41" s="12"/>
-      <c r="U41" s="12"/>
+      <c r="B41" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="18"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="18"/>
+      <c r="S41" s="18"/>
+      <c r="T41" s="18"/>
+      <c r="U41" s="18"/>
       <c r="AA41" s="10"/>
       <c r="AB41" s="10"/>
       <c r="AC41" s="10"/>
-      <c r="AD41" s="22"/>
-      <c r="AE41" s="22"/>
-      <c r="AF41" s="22"/>
-      <c r="AG41" s="22"/>
-      <c r="AH41" s="22"/>
-      <c r="AI41" s="22"/>
-      <c r="AJ41" s="22"/>
-      <c r="AK41" s="22"/>
+      <c r="AD41" s="16"/>
+      <c r="AE41" s="16"/>
+      <c r="AF41" s="16"/>
+      <c r="AG41" s="16"/>
+      <c r="AH41" s="16"/>
+      <c r="AI41" s="16"/>
+      <c r="AJ41" s="16"/>
+      <c r="AK41" s="16"/>
     </row>
     <row r="42" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="13"/>
-      <c r="L42" s="13"/>
-      <c r="M42" s="13"/>
-      <c r="N42" s="13"/>
-      <c r="O42" s="13"/>
-      <c r="P42" s="13"/>
-      <c r="Q42" s="13"/>
-      <c r="R42" s="13"/>
-      <c r="S42" s="13"/>
-      <c r="T42" s="13"/>
-      <c r="U42" s="13"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="19"/>
+      <c r="O42" s="19"/>
+      <c r="P42" s="19"/>
+      <c r="Q42" s="19"/>
+      <c r="R42" s="19"/>
+      <c r="S42" s="19"/>
+      <c r="T42" s="19"/>
+      <c r="U42" s="19"/>
       <c r="AA42" s="10"/>
       <c r="AB42" s="10"/>
       <c r="AC42" s="10"/>
-      <c r="AD42" s="22"/>
-      <c r="AE42" s="22"/>
-      <c r="AF42" s="22"/>
-      <c r="AG42" s="22"/>
-      <c r="AH42" s="22"/>
-      <c r="AI42" s="22"/>
-      <c r="AJ42" s="22"/>
-      <c r="AK42" s="22"/>
+      <c r="AD42" s="16"/>
+      <c r="AE42" s="16"/>
+      <c r="AF42" s="16"/>
+      <c r="AG42" s="16"/>
+      <c r="AH42" s="16"/>
+      <c r="AI42" s="16"/>
+      <c r="AJ42" s="16"/>
+      <c r="AK42" s="16"/>
     </row>
     <row r="43" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
@@ -2934,7 +2959,7 @@
       <c r="P43" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q43" s="20" t="s">
+      <c r="Q43" s="14" t="s">
         <v>8</v>
       </c>
       <c r="R43" s="7" t="s">
@@ -2949,20 +2974,20 @@
       <c r="U43" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W43" s="21"/>
-      <c r="X43" s="21"/>
-      <c r="Y43" s="21"/>
+      <c r="W43" s="15"/>
+      <c r="X43" s="15"/>
+      <c r="Y43" s="15"/>
       <c r="AA43" s="10"/>
       <c r="AB43" s="10"/>
       <c r="AC43" s="10"/>
-      <c r="AD43" s="22"/>
-      <c r="AE43" s="22"/>
-      <c r="AF43" s="22"/>
-      <c r="AG43" s="22"/>
-      <c r="AH43" s="22"/>
-      <c r="AI43" s="22"/>
-      <c r="AJ43" s="22"/>
-      <c r="AK43" s="22"/>
+      <c r="AD43" s="16"/>
+      <c r="AE43" s="16"/>
+      <c r="AF43" s="16"/>
+      <c r="AG43" s="16"/>
+      <c r="AH43" s="16"/>
+      <c r="AI43" s="16"/>
+      <c r="AJ43" s="16"/>
+      <c r="AK43" s="16"/>
     </row>
     <row r="44" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A44" s="11">
@@ -3014,49 +3039,47 @@
       <c r="S44" s="7"/>
       <c r="T44" s="7"/>
       <c r="U44" s="7"/>
-      <c r="W44" s="21"/>
-      <c r="X44" s="21"/>
-      <c r="Y44" s="21"/>
+      <c r="W44" s="15"/>
+      <c r="X44" s="15"/>
+      <c r="Y44" s="15"/>
       <c r="AA44" s="10"/>
       <c r="AB44" s="10"/>
       <c r="AC44" s="10"/>
-      <c r="AD44" s="22"/>
-      <c r="AE44" s="22"/>
-      <c r="AF44" s="22"/>
-      <c r="AG44" s="22"/>
-      <c r="AH44" s="22"/>
-      <c r="AI44" s="22"/>
-      <c r="AJ44" s="22"/>
-      <c r="AK44" s="22"/>
+      <c r="AD44" s="16"/>
+      <c r="AE44" s="16"/>
+      <c r="AF44" s="16"/>
+      <c r="AG44" s="16"/>
+      <c r="AH44" s="16"/>
+      <c r="AI44" s="16"/>
+      <c r="AJ44" s="16"/>
+      <c r="AK44" s="16"/>
     </row>
     <row r="45" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A45" s="11">
         <v>2</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="B45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I45" s="4"/>
       <c r="J45" s="3" t="s">
         <v>8</v>
       </c>
@@ -3083,49 +3106,47 @@
       <c r="S45" s="2"/>
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
-      <c r="W45" s="21"/>
-      <c r="X45" s="21"/>
-      <c r="Y45" s="21"/>
+      <c r="W45" s="15"/>
+      <c r="X45" s="15"/>
+      <c r="Y45" s="15"/>
       <c r="AA45" s="10"/>
       <c r="AB45" s="10"/>
       <c r="AC45" s="10"/>
-      <c r="AD45" s="22"/>
-      <c r="AE45" s="22"/>
-      <c r="AF45" s="22"/>
-      <c r="AG45" s="22"/>
-      <c r="AH45" s="22"/>
-      <c r="AI45" s="22"/>
-      <c r="AJ45" s="22"/>
-      <c r="AK45" s="22"/>
+      <c r="AD45" s="16"/>
+      <c r="AE45" s="16"/>
+      <c r="AF45" s="16"/>
+      <c r="AG45" s="16"/>
+      <c r="AH45" s="16"/>
+      <c r="AI45" s="16"/>
+      <c r="AJ45" s="16"/>
+      <c r="AK45" s="16"/>
     </row>
     <row r="46" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
         <v>3</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>11</v>
+      <c r="B46" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>26</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H46" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I46" s="4"/>
       <c r="J46" s="3" t="s">
         <v>8</v>
       </c>
@@ -3152,20 +3173,20 @@
       <c r="S46" s="2"/>
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
-      <c r="W46" s="21"/>
-      <c r="X46" s="21"/>
-      <c r="Y46" s="21"/>
+      <c r="W46" s="15"/>
+      <c r="X46" s="15"/>
+      <c r="Y46" s="15"/>
       <c r="AA46" s="10"/>
       <c r="AB46" s="10"/>
       <c r="AC46" s="10"/>
-      <c r="AD46" s="22"/>
-      <c r="AE46" s="22"/>
-      <c r="AF46" s="22"/>
-      <c r="AG46" s="22"/>
-      <c r="AH46" s="22"/>
-      <c r="AI46" s="22"/>
-      <c r="AJ46" s="22"/>
-      <c r="AK46" s="22"/>
+      <c r="AD46" s="16"/>
+      <c r="AE46" s="16"/>
+      <c r="AF46" s="16"/>
+      <c r="AG46" s="16"/>
+      <c r="AH46" s="16"/>
+      <c r="AI46" s="16"/>
+      <c r="AJ46" s="16"/>
+      <c r="AK46" s="16"/>
     </row>
     <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B47" s="11">
@@ -3228,190 +3249,190 @@
       <c r="U47" s="11">
         <v>19</v>
       </c>
-      <c r="W47" s="21"/>
-      <c r="X47" s="21"/>
-      <c r="Y47" s="21"/>
+      <c r="W47" s="15"/>
+      <c r="X47" s="15"/>
+      <c r="Y47" s="15"/>
       <c r="AA47" s="10"/>
       <c r="AB47" s="10"/>
       <c r="AC47" s="10"/>
-      <c r="AD47" s="22"/>
-      <c r="AE47" s="22"/>
-      <c r="AF47" s="22"/>
-      <c r="AG47" s="22"/>
-      <c r="AH47" s="22"/>
-      <c r="AI47" s="22"/>
-      <c r="AJ47" s="22"/>
-      <c r="AK47" s="22"/>
+      <c r="AD47" s="16"/>
+      <c r="AE47" s="16"/>
+      <c r="AF47" s="16"/>
+      <c r="AG47" s="16"/>
+      <c r="AH47" s="16"/>
+      <c r="AI47" s="16"/>
+      <c r="AJ47" s="16"/>
+      <c r="AK47" s="16"/>
     </row>
     <row r="48" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="AD48" s="22"/>
-      <c r="AE48" s="22"/>
-      <c r="AF48" s="22"/>
-      <c r="AG48" s="22"/>
-      <c r="AH48" s="22"/>
-      <c r="AI48" s="22"/>
-      <c r="AJ48" s="22"/>
-      <c r="AK48" s="22"/>
+      <c r="AD48" s="16"/>
+      <c r="AE48" s="16"/>
+      <c r="AF48" s="16"/>
+      <c r="AG48" s="16"/>
+      <c r="AH48" s="16"/>
+      <c r="AI48" s="16"/>
+      <c r="AJ48" s="16"/>
+      <c r="AK48" s="16"/>
     </row>
     <row r="49" spans="30:37" x14ac:dyDescent="0.25">
-      <c r="AD49" s="22"/>
-      <c r="AE49" s="22"/>
-      <c r="AF49" s="22"/>
-      <c r="AG49" s="22"/>
-      <c r="AH49" s="22"/>
-      <c r="AI49" s="22"/>
-      <c r="AJ49" s="22"/>
-      <c r="AK49" s="22"/>
+      <c r="AD49" s="16"/>
+      <c r="AE49" s="16"/>
+      <c r="AF49" s="16"/>
+      <c r="AG49" s="16"/>
+      <c r="AH49" s="16"/>
+      <c r="AI49" s="16"/>
+      <c r="AJ49" s="16"/>
+      <c r="AK49" s="16"/>
     </row>
     <row r="50" spans="30:37" x14ac:dyDescent="0.25">
-      <c r="AD50" s="22"/>
-      <c r="AE50" s="22"/>
-      <c r="AF50" s="22"/>
-      <c r="AG50" s="22"/>
-      <c r="AH50" s="22"/>
-      <c r="AI50" s="22"/>
-      <c r="AJ50" s="22"/>
-      <c r="AK50" s="22"/>
+      <c r="AD50" s="16"/>
+      <c r="AE50" s="16"/>
+      <c r="AF50" s="16"/>
+      <c r="AG50" s="16"/>
+      <c r="AH50" s="16"/>
+      <c r="AI50" s="16"/>
+      <c r="AJ50" s="16"/>
+      <c r="AK50" s="16"/>
     </row>
     <row r="51" spans="30:37" x14ac:dyDescent="0.25">
-      <c r="AD51" s="22"/>
-      <c r="AE51" s="22"/>
-      <c r="AF51" s="22"/>
-      <c r="AG51" s="22"/>
-      <c r="AH51" s="22"/>
-      <c r="AI51" s="22"/>
-      <c r="AJ51" s="22"/>
-      <c r="AK51" s="22"/>
+      <c r="AD51" s="16"/>
+      <c r="AE51" s="16"/>
+      <c r="AF51" s="16"/>
+      <c r="AG51" s="16"/>
+      <c r="AH51" s="16"/>
+      <c r="AI51" s="16"/>
+      <c r="AJ51" s="16"/>
+      <c r="AK51" s="16"/>
     </row>
     <row r="52" spans="30:37" x14ac:dyDescent="0.25">
-      <c r="AD52" s="22"/>
-      <c r="AE52" s="22"/>
-      <c r="AF52" s="22"/>
-      <c r="AG52" s="22"/>
-      <c r="AH52" s="22"/>
-      <c r="AI52" s="22"/>
-      <c r="AJ52" s="22"/>
-      <c r="AK52" s="22"/>
+      <c r="AD52" s="16"/>
+      <c r="AE52" s="16"/>
+      <c r="AF52" s="16"/>
+      <c r="AG52" s="16"/>
+      <c r="AH52" s="16"/>
+      <c r="AI52" s="16"/>
+      <c r="AJ52" s="16"/>
+      <c r="AK52" s="16"/>
     </row>
     <row r="53" spans="30:37" x14ac:dyDescent="0.25">
-      <c r="AD53" s="22"/>
-      <c r="AE53" s="22"/>
-      <c r="AF53" s="22"/>
-      <c r="AG53" s="22"/>
-      <c r="AH53" s="22"/>
-      <c r="AI53" s="22"/>
-      <c r="AJ53" s="22"/>
-      <c r="AK53" s="22"/>
+      <c r="AD53" s="16"/>
+      <c r="AE53" s="16"/>
+      <c r="AF53" s="16"/>
+      <c r="AG53" s="16"/>
+      <c r="AH53" s="16"/>
+      <c r="AI53" s="16"/>
+      <c r="AJ53" s="16"/>
+      <c r="AK53" s="16"/>
     </row>
     <row r="54" spans="30:37" x14ac:dyDescent="0.25">
-      <c r="AD54" s="22"/>
-      <c r="AE54" s="22"/>
-      <c r="AF54" s="22"/>
-      <c r="AG54" s="22"/>
-      <c r="AH54" s="22"/>
-      <c r="AI54" s="22"/>
-      <c r="AJ54" s="22"/>
-      <c r="AK54" s="22"/>
+      <c r="AD54" s="16"/>
+      <c r="AE54" s="16"/>
+      <c r="AF54" s="16"/>
+      <c r="AG54" s="16"/>
+      <c r="AH54" s="16"/>
+      <c r="AI54" s="16"/>
+      <c r="AJ54" s="16"/>
+      <c r="AK54" s="16"/>
     </row>
     <row r="55" spans="30:37" x14ac:dyDescent="0.25">
-      <c r="AD55" s="22"/>
-      <c r="AE55" s="22"/>
-      <c r="AF55" s="22"/>
-      <c r="AG55" s="22"/>
-      <c r="AH55" s="22"/>
-      <c r="AI55" s="22"/>
-      <c r="AJ55" s="22"/>
-      <c r="AK55" s="22"/>
+      <c r="AD55" s="16"/>
+      <c r="AE55" s="16"/>
+      <c r="AF55" s="16"/>
+      <c r="AG55" s="16"/>
+      <c r="AH55" s="16"/>
+      <c r="AI55" s="16"/>
+      <c r="AJ55" s="16"/>
+      <c r="AK55" s="16"/>
     </row>
     <row r="56" spans="30:37" x14ac:dyDescent="0.25">
-      <c r="AD56" s="22"/>
-      <c r="AE56" s="22"/>
-      <c r="AF56" s="22"/>
-      <c r="AG56" s="22"/>
-      <c r="AH56" s="22"/>
-      <c r="AI56" s="22"/>
-      <c r="AJ56" s="22"/>
-      <c r="AK56" s="22"/>
+      <c r="AD56" s="16"/>
+      <c r="AE56" s="16"/>
+      <c r="AF56" s="16"/>
+      <c r="AG56" s="16"/>
+      <c r="AH56" s="16"/>
+      <c r="AI56" s="16"/>
+      <c r="AJ56" s="16"/>
+      <c r="AK56" s="16"/>
     </row>
     <row r="57" spans="30:37" x14ac:dyDescent="0.25">
-      <c r="AD57" s="22"/>
-      <c r="AE57" s="22"/>
-      <c r="AF57" s="22"/>
-      <c r="AG57" s="22"/>
-      <c r="AH57" s="22"/>
-      <c r="AI57" s="22"/>
-      <c r="AJ57" s="22"/>
-      <c r="AK57" s="22"/>
+      <c r="AD57" s="16"/>
+      <c r="AE57" s="16"/>
+      <c r="AF57" s="16"/>
+      <c r="AG57" s="16"/>
+      <c r="AH57" s="16"/>
+      <c r="AI57" s="16"/>
+      <c r="AJ57" s="16"/>
+      <c r="AK57" s="16"/>
     </row>
     <row r="58" spans="30:37" x14ac:dyDescent="0.25">
-      <c r="AD58" s="22"/>
-      <c r="AE58" s="22"/>
-      <c r="AF58" s="22"/>
-      <c r="AG58" s="22"/>
-      <c r="AH58" s="22"/>
-      <c r="AI58" s="22"/>
-      <c r="AJ58" s="22"/>
-      <c r="AK58" s="22"/>
+      <c r="AD58" s="16"/>
+      <c r="AE58" s="16"/>
+      <c r="AF58" s="16"/>
+      <c r="AG58" s="16"/>
+      <c r="AH58" s="16"/>
+      <c r="AI58" s="16"/>
+      <c r="AJ58" s="16"/>
+      <c r="AK58" s="16"/>
     </row>
     <row r="59" spans="30:37" x14ac:dyDescent="0.25">
-      <c r="AD59" s="22"/>
-      <c r="AE59" s="22"/>
-      <c r="AF59" s="22"/>
-      <c r="AG59" s="22"/>
-      <c r="AH59" s="22"/>
-      <c r="AI59" s="22"/>
-      <c r="AJ59" s="22"/>
-      <c r="AK59" s="22"/>
+      <c r="AD59" s="16"/>
+      <c r="AE59" s="16"/>
+      <c r="AF59" s="16"/>
+      <c r="AG59" s="16"/>
+      <c r="AH59" s="16"/>
+      <c r="AI59" s="16"/>
+      <c r="AJ59" s="16"/>
+      <c r="AK59" s="16"/>
     </row>
     <row r="60" spans="30:37" x14ac:dyDescent="0.25">
-      <c r="AD60" s="22"/>
-      <c r="AE60" s="22"/>
-      <c r="AF60" s="22"/>
-      <c r="AG60" s="22"/>
-      <c r="AH60" s="22"/>
-      <c r="AI60" s="22"/>
-      <c r="AJ60" s="22"/>
-      <c r="AK60" s="22"/>
+      <c r="AD60" s="16"/>
+      <c r="AE60" s="16"/>
+      <c r="AF60" s="16"/>
+      <c r="AG60" s="16"/>
+      <c r="AH60" s="16"/>
+      <c r="AI60" s="16"/>
+      <c r="AJ60" s="16"/>
+      <c r="AK60" s="16"/>
     </row>
     <row r="61" spans="30:37" x14ac:dyDescent="0.25">
-      <c r="AD61" s="22"/>
-      <c r="AE61" s="22"/>
-      <c r="AF61" s="22"/>
-      <c r="AG61" s="22"/>
-      <c r="AH61" s="22"/>
-      <c r="AI61" s="22"/>
-      <c r="AJ61" s="22"/>
-      <c r="AK61" s="22"/>
+      <c r="AD61" s="16"/>
+      <c r="AE61" s="16"/>
+      <c r="AF61" s="16"/>
+      <c r="AG61" s="16"/>
+      <c r="AH61" s="16"/>
+      <c r="AI61" s="16"/>
+      <c r="AJ61" s="16"/>
+      <c r="AK61" s="16"/>
     </row>
     <row r="62" spans="30:37" x14ac:dyDescent="0.25">
-      <c r="AD62" s="22"/>
-      <c r="AE62" s="22"/>
-      <c r="AF62" s="22"/>
-      <c r="AG62" s="22"/>
-      <c r="AH62" s="22"/>
-      <c r="AI62" s="22"/>
-      <c r="AJ62" s="22"/>
-      <c r="AK62" s="22"/>
+      <c r="AD62" s="16"/>
+      <c r="AE62" s="16"/>
+      <c r="AF62" s="16"/>
+      <c r="AG62" s="16"/>
+      <c r="AH62" s="16"/>
+      <c r="AI62" s="16"/>
+      <c r="AJ62" s="16"/>
+      <c r="AK62" s="16"/>
     </row>
     <row r="63" spans="30:37" x14ac:dyDescent="0.25">
-      <c r="AD63" s="22"/>
-      <c r="AE63" s="22"/>
-      <c r="AF63" s="22"/>
-      <c r="AG63" s="22"/>
-      <c r="AH63" s="22"/>
-      <c r="AI63" s="22"/>
-      <c r="AJ63" s="22"/>
-      <c r="AK63" s="22"/>
+      <c r="AD63" s="16"/>
+      <c r="AE63" s="16"/>
+      <c r="AF63" s="16"/>
+      <c r="AG63" s="16"/>
+      <c r="AH63" s="16"/>
+      <c r="AI63" s="16"/>
+      <c r="AJ63" s="16"/>
+      <c r="AK63" s="16"/>
     </row>
     <row r="64" spans="30:37" x14ac:dyDescent="0.25">
-      <c r="AD64" s="21"/>
-      <c r="AE64" s="21"/>
-      <c r="AF64" s="21"/>
-      <c r="AG64" s="21"/>
-      <c r="AH64" s="21"/>
-      <c r="AI64" s="21"/>
-      <c r="AJ64" s="21"/>
-      <c r="AK64" s="21"/>
+      <c r="AD64" s="15"/>
+      <c r="AE64" s="15"/>
+      <c r="AF64" s="15"/>
+      <c r="AG64" s="15"/>
+      <c r="AH64" s="15"/>
+      <c r="AI64" s="15"/>
+      <c r="AJ64" s="15"/>
+      <c r="AK64" s="15"/>
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.25">
       <c r="Z65" s="10"/>
@@ -3471,26 +3492,26 @@
     </row>
     <row r="73" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A73" s="10"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="14"/>
-      <c r="G73" s="14"/>
-      <c r="H73" s="14"/>
-      <c r="I73" s="14"/>
-      <c r="J73" s="14"/>
-      <c r="K73" s="14"/>
-      <c r="L73" s="14"/>
-      <c r="M73" s="14"/>
-      <c r="N73" s="14"/>
-      <c r="O73" s="14"/>
-      <c r="P73" s="14"/>
-      <c r="Q73" s="14"/>
-      <c r="R73" s="14"/>
-      <c r="S73" s="14"/>
-      <c r="T73" s="14"/>
-      <c r="U73" s="14"/>
+      <c r="B73" s="23"/>
+      <c r="C73" s="23"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="23"/>
+      <c r="F73" s="23"/>
+      <c r="G73" s="23"/>
+      <c r="H73" s="23"/>
+      <c r="I73" s="23"/>
+      <c r="J73" s="23"/>
+      <c r="K73" s="23"/>
+      <c r="L73" s="23"/>
+      <c r="M73" s="23"/>
+      <c r="N73" s="23"/>
+      <c r="O73" s="23"/>
+      <c r="P73" s="23"/>
+      <c r="Q73" s="23"/>
+      <c r="R73" s="23"/>
+      <c r="S73" s="23"/>
+      <c r="T73" s="23"/>
+      <c r="U73" s="23"/>
       <c r="V73" s="10"/>
       <c r="W73" s="10"/>
       <c r="X73" s="10"/>
@@ -3499,26 +3520,26 @@
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A74" s="10"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
-      <c r="G74" s="14"/>
-      <c r="H74" s="14"/>
-      <c r="I74" s="14"/>
-      <c r="J74" s="14"/>
-      <c r="K74" s="14"/>
-      <c r="L74" s="14"/>
-      <c r="M74" s="14"/>
-      <c r="N74" s="14"/>
-      <c r="O74" s="14"/>
-      <c r="P74" s="14"/>
-      <c r="Q74" s="14"/>
-      <c r="R74" s="14"/>
-      <c r="S74" s="14"/>
-      <c r="T74" s="14"/>
-      <c r="U74" s="14"/>
+      <c r="B74" s="23"/>
+      <c r="C74" s="23"/>
+      <c r="D74" s="23"/>
+      <c r="E74" s="23"/>
+      <c r="F74" s="23"/>
+      <c r="G74" s="23"/>
+      <c r="H74" s="23"/>
+      <c r="I74" s="23"/>
+      <c r="J74" s="23"/>
+      <c r="K74" s="23"/>
+      <c r="L74" s="23"/>
+      <c r="M74" s="23"/>
+      <c r="N74" s="23"/>
+      <c r="O74" s="23"/>
+      <c r="P74" s="23"/>
+      <c r="Q74" s="23"/>
+      <c r="R74" s="23"/>
+      <c r="S74" s="23"/>
+      <c r="T74" s="23"/>
+      <c r="U74" s="23"/>
       <c r="V74" s="10"/>
       <c r="W74" s="10"/>
       <c r="X74" s="10"/>
@@ -3672,23 +3693,23 @@
       <c r="AC82" s="10"/>
     </row>
     <row r="83" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="Z83" s="21"/>
+      <c r="Z83" s="15"/>
       <c r="AC83" s="10"/>
     </row>
     <row r="84" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="Z84" s="21"/>
+      <c r="Z84" s="15"/>
       <c r="AC84" s="10"/>
     </row>
     <row r="85" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="Z85" s="21"/>
+      <c r="Z85" s="15"/>
       <c r="AC85" s="10"/>
     </row>
     <row r="86" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="Z86" s="21"/>
+      <c r="Z86" s="15"/>
       <c r="AC86" s="10"/>
     </row>
     <row r="87" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="Z87" s="21"/>
+      <c r="Z87" s="15"/>
       <c r="AC87" s="10"/>
     </row>
     <row r="88" spans="1:29" x14ac:dyDescent="0.25">
@@ -3723,26 +3744,26 @@
     </row>
     <row r="89" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A89" s="10"/>
-      <c r="B89" s="14"/>
-      <c r="C89" s="14"/>
-      <c r="D89" s="14"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="14"/>
-      <c r="G89" s="14"/>
-      <c r="H89" s="14"/>
-      <c r="I89" s="14"/>
-      <c r="J89" s="14"/>
-      <c r="K89" s="14"/>
-      <c r="L89" s="14"/>
-      <c r="M89" s="14"/>
-      <c r="N89" s="14"/>
-      <c r="O89" s="14"/>
-      <c r="P89" s="14"/>
-      <c r="Q89" s="14"/>
-      <c r="R89" s="14"/>
-      <c r="S89" s="14"/>
-      <c r="T89" s="14"/>
-      <c r="U89" s="14"/>
+      <c r="B89" s="23"/>
+      <c r="C89" s="23"/>
+      <c r="D89" s="23"/>
+      <c r="E89" s="23"/>
+      <c r="F89" s="23"/>
+      <c r="G89" s="23"/>
+      <c r="H89" s="23"/>
+      <c r="I89" s="23"/>
+      <c r="J89" s="23"/>
+      <c r="K89" s="23"/>
+      <c r="L89" s="23"/>
+      <c r="M89" s="23"/>
+      <c r="N89" s="23"/>
+      <c r="O89" s="23"/>
+      <c r="P89" s="23"/>
+      <c r="Q89" s="23"/>
+      <c r="R89" s="23"/>
+      <c r="S89" s="23"/>
+      <c r="T89" s="23"/>
+      <c r="U89" s="23"/>
       <c r="V89" s="10"/>
       <c r="W89" s="10"/>
       <c r="X89" s="10"/>
@@ -3753,26 +3774,26 @@
     </row>
     <row r="90" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A90" s="10"/>
-      <c r="B90" s="14"/>
-      <c r="C90" s="14"/>
-      <c r="D90" s="14"/>
-      <c r="E90" s="14"/>
-      <c r="F90" s="14"/>
-      <c r="G90" s="14"/>
-      <c r="H90" s="14"/>
-      <c r="I90" s="14"/>
-      <c r="J90" s="14"/>
-      <c r="K90" s="14"/>
-      <c r="L90" s="14"/>
-      <c r="M90" s="14"/>
-      <c r="N90" s="14"/>
-      <c r="O90" s="14"/>
-      <c r="P90" s="14"/>
-      <c r="Q90" s="14"/>
-      <c r="R90" s="14"/>
-      <c r="S90" s="14"/>
-      <c r="T90" s="14"/>
-      <c r="U90" s="14"/>
+      <c r="B90" s="23"/>
+      <c r="C90" s="23"/>
+      <c r="D90" s="23"/>
+      <c r="E90" s="23"/>
+      <c r="F90" s="23"/>
+      <c r="G90" s="23"/>
+      <c r="H90" s="23"/>
+      <c r="I90" s="23"/>
+      <c r="J90" s="23"/>
+      <c r="K90" s="23"/>
+      <c r="L90" s="23"/>
+      <c r="M90" s="23"/>
+      <c r="N90" s="23"/>
+      <c r="O90" s="23"/>
+      <c r="P90" s="23"/>
+      <c r="Q90" s="23"/>
+      <c r="R90" s="23"/>
+      <c r="S90" s="23"/>
+      <c r="T90" s="23"/>
+      <c r="U90" s="23"/>
       <c r="V90" s="10"/>
       <c r="W90" s="10"/>
       <c r="X90" s="10"/>
@@ -3963,26 +3984,26 @@
     </row>
     <row r="97" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A97" s="10"/>
-      <c r="B97" s="14"/>
-      <c r="C97" s="14"/>
-      <c r="D97" s="14"/>
-      <c r="E97" s="14"/>
-      <c r="F97" s="14"/>
-      <c r="G97" s="14"/>
-      <c r="H97" s="14"/>
-      <c r="I97" s="14"/>
-      <c r="J97" s="14"/>
-      <c r="K97" s="14"/>
-      <c r="L97" s="14"/>
-      <c r="M97" s="14"/>
-      <c r="N97" s="14"/>
-      <c r="O97" s="14"/>
-      <c r="P97" s="14"/>
-      <c r="Q97" s="14"/>
-      <c r="R97" s="14"/>
-      <c r="S97" s="14"/>
-      <c r="T97" s="14"/>
-      <c r="U97" s="14"/>
+      <c r="B97" s="23"/>
+      <c r="C97" s="23"/>
+      <c r="D97" s="23"/>
+      <c r="E97" s="23"/>
+      <c r="F97" s="23"/>
+      <c r="G97" s="23"/>
+      <c r="H97" s="23"/>
+      <c r="I97" s="23"/>
+      <c r="J97" s="23"/>
+      <c r="K97" s="23"/>
+      <c r="L97" s="23"/>
+      <c r="M97" s="23"/>
+      <c r="N97" s="23"/>
+      <c r="O97" s="23"/>
+      <c r="P97" s="23"/>
+      <c r="Q97" s="23"/>
+      <c r="R97" s="23"/>
+      <c r="S97" s="23"/>
+      <c r="T97" s="23"/>
+      <c r="U97" s="23"/>
       <c r="V97" s="10"/>
       <c r="W97" s="10"/>
       <c r="X97" s="10"/>
@@ -3993,26 +4014,26 @@
     </row>
     <row r="98" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A98" s="10"/>
-      <c r="B98" s="14"/>
-      <c r="C98" s="14"/>
-      <c r="D98" s="14"/>
-      <c r="E98" s="14"/>
-      <c r="F98" s="14"/>
-      <c r="G98" s="14"/>
-      <c r="H98" s="14"/>
-      <c r="I98" s="14"/>
-      <c r="J98" s="14"/>
-      <c r="K98" s="14"/>
-      <c r="L98" s="14"/>
-      <c r="M98" s="14"/>
-      <c r="N98" s="14"/>
-      <c r="O98" s="14"/>
-      <c r="P98" s="14"/>
-      <c r="Q98" s="14"/>
-      <c r="R98" s="14"/>
-      <c r="S98" s="14"/>
-      <c r="T98" s="14"/>
-      <c r="U98" s="14"/>
+      <c r="B98" s="23"/>
+      <c r="C98" s="23"/>
+      <c r="D98" s="23"/>
+      <c r="E98" s="23"/>
+      <c r="F98" s="23"/>
+      <c r="G98" s="23"/>
+      <c r="H98" s="23"/>
+      <c r="I98" s="23"/>
+      <c r="J98" s="23"/>
+      <c r="K98" s="23"/>
+      <c r="L98" s="23"/>
+      <c r="M98" s="23"/>
+      <c r="N98" s="23"/>
+      <c r="O98" s="23"/>
+      <c r="P98" s="23"/>
+      <c r="Q98" s="23"/>
+      <c r="R98" s="23"/>
+      <c r="S98" s="23"/>
+      <c r="T98" s="23"/>
+      <c r="U98" s="23"/>
       <c r="V98" s="10"/>
       <c r="W98" s="10"/>
       <c r="X98" s="10"/>
@@ -4203,26 +4224,26 @@
     </row>
     <row r="105" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A105" s="10"/>
-      <c r="B105" s="14"/>
-      <c r="C105" s="14"/>
-      <c r="D105" s="14"/>
-      <c r="E105" s="14"/>
-      <c r="F105" s="14"/>
-      <c r="G105" s="14"/>
-      <c r="H105" s="14"/>
-      <c r="I105" s="14"/>
-      <c r="J105" s="14"/>
-      <c r="K105" s="14"/>
-      <c r="L105" s="14"/>
-      <c r="M105" s="14"/>
-      <c r="N105" s="14"/>
-      <c r="O105" s="14"/>
-      <c r="P105" s="14"/>
-      <c r="Q105" s="14"/>
-      <c r="R105" s="14"/>
-      <c r="S105" s="14"/>
-      <c r="T105" s="14"/>
-      <c r="U105" s="14"/>
+      <c r="B105" s="23"/>
+      <c r="C105" s="23"/>
+      <c r="D105" s="23"/>
+      <c r="E105" s="23"/>
+      <c r="F105" s="23"/>
+      <c r="G105" s="23"/>
+      <c r="H105" s="23"/>
+      <c r="I105" s="23"/>
+      <c r="J105" s="23"/>
+      <c r="K105" s="23"/>
+      <c r="L105" s="23"/>
+      <c r="M105" s="23"/>
+      <c r="N105" s="23"/>
+      <c r="O105" s="23"/>
+      <c r="P105" s="23"/>
+      <c r="Q105" s="23"/>
+      <c r="R105" s="23"/>
+      <c r="S105" s="23"/>
+      <c r="T105" s="23"/>
+      <c r="U105" s="23"/>
       <c r="V105" s="10"/>
       <c r="W105" s="10"/>
       <c r="X105" s="10"/>
@@ -4233,26 +4254,26 @@
     </row>
     <row r="106" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A106" s="10"/>
-      <c r="B106" s="14"/>
-      <c r="C106" s="14"/>
-      <c r="D106" s="14"/>
-      <c r="E106" s="14"/>
-      <c r="F106" s="14"/>
-      <c r="G106" s="14"/>
-      <c r="H106" s="14"/>
-      <c r="I106" s="14"/>
-      <c r="J106" s="14"/>
-      <c r="K106" s="14"/>
-      <c r="L106" s="14"/>
-      <c r="M106" s="14"/>
-      <c r="N106" s="14"/>
-      <c r="O106" s="14"/>
-      <c r="P106" s="14"/>
-      <c r="Q106" s="14"/>
-      <c r="R106" s="14"/>
-      <c r="S106" s="14"/>
-      <c r="T106" s="14"/>
-      <c r="U106" s="14"/>
+      <c r="B106" s="23"/>
+      <c r="C106" s="23"/>
+      <c r="D106" s="23"/>
+      <c r="E106" s="23"/>
+      <c r="F106" s="23"/>
+      <c r="G106" s="23"/>
+      <c r="H106" s="23"/>
+      <c r="I106" s="23"/>
+      <c r="J106" s="23"/>
+      <c r="K106" s="23"/>
+      <c r="L106" s="23"/>
+      <c r="M106" s="23"/>
+      <c r="N106" s="23"/>
+      <c r="O106" s="23"/>
+      <c r="P106" s="23"/>
+      <c r="Q106" s="23"/>
+      <c r="R106" s="23"/>
+      <c r="S106" s="23"/>
+      <c r="T106" s="23"/>
+      <c r="U106" s="23"/>
       <c r="V106" s="10"/>
       <c r="W106" s="10"/>
       <c r="X106" s="10"/>
@@ -4443,26 +4464,26 @@
     </row>
     <row r="113" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A113" s="10"/>
-      <c r="B113" s="14"/>
-      <c r="C113" s="14"/>
-      <c r="D113" s="14"/>
-      <c r="E113" s="14"/>
-      <c r="F113" s="14"/>
-      <c r="G113" s="14"/>
-      <c r="H113" s="14"/>
-      <c r="I113" s="14"/>
-      <c r="J113" s="14"/>
-      <c r="K113" s="14"/>
-      <c r="L113" s="14"/>
-      <c r="M113" s="14"/>
-      <c r="N113" s="14"/>
-      <c r="O113" s="14"/>
-      <c r="P113" s="14"/>
-      <c r="Q113" s="14"/>
-      <c r="R113" s="14"/>
-      <c r="S113" s="14"/>
-      <c r="T113" s="14"/>
-      <c r="U113" s="14"/>
+      <c r="B113" s="23"/>
+      <c r="C113" s="23"/>
+      <c r="D113" s="23"/>
+      <c r="E113" s="23"/>
+      <c r="F113" s="23"/>
+      <c r="G113" s="23"/>
+      <c r="H113" s="23"/>
+      <c r="I113" s="23"/>
+      <c r="J113" s="23"/>
+      <c r="K113" s="23"/>
+      <c r="L113" s="23"/>
+      <c r="M113" s="23"/>
+      <c r="N113" s="23"/>
+      <c r="O113" s="23"/>
+      <c r="P113" s="23"/>
+      <c r="Q113" s="23"/>
+      <c r="R113" s="23"/>
+      <c r="S113" s="23"/>
+      <c r="T113" s="23"/>
+      <c r="U113" s="23"/>
       <c r="V113" s="10"/>
       <c r="W113" s="10"/>
       <c r="X113" s="10"/>
@@ -4473,26 +4494,26 @@
     </row>
     <row r="114" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A114" s="10"/>
-      <c r="B114" s="14"/>
-      <c r="C114" s="14"/>
-      <c r="D114" s="14"/>
-      <c r="E114" s="14"/>
-      <c r="F114" s="14"/>
-      <c r="G114" s="14"/>
-      <c r="H114" s="14"/>
-      <c r="I114" s="14"/>
-      <c r="J114" s="14"/>
-      <c r="K114" s="14"/>
-      <c r="L114" s="14"/>
-      <c r="M114" s="14"/>
-      <c r="N114" s="14"/>
-      <c r="O114" s="14"/>
-      <c r="P114" s="14"/>
-      <c r="Q114" s="14"/>
-      <c r="R114" s="14"/>
-      <c r="S114" s="14"/>
-      <c r="T114" s="14"/>
-      <c r="U114" s="14"/>
+      <c r="B114" s="23"/>
+      <c r="C114" s="23"/>
+      <c r="D114" s="23"/>
+      <c r="E114" s="23"/>
+      <c r="F114" s="23"/>
+      <c r="G114" s="23"/>
+      <c r="H114" s="23"/>
+      <c r="I114" s="23"/>
+      <c r="J114" s="23"/>
+      <c r="K114" s="23"/>
+      <c r="L114" s="23"/>
+      <c r="M114" s="23"/>
+      <c r="N114" s="23"/>
+      <c r="O114" s="23"/>
+      <c r="P114" s="23"/>
+      <c r="Q114" s="23"/>
+      <c r="R114" s="23"/>
+      <c r="S114" s="23"/>
+      <c r="T114" s="23"/>
+      <c r="U114" s="23"/>
       <c r="V114" s="10"/>
       <c r="W114" s="10"/>
       <c r="X114" s="10"/>
@@ -4508,9 +4529,9 @@
       <c r="D115" s="10"/>
       <c r="E115" s="10"/>
       <c r="F115" s="10"/>
-      <c r="G115" s="14"/>
-      <c r="H115" s="14"/>
-      <c r="I115" s="14"/>
+      <c r="G115" s="23"/>
+      <c r="H115" s="23"/>
+      <c r="I115" s="23"/>
       <c r="J115" s="10"/>
       <c r="K115" s="10"/>
       <c r="L115" s="10"/>
@@ -4538,9 +4559,9 @@
       <c r="D116" s="10"/>
       <c r="E116" s="10"/>
       <c r="F116" s="10"/>
-      <c r="G116" s="14"/>
-      <c r="H116" s="14"/>
-      <c r="I116" s="14"/>
+      <c r="G116" s="23"/>
+      <c r="H116" s="23"/>
+      <c r="I116" s="23"/>
       <c r="J116" s="10"/>
       <c r="K116" s="10"/>
       <c r="L116" s="10"/>
@@ -4577,10 +4598,10 @@
       <c r="M117" s="10"/>
       <c r="N117" s="10"/>
       <c r="O117" s="10"/>
-      <c r="P117" s="14"/>
-      <c r="Q117" s="14"/>
-      <c r="R117" s="14"/>
-      <c r="S117" s="14"/>
+      <c r="P117" s="23"/>
+      <c r="Q117" s="23"/>
+      <c r="R117" s="23"/>
+      <c r="S117" s="23"/>
       <c r="T117" s="10"/>
       <c r="U117" s="10"/>
       <c r="V117" s="10"/>
@@ -4607,10 +4628,10 @@
       <c r="M118" s="10"/>
       <c r="N118" s="10"/>
       <c r="O118" s="10"/>
-      <c r="P118" s="14"/>
-      <c r="Q118" s="14"/>
-      <c r="R118" s="14"/>
-      <c r="S118" s="14"/>
+      <c r="P118" s="23"/>
+      <c r="Q118" s="23"/>
+      <c r="R118" s="23"/>
+      <c r="S118" s="23"/>
       <c r="T118" s="10"/>
       <c r="U118" s="10"/>
       <c r="V118" s="10"/>
@@ -4683,26 +4704,26 @@
     </row>
     <row r="121" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A121" s="10"/>
-      <c r="B121" s="14"/>
-      <c r="C121" s="14"/>
-      <c r="D121" s="14"/>
-      <c r="E121" s="14"/>
-      <c r="F121" s="14"/>
-      <c r="G121" s="14"/>
-      <c r="H121" s="14"/>
-      <c r="I121" s="14"/>
-      <c r="J121" s="14"/>
-      <c r="K121" s="14"/>
-      <c r="L121" s="14"/>
-      <c r="M121" s="14"/>
-      <c r="N121" s="14"/>
-      <c r="O121" s="14"/>
-      <c r="P121" s="14"/>
-      <c r="Q121" s="14"/>
-      <c r="R121" s="14"/>
-      <c r="S121" s="14"/>
-      <c r="T121" s="14"/>
-      <c r="U121" s="14"/>
+      <c r="B121" s="23"/>
+      <c r="C121" s="23"/>
+      <c r="D121" s="23"/>
+      <c r="E121" s="23"/>
+      <c r="F121" s="23"/>
+      <c r="G121" s="23"/>
+      <c r="H121" s="23"/>
+      <c r="I121" s="23"/>
+      <c r="J121" s="23"/>
+      <c r="K121" s="23"/>
+      <c r="L121" s="23"/>
+      <c r="M121" s="23"/>
+      <c r="N121" s="23"/>
+      <c r="O121" s="23"/>
+      <c r="P121" s="23"/>
+      <c r="Q121" s="23"/>
+      <c r="R121" s="23"/>
+      <c r="S121" s="23"/>
+      <c r="T121" s="23"/>
+      <c r="U121" s="23"/>
       <c r="V121" s="10"/>
       <c r="W121" s="10"/>
       <c r="X121" s="10"/>
@@ -4713,26 +4734,26 @@
     </row>
     <row r="122" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A122" s="10"/>
-      <c r="B122" s="14"/>
-      <c r="C122" s="14"/>
-      <c r="D122" s="14"/>
-      <c r="E122" s="14"/>
-      <c r="F122" s="14"/>
-      <c r="G122" s="14"/>
-      <c r="H122" s="14"/>
-      <c r="I122" s="14"/>
-      <c r="J122" s="14"/>
-      <c r="K122" s="14"/>
-      <c r="L122" s="14"/>
-      <c r="M122" s="14"/>
-      <c r="N122" s="14"/>
-      <c r="O122" s="14"/>
-      <c r="P122" s="14"/>
-      <c r="Q122" s="14"/>
-      <c r="R122" s="14"/>
-      <c r="S122" s="14"/>
-      <c r="T122" s="14"/>
-      <c r="U122" s="14"/>
+      <c r="B122" s="23"/>
+      <c r="C122" s="23"/>
+      <c r="D122" s="23"/>
+      <c r="E122" s="23"/>
+      <c r="F122" s="23"/>
+      <c r="G122" s="23"/>
+      <c r="H122" s="23"/>
+      <c r="I122" s="23"/>
+      <c r="J122" s="23"/>
+      <c r="K122" s="23"/>
+      <c r="L122" s="23"/>
+      <c r="M122" s="23"/>
+      <c r="N122" s="23"/>
+      <c r="O122" s="23"/>
+      <c r="P122" s="23"/>
+      <c r="Q122" s="23"/>
+      <c r="R122" s="23"/>
+      <c r="S122" s="23"/>
+      <c r="T122" s="23"/>
+      <c r="U122" s="23"/>
       <c r="V122" s="10"/>
       <c r="W122" s="10"/>
       <c r="X122" s="10"/>
@@ -4923,26 +4944,26 @@
     </row>
     <row r="129" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A129" s="10"/>
-      <c r="B129" s="14"/>
-      <c r="C129" s="14"/>
-      <c r="D129" s="14"/>
-      <c r="E129" s="14"/>
-      <c r="F129" s="14"/>
-      <c r="G129" s="14"/>
-      <c r="H129" s="14"/>
-      <c r="I129" s="14"/>
-      <c r="J129" s="14"/>
-      <c r="K129" s="14"/>
-      <c r="L129" s="14"/>
-      <c r="M129" s="14"/>
-      <c r="N129" s="14"/>
-      <c r="O129" s="14"/>
-      <c r="P129" s="14"/>
-      <c r="Q129" s="14"/>
-      <c r="R129" s="14"/>
-      <c r="S129" s="14"/>
-      <c r="T129" s="14"/>
-      <c r="U129" s="14"/>
+      <c r="B129" s="23"/>
+      <c r="C129" s="23"/>
+      <c r="D129" s="23"/>
+      <c r="E129" s="23"/>
+      <c r="F129" s="23"/>
+      <c r="G129" s="23"/>
+      <c r="H129" s="23"/>
+      <c r="I129" s="23"/>
+      <c r="J129" s="23"/>
+      <c r="K129" s="23"/>
+      <c r="L129" s="23"/>
+      <c r="M129" s="23"/>
+      <c r="N129" s="23"/>
+      <c r="O129" s="23"/>
+      <c r="P129" s="23"/>
+      <c r="Q129" s="23"/>
+      <c r="R129" s="23"/>
+      <c r="S129" s="23"/>
+      <c r="T129" s="23"/>
+      <c r="U129" s="23"/>
       <c r="V129" s="10"/>
       <c r="W129" s="10"/>
       <c r="X129" s="10"/>
@@ -4953,26 +4974,26 @@
     </row>
     <row r="130" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A130" s="10"/>
-      <c r="B130" s="14"/>
-      <c r="C130" s="14"/>
-      <c r="D130" s="14"/>
-      <c r="E130" s="14"/>
-      <c r="F130" s="14"/>
-      <c r="G130" s="14"/>
-      <c r="H130" s="14"/>
-      <c r="I130" s="14"/>
-      <c r="J130" s="14"/>
-      <c r="K130" s="14"/>
-      <c r="L130" s="14"/>
-      <c r="M130" s="14"/>
-      <c r="N130" s="14"/>
-      <c r="O130" s="14"/>
-      <c r="P130" s="14"/>
-      <c r="Q130" s="14"/>
-      <c r="R130" s="14"/>
-      <c r="S130" s="14"/>
-      <c r="T130" s="14"/>
-      <c r="U130" s="14"/>
+      <c r="B130" s="23"/>
+      <c r="C130" s="23"/>
+      <c r="D130" s="23"/>
+      <c r="E130" s="23"/>
+      <c r="F130" s="23"/>
+      <c r="G130" s="23"/>
+      <c r="H130" s="23"/>
+      <c r="I130" s="23"/>
+      <c r="J130" s="23"/>
+      <c r="K130" s="23"/>
+      <c r="L130" s="23"/>
+      <c r="M130" s="23"/>
+      <c r="N130" s="23"/>
+      <c r="O130" s="23"/>
+      <c r="P130" s="23"/>
+      <c r="Q130" s="23"/>
+      <c r="R130" s="23"/>
+      <c r="S130" s="23"/>
+      <c r="T130" s="23"/>
+      <c r="U130" s="23"/>
       <c r="V130" s="10"/>
       <c r="W130" s="10"/>
       <c r="X130" s="10"/>
@@ -5281,11 +5302,10 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="R5:U5"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="C28:J28"/>
-    <mergeCell ref="B121:U122"/>
+    <mergeCell ref="B73:U74"/>
+    <mergeCell ref="B89:U90"/>
+    <mergeCell ref="B97:U98"/>
+    <mergeCell ref="B41:U42"/>
     <mergeCell ref="B129:U130"/>
     <mergeCell ref="B105:U106"/>
     <mergeCell ref="B113:U114"/>
@@ -5293,15 +5313,16 @@
     <mergeCell ref="G116:I116"/>
     <mergeCell ref="P117:S117"/>
     <mergeCell ref="P118:S118"/>
-    <mergeCell ref="B73:U74"/>
-    <mergeCell ref="B89:U90"/>
-    <mergeCell ref="B97:U98"/>
-    <mergeCell ref="B41:U42"/>
+    <mergeCell ref="B121:U122"/>
     <mergeCell ref="B1:U2"/>
     <mergeCell ref="B9:U10"/>
     <mergeCell ref="B17:U18"/>
     <mergeCell ref="B25:U26"/>
     <mergeCell ref="B33:U34"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="C28:J28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
lcdController done (untested) added encoderController
</commit_message>
<xml_diff>
--- a/LCD User Interface.xlsx
+++ b/LCD User Interface.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Stromvy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46976388-7E1A-4FD2-8B1A-363CC4544458}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DD261E-A882-4B9F-BC79-37BE89579C5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -495,6 +494,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -508,9 +510,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -804,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="X35" sqref="X35"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -816,50 +815,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
@@ -909,11 +908,11 @@
         <v>65</v>
       </c>
       <c r="Q3" s="1"/>
-      <c r="R3" s="20" t="s">
+      <c r="R3" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="S3" s="22"/>
-      <c r="T3" s="21"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="22"/>
       <c r="U3" s="1"/>
       <c r="W3" s="15"/>
       <c r="X3" s="15"/>
@@ -974,10 +973,10 @@
         <v>2</v>
       </c>
       <c r="Q4" s="1"/>
-      <c r="R4" s="20" t="s">
+      <c r="R4" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="S4" s="21"/>
+      <c r="S4" s="22"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="W4" s="15"/>
@@ -1106,11 +1105,11 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="20" t="s">
+      <c r="R6" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="S6" s="22"/>
-      <c r="T6" s="21"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="22"/>
       <c r="U6" s="12"/>
       <c r="W6" s="15"/>
       <c r="X6" s="15"/>
@@ -1202,28 +1201,28 @@
       <c r="AD8" s="15"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
       <c r="W9" s="15"/>
       <c r="X9" s="15"/>
       <c r="Y9" s="15"/>
@@ -1234,26 +1233,26 @@
       <c r="AD9" s="15"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="20"/>
       <c r="W10" s="15"/>
       <c r="X10" s="15"/>
       <c r="Y10" s="15"/>
@@ -1627,28 +1626,28 @@
       <c r="AK16" s="16"/>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
       <c r="W17" s="15"/>
       <c r="X17" s="15"/>
       <c r="Y17" s="15"/>
@@ -1666,26 +1665,26 @@
       <c r="AK17" s="16"/>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="19"/>
-      <c r="S18" s="19"/>
-      <c r="T18" s="19"/>
-      <c r="U18" s="19"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
+      <c r="T18" s="20"/>
+      <c r="U18" s="20"/>
       <c r="W18" s="15"/>
       <c r="X18" s="15"/>
       <c r="Y18" s="15"/>
@@ -2044,28 +2043,28 @@
       <c r="AK24" s="16"/>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="18"/>
-      <c r="P25" s="18"/>
-      <c r="Q25" s="18"/>
-      <c r="R25" s="18"/>
-      <c r="S25" s="18"/>
-      <c r="T25" s="18"/>
-      <c r="U25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="19"/>
       <c r="AE25" s="16"/>
       <c r="AF25" s="16"/>
       <c r="AG25" s="16"/>
@@ -2075,26 +2074,26 @@
       <c r="AK25" s="16"/>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19"/>
-      <c r="O26" s="19"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="19"/>
-      <c r="S26" s="19"/>
-      <c r="T26" s="19"/>
-      <c r="U26" s="19"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="20"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="20"/>
+      <c r="S26" s="20"/>
+      <c r="T26" s="20"/>
+      <c r="U26" s="20"/>
       <c r="AE26" s="16"/>
       <c r="AF26" s="16"/>
       <c r="AG26" s="16"/>
@@ -2436,28 +2435,28 @@
       <c r="AK32" s="16"/>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18"/>
-      <c r="O33" s="18"/>
-      <c r="P33" s="18"/>
-      <c r="Q33" s="18"/>
-      <c r="R33" s="18"/>
-      <c r="S33" s="18"/>
-      <c r="T33" s="18"/>
-      <c r="U33" s="18"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
+      <c r="U33" s="19"/>
       <c r="AF33" s="16"/>
       <c r="AG33" s="16"/>
       <c r="AH33" s="16"/>
@@ -2466,26 +2465,26 @@
       <c r="AK33" s="16"/>
     </row>
     <row r="34" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
-      <c r="O34" s="19"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="19"/>
-      <c r="R34" s="19"/>
-      <c r="S34" s="19"/>
-      <c r="T34" s="19"/>
-      <c r="U34" s="19"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="20"/>
+      <c r="O34" s="20"/>
+      <c r="P34" s="20"/>
+      <c r="Q34" s="20"/>
+      <c r="R34" s="20"/>
+      <c r="S34" s="20"/>
+      <c r="T34" s="20"/>
+      <c r="U34" s="20"/>
       <c r="AF34" s="16"/>
       <c r="AG34" s="16"/>
       <c r="AH34" s="16"/>
@@ -2847,28 +2846,28 @@
       <c r="AK40" s="16"/>
     </row>
     <row r="41" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-      <c r="N41" s="18"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="18"/>
-      <c r="Q41" s="18"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="18"/>
-      <c r="T41" s="18"/>
-      <c r="U41" s="18"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="19"/>
+      <c r="O41" s="19"/>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="19"/>
+      <c r="R41" s="19"/>
+      <c r="S41" s="19"/>
+      <c r="T41" s="19"/>
+      <c r="U41" s="19"/>
       <c r="AA41" s="10"/>
       <c r="AB41" s="10"/>
       <c r="AC41" s="10"/>
@@ -2882,26 +2881,26 @@
       <c r="AK41" s="16"/>
     </row>
     <row r="42" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="19"/>
-      <c r="M42" s="19"/>
-      <c r="N42" s="19"/>
-      <c r="O42" s="19"/>
-      <c r="P42" s="19"/>
-      <c r="Q42" s="19"/>
-      <c r="R42" s="19"/>
-      <c r="S42" s="19"/>
-      <c r="T42" s="19"/>
-      <c r="U42" s="19"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="20"/>
+      <c r="O42" s="20"/>
+      <c r="P42" s="20"/>
+      <c r="Q42" s="20"/>
+      <c r="R42" s="20"/>
+      <c r="S42" s="20"/>
+      <c r="T42" s="20"/>
+      <c r="U42" s="20"/>
       <c r="AA42" s="10"/>
       <c r="AB42" s="10"/>
       <c r="AC42" s="10"/>
@@ -3492,26 +3491,26 @@
     </row>
     <row r="73" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A73" s="10"/>
-      <c r="B73" s="23"/>
-      <c r="C73" s="23"/>
-      <c r="D73" s="23"/>
-      <c r="E73" s="23"/>
-      <c r="F73" s="23"/>
-      <c r="G73" s="23"/>
-      <c r="H73" s="23"/>
-      <c r="I73" s="23"/>
-      <c r="J73" s="23"/>
-      <c r="K73" s="23"/>
-      <c r="L73" s="23"/>
-      <c r="M73" s="23"/>
-      <c r="N73" s="23"/>
-      <c r="O73" s="23"/>
-      <c r="P73" s="23"/>
-      <c r="Q73" s="23"/>
-      <c r="R73" s="23"/>
-      <c r="S73" s="23"/>
-      <c r="T73" s="23"/>
-      <c r="U73" s="23"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="18"/>
+      <c r="G73" s="18"/>
+      <c r="H73" s="18"/>
+      <c r="I73" s="18"/>
+      <c r="J73" s="18"/>
+      <c r="K73" s="18"/>
+      <c r="L73" s="18"/>
+      <c r="M73" s="18"/>
+      <c r="N73" s="18"/>
+      <c r="O73" s="18"/>
+      <c r="P73" s="18"/>
+      <c r="Q73" s="18"/>
+      <c r="R73" s="18"/>
+      <c r="S73" s="18"/>
+      <c r="T73" s="18"/>
+      <c r="U73" s="18"/>
       <c r="V73" s="10"/>
       <c r="W73" s="10"/>
       <c r="X73" s="10"/>
@@ -3520,26 +3519,26 @@
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A74" s="10"/>
-      <c r="B74" s="23"/>
-      <c r="C74" s="23"/>
-      <c r="D74" s="23"/>
-      <c r="E74" s="23"/>
-      <c r="F74" s="23"/>
-      <c r="G74" s="23"/>
-      <c r="H74" s="23"/>
-      <c r="I74" s="23"/>
-      <c r="J74" s="23"/>
-      <c r="K74" s="23"/>
-      <c r="L74" s="23"/>
-      <c r="M74" s="23"/>
-      <c r="N74" s="23"/>
-      <c r="O74" s="23"/>
-      <c r="P74" s="23"/>
-      <c r="Q74" s="23"/>
-      <c r="R74" s="23"/>
-      <c r="S74" s="23"/>
-      <c r="T74" s="23"/>
-      <c r="U74" s="23"/>
+      <c r="B74" s="18"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
+      <c r="G74" s="18"/>
+      <c r="H74" s="18"/>
+      <c r="I74" s="18"/>
+      <c r="J74" s="18"/>
+      <c r="K74" s="18"/>
+      <c r="L74" s="18"/>
+      <c r="M74" s="18"/>
+      <c r="N74" s="18"/>
+      <c r="O74" s="18"/>
+      <c r="P74" s="18"/>
+      <c r="Q74" s="18"/>
+      <c r="R74" s="18"/>
+      <c r="S74" s="18"/>
+      <c r="T74" s="18"/>
+      <c r="U74" s="18"/>
       <c r="V74" s="10"/>
       <c r="W74" s="10"/>
       <c r="X74" s="10"/>
@@ -3744,26 +3743,26 @@
     </row>
     <row r="89" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A89" s="10"/>
-      <c r="B89" s="23"/>
-      <c r="C89" s="23"/>
-      <c r="D89" s="23"/>
-      <c r="E89" s="23"/>
-      <c r="F89" s="23"/>
-      <c r="G89" s="23"/>
-      <c r="H89" s="23"/>
-      <c r="I89" s="23"/>
-      <c r="J89" s="23"/>
-      <c r="K89" s="23"/>
-      <c r="L89" s="23"/>
-      <c r="M89" s="23"/>
-      <c r="N89" s="23"/>
-      <c r="O89" s="23"/>
-      <c r="P89" s="23"/>
-      <c r="Q89" s="23"/>
-      <c r="R89" s="23"/>
-      <c r="S89" s="23"/>
-      <c r="T89" s="23"/>
-      <c r="U89" s="23"/>
+      <c r="B89" s="18"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="18"/>
+      <c r="E89" s="18"/>
+      <c r="F89" s="18"/>
+      <c r="G89" s="18"/>
+      <c r="H89" s="18"/>
+      <c r="I89" s="18"/>
+      <c r="J89" s="18"/>
+      <c r="K89" s="18"/>
+      <c r="L89" s="18"/>
+      <c r="M89" s="18"/>
+      <c r="N89" s="18"/>
+      <c r="O89" s="18"/>
+      <c r="P89" s="18"/>
+      <c r="Q89" s="18"/>
+      <c r="R89" s="18"/>
+      <c r="S89" s="18"/>
+      <c r="T89" s="18"/>
+      <c r="U89" s="18"/>
       <c r="V89" s="10"/>
       <c r="W89" s="10"/>
       <c r="X89" s="10"/>
@@ -3774,26 +3773,26 @@
     </row>
     <row r="90" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A90" s="10"/>
-      <c r="B90" s="23"/>
-      <c r="C90" s="23"/>
-      <c r="D90" s="23"/>
-      <c r="E90" s="23"/>
-      <c r="F90" s="23"/>
-      <c r="G90" s="23"/>
-      <c r="H90" s="23"/>
-      <c r="I90" s="23"/>
-      <c r="J90" s="23"/>
-      <c r="K90" s="23"/>
-      <c r="L90" s="23"/>
-      <c r="M90" s="23"/>
-      <c r="N90" s="23"/>
-      <c r="O90" s="23"/>
-      <c r="P90" s="23"/>
-      <c r="Q90" s="23"/>
-      <c r="R90" s="23"/>
-      <c r="S90" s="23"/>
-      <c r="T90" s="23"/>
-      <c r="U90" s="23"/>
+      <c r="B90" s="18"/>
+      <c r="C90" s="18"/>
+      <c r="D90" s="18"/>
+      <c r="E90" s="18"/>
+      <c r="F90" s="18"/>
+      <c r="G90" s="18"/>
+      <c r="H90" s="18"/>
+      <c r="I90" s="18"/>
+      <c r="J90" s="18"/>
+      <c r="K90" s="18"/>
+      <c r="L90" s="18"/>
+      <c r="M90" s="18"/>
+      <c r="N90" s="18"/>
+      <c r="O90" s="18"/>
+      <c r="P90" s="18"/>
+      <c r="Q90" s="18"/>
+      <c r="R90" s="18"/>
+      <c r="S90" s="18"/>
+      <c r="T90" s="18"/>
+      <c r="U90" s="18"/>
       <c r="V90" s="10"/>
       <c r="W90" s="10"/>
       <c r="X90" s="10"/>
@@ -3984,26 +3983,26 @@
     </row>
     <row r="97" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A97" s="10"/>
-      <c r="B97" s="23"/>
-      <c r="C97" s="23"/>
-      <c r="D97" s="23"/>
-      <c r="E97" s="23"/>
-      <c r="F97" s="23"/>
-      <c r="G97" s="23"/>
-      <c r="H97" s="23"/>
-      <c r="I97" s="23"/>
-      <c r="J97" s="23"/>
-      <c r="K97" s="23"/>
-      <c r="L97" s="23"/>
-      <c r="M97" s="23"/>
-      <c r="N97" s="23"/>
-      <c r="O97" s="23"/>
-      <c r="P97" s="23"/>
-      <c r="Q97" s="23"/>
-      <c r="R97" s="23"/>
-      <c r="S97" s="23"/>
-      <c r="T97" s="23"/>
-      <c r="U97" s="23"/>
+      <c r="B97" s="18"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="18"/>
+      <c r="E97" s="18"/>
+      <c r="F97" s="18"/>
+      <c r="G97" s="18"/>
+      <c r="H97" s="18"/>
+      <c r="I97" s="18"/>
+      <c r="J97" s="18"/>
+      <c r="K97" s="18"/>
+      <c r="L97" s="18"/>
+      <c r="M97" s="18"/>
+      <c r="N97" s="18"/>
+      <c r="O97" s="18"/>
+      <c r="P97" s="18"/>
+      <c r="Q97" s="18"/>
+      <c r="R97" s="18"/>
+      <c r="S97" s="18"/>
+      <c r="T97" s="18"/>
+      <c r="U97" s="18"/>
       <c r="V97" s="10"/>
       <c r="W97" s="10"/>
       <c r="X97" s="10"/>
@@ -4014,26 +4013,26 @@
     </row>
     <row r="98" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A98" s="10"/>
-      <c r="B98" s="23"/>
-      <c r="C98" s="23"/>
-      <c r="D98" s="23"/>
-      <c r="E98" s="23"/>
-      <c r="F98" s="23"/>
-      <c r="G98" s="23"/>
-      <c r="H98" s="23"/>
-      <c r="I98" s="23"/>
-      <c r="J98" s="23"/>
-      <c r="K98" s="23"/>
-      <c r="L98" s="23"/>
-      <c r="M98" s="23"/>
-      <c r="N98" s="23"/>
-      <c r="O98" s="23"/>
-      <c r="P98" s="23"/>
-      <c r="Q98" s="23"/>
-      <c r="R98" s="23"/>
-      <c r="S98" s="23"/>
-      <c r="T98" s="23"/>
-      <c r="U98" s="23"/>
+      <c r="B98" s="18"/>
+      <c r="C98" s="18"/>
+      <c r="D98" s="18"/>
+      <c r="E98" s="18"/>
+      <c r="F98" s="18"/>
+      <c r="G98" s="18"/>
+      <c r="H98" s="18"/>
+      <c r="I98" s="18"/>
+      <c r="J98" s="18"/>
+      <c r="K98" s="18"/>
+      <c r="L98" s="18"/>
+      <c r="M98" s="18"/>
+      <c r="N98" s="18"/>
+      <c r="O98" s="18"/>
+      <c r="P98" s="18"/>
+      <c r="Q98" s="18"/>
+      <c r="R98" s="18"/>
+      <c r="S98" s="18"/>
+      <c r="T98" s="18"/>
+      <c r="U98" s="18"/>
       <c r="V98" s="10"/>
       <c r="W98" s="10"/>
       <c r="X98" s="10"/>
@@ -4224,26 +4223,26 @@
     </row>
     <row r="105" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A105" s="10"/>
-      <c r="B105" s="23"/>
-      <c r="C105" s="23"/>
-      <c r="D105" s="23"/>
-      <c r="E105" s="23"/>
-      <c r="F105" s="23"/>
-      <c r="G105" s="23"/>
-      <c r="H105" s="23"/>
-      <c r="I105" s="23"/>
-      <c r="J105" s="23"/>
-      <c r="K105" s="23"/>
-      <c r="L105" s="23"/>
-      <c r="M105" s="23"/>
-      <c r="N105" s="23"/>
-      <c r="O105" s="23"/>
-      <c r="P105" s="23"/>
-      <c r="Q105" s="23"/>
-      <c r="R105" s="23"/>
-      <c r="S105" s="23"/>
-      <c r="T105" s="23"/>
-      <c r="U105" s="23"/>
+      <c r="B105" s="18"/>
+      <c r="C105" s="18"/>
+      <c r="D105" s="18"/>
+      <c r="E105" s="18"/>
+      <c r="F105" s="18"/>
+      <c r="G105" s="18"/>
+      <c r="H105" s="18"/>
+      <c r="I105" s="18"/>
+      <c r="J105" s="18"/>
+      <c r="K105" s="18"/>
+      <c r="L105" s="18"/>
+      <c r="M105" s="18"/>
+      <c r="N105" s="18"/>
+      <c r="O105" s="18"/>
+      <c r="P105" s="18"/>
+      <c r="Q105" s="18"/>
+      <c r="R105" s="18"/>
+      <c r="S105" s="18"/>
+      <c r="T105" s="18"/>
+      <c r="U105" s="18"/>
       <c r="V105" s="10"/>
       <c r="W105" s="10"/>
       <c r="X105" s="10"/>
@@ -4254,26 +4253,26 @@
     </row>
     <row r="106" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A106" s="10"/>
-      <c r="B106" s="23"/>
-      <c r="C106" s="23"/>
-      <c r="D106" s="23"/>
-      <c r="E106" s="23"/>
-      <c r="F106" s="23"/>
-      <c r="G106" s="23"/>
-      <c r="H106" s="23"/>
-      <c r="I106" s="23"/>
-      <c r="J106" s="23"/>
-      <c r="K106" s="23"/>
-      <c r="L106" s="23"/>
-      <c r="M106" s="23"/>
-      <c r="N106" s="23"/>
-      <c r="O106" s="23"/>
-      <c r="P106" s="23"/>
-      <c r="Q106" s="23"/>
-      <c r="R106" s="23"/>
-      <c r="S106" s="23"/>
-      <c r="T106" s="23"/>
-      <c r="U106" s="23"/>
+      <c r="B106" s="18"/>
+      <c r="C106" s="18"/>
+      <c r="D106" s="18"/>
+      <c r="E106" s="18"/>
+      <c r="F106" s="18"/>
+      <c r="G106" s="18"/>
+      <c r="H106" s="18"/>
+      <c r="I106" s="18"/>
+      <c r="J106" s="18"/>
+      <c r="K106" s="18"/>
+      <c r="L106" s="18"/>
+      <c r="M106" s="18"/>
+      <c r="N106" s="18"/>
+      <c r="O106" s="18"/>
+      <c r="P106" s="18"/>
+      <c r="Q106" s="18"/>
+      <c r="R106" s="18"/>
+      <c r="S106" s="18"/>
+      <c r="T106" s="18"/>
+      <c r="U106" s="18"/>
       <c r="V106" s="10"/>
       <c r="W106" s="10"/>
       <c r="X106" s="10"/>
@@ -4464,26 +4463,26 @@
     </row>
     <row r="113" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A113" s="10"/>
-      <c r="B113" s="23"/>
-      <c r="C113" s="23"/>
-      <c r="D113" s="23"/>
-      <c r="E113" s="23"/>
-      <c r="F113" s="23"/>
-      <c r="G113" s="23"/>
-      <c r="H113" s="23"/>
-      <c r="I113" s="23"/>
-      <c r="J113" s="23"/>
-      <c r="K113" s="23"/>
-      <c r="L113" s="23"/>
-      <c r="M113" s="23"/>
-      <c r="N113" s="23"/>
-      <c r="O113" s="23"/>
-      <c r="P113" s="23"/>
-      <c r="Q113" s="23"/>
-      <c r="R113" s="23"/>
-      <c r="S113" s="23"/>
-      <c r="T113" s="23"/>
-      <c r="U113" s="23"/>
+      <c r="B113" s="18"/>
+      <c r="C113" s="18"/>
+      <c r="D113" s="18"/>
+      <c r="E113" s="18"/>
+      <c r="F113" s="18"/>
+      <c r="G113" s="18"/>
+      <c r="H113" s="18"/>
+      <c r="I113" s="18"/>
+      <c r="J113" s="18"/>
+      <c r="K113" s="18"/>
+      <c r="L113" s="18"/>
+      <c r="M113" s="18"/>
+      <c r="N113" s="18"/>
+      <c r="O113" s="18"/>
+      <c r="P113" s="18"/>
+      <c r="Q113" s="18"/>
+      <c r="R113" s="18"/>
+      <c r="S113" s="18"/>
+      <c r="T113" s="18"/>
+      <c r="U113" s="18"/>
       <c r="V113" s="10"/>
       <c r="W113" s="10"/>
       <c r="X113" s="10"/>
@@ -4494,26 +4493,26 @@
     </row>
     <row r="114" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A114" s="10"/>
-      <c r="B114" s="23"/>
-      <c r="C114" s="23"/>
-      <c r="D114" s="23"/>
-      <c r="E114" s="23"/>
-      <c r="F114" s="23"/>
-      <c r="G114" s="23"/>
-      <c r="H114" s="23"/>
-      <c r="I114" s="23"/>
-      <c r="J114" s="23"/>
-      <c r="K114" s="23"/>
-      <c r="L114" s="23"/>
-      <c r="M114" s="23"/>
-      <c r="N114" s="23"/>
-      <c r="O114" s="23"/>
-      <c r="P114" s="23"/>
-      <c r="Q114" s="23"/>
-      <c r="R114" s="23"/>
-      <c r="S114" s="23"/>
-      <c r="T114" s="23"/>
-      <c r="U114" s="23"/>
+      <c r="B114" s="18"/>
+      <c r="C114" s="18"/>
+      <c r="D114" s="18"/>
+      <c r="E114" s="18"/>
+      <c r="F114" s="18"/>
+      <c r="G114" s="18"/>
+      <c r="H114" s="18"/>
+      <c r="I114" s="18"/>
+      <c r="J114" s="18"/>
+      <c r="K114" s="18"/>
+      <c r="L114" s="18"/>
+      <c r="M114" s="18"/>
+      <c r="N114" s="18"/>
+      <c r="O114" s="18"/>
+      <c r="P114" s="18"/>
+      <c r="Q114" s="18"/>
+      <c r="R114" s="18"/>
+      <c r="S114" s="18"/>
+      <c r="T114" s="18"/>
+      <c r="U114" s="18"/>
       <c r="V114" s="10"/>
       <c r="W114" s="10"/>
       <c r="X114" s="10"/>
@@ -4529,9 +4528,9 @@
       <c r="D115" s="10"/>
       <c r="E115" s="10"/>
       <c r="F115" s="10"/>
-      <c r="G115" s="23"/>
-      <c r="H115" s="23"/>
-      <c r="I115" s="23"/>
+      <c r="G115" s="18"/>
+      <c r="H115" s="18"/>
+      <c r="I115" s="18"/>
       <c r="J115" s="10"/>
       <c r="K115" s="10"/>
       <c r="L115" s="10"/>
@@ -4559,9 +4558,9 @@
       <c r="D116" s="10"/>
       <c r="E116" s="10"/>
       <c r="F116" s="10"/>
-      <c r="G116" s="23"/>
-      <c r="H116" s="23"/>
-      <c r="I116" s="23"/>
+      <c r="G116" s="18"/>
+      <c r="H116" s="18"/>
+      <c r="I116" s="18"/>
       <c r="J116" s="10"/>
       <c r="K116" s="10"/>
       <c r="L116" s="10"/>
@@ -4598,10 +4597,10 @@
       <c r="M117" s="10"/>
       <c r="N117" s="10"/>
       <c r="O117" s="10"/>
-      <c r="P117" s="23"/>
-      <c r="Q117" s="23"/>
-      <c r="R117" s="23"/>
-      <c r="S117" s="23"/>
+      <c r="P117" s="18"/>
+      <c r="Q117" s="18"/>
+      <c r="R117" s="18"/>
+      <c r="S117" s="18"/>
       <c r="T117" s="10"/>
       <c r="U117" s="10"/>
       <c r="V117" s="10"/>
@@ -4628,10 +4627,10 @@
       <c r="M118" s="10"/>
       <c r="N118" s="10"/>
       <c r="O118" s="10"/>
-      <c r="P118" s="23"/>
-      <c r="Q118" s="23"/>
-      <c r="R118" s="23"/>
-      <c r="S118" s="23"/>
+      <c r="P118" s="18"/>
+      <c r="Q118" s="18"/>
+      <c r="R118" s="18"/>
+      <c r="S118" s="18"/>
       <c r="T118" s="10"/>
       <c r="U118" s="10"/>
       <c r="V118" s="10"/>
@@ -4704,26 +4703,26 @@
     </row>
     <row r="121" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A121" s="10"/>
-      <c r="B121" s="23"/>
-      <c r="C121" s="23"/>
-      <c r="D121" s="23"/>
-      <c r="E121" s="23"/>
-      <c r="F121" s="23"/>
-      <c r="G121" s="23"/>
-      <c r="H121" s="23"/>
-      <c r="I121" s="23"/>
-      <c r="J121" s="23"/>
-      <c r="K121" s="23"/>
-      <c r="L121" s="23"/>
-      <c r="M121" s="23"/>
-      <c r="N121" s="23"/>
-      <c r="O121" s="23"/>
-      <c r="P121" s="23"/>
-      <c r="Q121" s="23"/>
-      <c r="R121" s="23"/>
-      <c r="S121" s="23"/>
-      <c r="T121" s="23"/>
-      <c r="U121" s="23"/>
+      <c r="B121" s="18"/>
+      <c r="C121" s="18"/>
+      <c r="D121" s="18"/>
+      <c r="E121" s="18"/>
+      <c r="F121" s="18"/>
+      <c r="G121" s="18"/>
+      <c r="H121" s="18"/>
+      <c r="I121" s="18"/>
+      <c r="J121" s="18"/>
+      <c r="K121" s="18"/>
+      <c r="L121" s="18"/>
+      <c r="M121" s="18"/>
+      <c r="N121" s="18"/>
+      <c r="O121" s="18"/>
+      <c r="P121" s="18"/>
+      <c r="Q121" s="18"/>
+      <c r="R121" s="18"/>
+      <c r="S121" s="18"/>
+      <c r="T121" s="18"/>
+      <c r="U121" s="18"/>
       <c r="V121" s="10"/>
       <c r="W121" s="10"/>
       <c r="X121" s="10"/>
@@ -4734,26 +4733,26 @@
     </row>
     <row r="122" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A122" s="10"/>
-      <c r="B122" s="23"/>
-      <c r="C122" s="23"/>
-      <c r="D122" s="23"/>
-      <c r="E122" s="23"/>
-      <c r="F122" s="23"/>
-      <c r="G122" s="23"/>
-      <c r="H122" s="23"/>
-      <c r="I122" s="23"/>
-      <c r="J122" s="23"/>
-      <c r="K122" s="23"/>
-      <c r="L122" s="23"/>
-      <c r="M122" s="23"/>
-      <c r="N122" s="23"/>
-      <c r="O122" s="23"/>
-      <c r="P122" s="23"/>
-      <c r="Q122" s="23"/>
-      <c r="R122" s="23"/>
-      <c r="S122" s="23"/>
-      <c r="T122" s="23"/>
-      <c r="U122" s="23"/>
+      <c r="B122" s="18"/>
+      <c r="C122" s="18"/>
+      <c r="D122" s="18"/>
+      <c r="E122" s="18"/>
+      <c r="F122" s="18"/>
+      <c r="G122" s="18"/>
+      <c r="H122" s="18"/>
+      <c r="I122" s="18"/>
+      <c r="J122" s="18"/>
+      <c r="K122" s="18"/>
+      <c r="L122" s="18"/>
+      <c r="M122" s="18"/>
+      <c r="N122" s="18"/>
+      <c r="O122" s="18"/>
+      <c r="P122" s="18"/>
+      <c r="Q122" s="18"/>
+      <c r="R122" s="18"/>
+      <c r="S122" s="18"/>
+      <c r="T122" s="18"/>
+      <c r="U122" s="18"/>
       <c r="V122" s="10"/>
       <c r="W122" s="10"/>
       <c r="X122" s="10"/>
@@ -4944,26 +4943,26 @@
     </row>
     <row r="129" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A129" s="10"/>
-      <c r="B129" s="23"/>
-      <c r="C129" s="23"/>
-      <c r="D129" s="23"/>
-      <c r="E129" s="23"/>
-      <c r="F129" s="23"/>
-      <c r="G129" s="23"/>
-      <c r="H129" s="23"/>
-      <c r="I129" s="23"/>
-      <c r="J129" s="23"/>
-      <c r="K129" s="23"/>
-      <c r="L129" s="23"/>
-      <c r="M129" s="23"/>
-      <c r="N129" s="23"/>
-      <c r="O129" s="23"/>
-      <c r="P129" s="23"/>
-      <c r="Q129" s="23"/>
-      <c r="R129" s="23"/>
-      <c r="S129" s="23"/>
-      <c r="T129" s="23"/>
-      <c r="U129" s="23"/>
+      <c r="B129" s="18"/>
+      <c r="C129" s="18"/>
+      <c r="D129" s="18"/>
+      <c r="E129" s="18"/>
+      <c r="F129" s="18"/>
+      <c r="G129" s="18"/>
+      <c r="H129" s="18"/>
+      <c r="I129" s="18"/>
+      <c r="J129" s="18"/>
+      <c r="K129" s="18"/>
+      <c r="L129" s="18"/>
+      <c r="M129" s="18"/>
+      <c r="N129" s="18"/>
+      <c r="O129" s="18"/>
+      <c r="P129" s="18"/>
+      <c r="Q129" s="18"/>
+      <c r="R129" s="18"/>
+      <c r="S129" s="18"/>
+      <c r="T129" s="18"/>
+      <c r="U129" s="18"/>
       <c r="V129" s="10"/>
       <c r="W129" s="10"/>
       <c r="X129" s="10"/>
@@ -4974,26 +4973,26 @@
     </row>
     <row r="130" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A130" s="10"/>
-      <c r="B130" s="23"/>
-      <c r="C130" s="23"/>
-      <c r="D130" s="23"/>
-      <c r="E130" s="23"/>
-      <c r="F130" s="23"/>
-      <c r="G130" s="23"/>
-      <c r="H130" s="23"/>
-      <c r="I130" s="23"/>
-      <c r="J130" s="23"/>
-      <c r="K130" s="23"/>
-      <c r="L130" s="23"/>
-      <c r="M130" s="23"/>
-      <c r="N130" s="23"/>
-      <c r="O130" s="23"/>
-      <c r="P130" s="23"/>
-      <c r="Q130" s="23"/>
-      <c r="R130" s="23"/>
-      <c r="S130" s="23"/>
-      <c r="T130" s="23"/>
-      <c r="U130" s="23"/>
+      <c r="B130" s="18"/>
+      <c r="C130" s="18"/>
+      <c r="D130" s="18"/>
+      <c r="E130" s="18"/>
+      <c r="F130" s="18"/>
+      <c r="G130" s="18"/>
+      <c r="H130" s="18"/>
+      <c r="I130" s="18"/>
+      <c r="J130" s="18"/>
+      <c r="K130" s="18"/>
+      <c r="L130" s="18"/>
+      <c r="M130" s="18"/>
+      <c r="N130" s="18"/>
+      <c r="O130" s="18"/>
+      <c r="P130" s="18"/>
+      <c r="Q130" s="18"/>
+      <c r="R130" s="18"/>
+      <c r="S130" s="18"/>
+      <c r="T130" s="18"/>
+      <c r="U130" s="18"/>
       <c r="V130" s="10"/>
       <c r="W130" s="10"/>
       <c r="X130" s="10"/>
@@ -5302,6 +5301,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B1:U2"/>
+    <mergeCell ref="B9:U10"/>
+    <mergeCell ref="B17:U18"/>
+    <mergeCell ref="B25:U26"/>
+    <mergeCell ref="B33:U34"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="C28:J28"/>
     <mergeCell ref="B73:U74"/>
     <mergeCell ref="B89:U90"/>
     <mergeCell ref="B97:U98"/>
@@ -5314,15 +5322,6 @@
     <mergeCell ref="P117:S117"/>
     <mergeCell ref="P118:S118"/>
     <mergeCell ref="B121:U122"/>
-    <mergeCell ref="B1:U2"/>
-    <mergeCell ref="B9:U10"/>
-    <mergeCell ref="B17:U18"/>
-    <mergeCell ref="B25:U26"/>
-    <mergeCell ref="B33:U34"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="C28:J28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
lcdController and encoderController work Added navigations
</commit_message>
<xml_diff>
--- a/LCD User Interface.xlsx
+++ b/LCD User Interface.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Stromvy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DD261E-A882-4B9F-BC79-37BE89579C5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DD2289-3362-4755-993D-FE5F719D4676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="102">
   <si>
     <t>x</t>
   </si>
@@ -289,13 +289,335 @@
   </si>
   <si>
     <t>)</t>
+  </si>
+  <si>
+    <r>
+      <t>#define</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> MAX_V_DAC </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>5000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>#define</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> MAX_I_ADC </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>5000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>#define</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> MIN_V_ADC </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>#define</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> MIN_I_ADC </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>#define</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> MAX_TIMER_DURATION </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>36000000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>#define</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> MIN_TIMER_DURATION </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>#define</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> MAX_LOG_INTERVAL </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>60000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>#define</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> MIN_LOG_INTERVAL </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>200</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>#define</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> MIN_FAN_PWM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>#define</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> MAX_FAN_PWM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>100</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>#define</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> MIN_FAN_TEMP </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>#define</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> MAX_FAN_TEMP </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>99</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>#define</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> MAX_CALIBRATION_FACTOR </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>10.0000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>#define</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> MIN_CALIBRATION_FACTOR </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0.0001</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,6 +656,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC586C0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF569CD6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFB5CEA8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="6">
@@ -441,7 +781,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -494,9 +834,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -520,6 +857,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -804,7 +1147,7 @@
   <dimension ref="A1:AK150"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="C45" sqref="C45:H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -815,50 +1158,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
@@ -908,11 +1251,11 @@
         <v>65</v>
       </c>
       <c r="Q3" s="1"/>
-      <c r="R3" s="21" t="s">
+      <c r="R3" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="S3" s="23"/>
-      <c r="T3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="21"/>
       <c r="U3" s="1"/>
       <c r="W3" s="15"/>
       <c r="X3" s="15"/>
@@ -973,10 +1316,10 @@
         <v>2</v>
       </c>
       <c r="Q4" s="1"/>
-      <c r="R4" s="21" t="s">
+      <c r="R4" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="S4" s="22"/>
+      <c r="S4" s="21"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="W4" s="15"/>
@@ -1105,11 +1448,11 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="21" t="s">
+      <c r="R6" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="S6" s="23"/>
-      <c r="T6" s="22"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="21"/>
       <c r="U6" s="12"/>
       <c r="W6" s="15"/>
       <c r="X6" s="15"/>
@@ -1201,28 +1544,28 @@
       <c r="AD8" s="15"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="19"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="18"/>
       <c r="W9" s="15"/>
       <c r="X9" s="15"/>
       <c r="Y9" s="15"/>
@@ -1233,26 +1576,26 @@
       <c r="AD9" s="15"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="20"/>
-      <c r="U10" s="20"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
       <c r="W10" s="15"/>
       <c r="X10" s="15"/>
       <c r="Y10" s="15"/>
@@ -1626,28 +1969,28 @@
       <c r="AK16" s="16"/>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="19"/>
-      <c r="S17" s="19"/>
-      <c r="T17" s="19"/>
-      <c r="U17" s="19"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18"/>
+      <c r="S17" s="18"/>
+      <c r="T17" s="18"/>
+      <c r="U17" s="18"/>
       <c r="W17" s="15"/>
       <c r="X17" s="15"/>
       <c r="Y17" s="15"/>
@@ -1665,26 +2008,26 @@
       <c r="AK17" s="16"/>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="20"/>
-      <c r="S18" s="20"/>
-      <c r="T18" s="20"/>
-      <c r="U18" s="20"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="19"/>
       <c r="W18" s="15"/>
       <c r="X18" s="15"/>
       <c r="Y18" s="15"/>
@@ -2043,28 +2386,28 @@
       <c r="AK24" s="16"/>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="19"/>
-      <c r="S25" s="19"/>
-      <c r="T25" s="19"/>
-      <c r="U25" s="19"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
+      <c r="S25" s="18"/>
+      <c r="T25" s="18"/>
+      <c r="U25" s="18"/>
       <c r="AE25" s="16"/>
       <c r="AF25" s="16"/>
       <c r="AG25" s="16"/>
@@ -2074,26 +2417,26 @@
       <c r="AK25" s="16"/>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="20"/>
-      <c r="R26" s="20"/>
-      <c r="S26" s="20"/>
-      <c r="T26" s="20"/>
-      <c r="U26" s="20"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
       <c r="AE26" s="16"/>
       <c r="AF26" s="16"/>
       <c r="AG26" s="16"/>
@@ -2178,16 +2521,16 @@
       <c r="B28" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="26"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="25"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
@@ -2202,6 +2545,9 @@
       <c r="W28" s="15"/>
       <c r="X28" s="15"/>
       <c r="Y28" s="15"/>
+      <c r="AB28" s="27" t="s">
+        <v>88</v>
+      </c>
       <c r="AE28" s="16"/>
       <c r="AF28" s="16"/>
       <c r="AG28" s="16"/>
@@ -2271,6 +2617,9 @@
       <c r="W29" s="15"/>
       <c r="X29" s="15"/>
       <c r="Y29" s="15"/>
+      <c r="AB29" s="27" t="s">
+        <v>89</v>
+      </c>
       <c r="AE29" s="16"/>
       <c r="AF29" s="16"/>
       <c r="AG29" s="16"/>
@@ -2316,6 +2665,9 @@
       <c r="W30" s="15"/>
       <c r="X30" s="15"/>
       <c r="Y30" s="15"/>
+      <c r="AB30" s="27" t="s">
+        <v>90</v>
+      </c>
       <c r="AE30" s="16"/>
       <c r="AF30" s="16"/>
       <c r="AG30" s="16"/>
@@ -2388,6 +2740,9 @@
       <c r="W31" s="15"/>
       <c r="X31" s="15"/>
       <c r="Y31" s="15"/>
+      <c r="AB31" s="27" t="s">
+        <v>91</v>
+      </c>
       <c r="AE31" s="16"/>
       <c r="AF31" s="16"/>
       <c r="AG31" s="16"/>
@@ -2424,7 +2779,9 @@
       <c r="Y32" s="10"/>
       <c r="Z32" s="10"/>
       <c r="AA32" s="10"/>
-      <c r="AB32" s="10"/>
+      <c r="AB32" s="27" t="s">
+        <v>92</v>
+      </c>
       <c r="AD32" s="16"/>
       <c r="AE32" s="16"/>
       <c r="AF32" s="16"/>
@@ -2435,28 +2792,31 @@
       <c r="AK32" s="16"/>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
-      <c r="O33" s="19"/>
-      <c r="P33" s="19"/>
-      <c r="Q33" s="19"/>
-      <c r="R33" s="19"/>
-      <c r="S33" s="19"/>
-      <c r="T33" s="19"/>
-      <c r="U33" s="19"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="18"/>
+      <c r="T33" s="18"/>
+      <c r="U33" s="18"/>
+      <c r="AB33" s="27" t="s">
+        <v>93</v>
+      </c>
       <c r="AF33" s="16"/>
       <c r="AG33" s="16"/>
       <c r="AH33" s="16"/>
@@ -2465,26 +2825,29 @@
       <c r="AK33" s="16"/>
     </row>
     <row r="34" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="20"/>
-      <c r="O34" s="20"/>
-      <c r="P34" s="20"/>
-      <c r="Q34" s="20"/>
-      <c r="R34" s="20"/>
-      <c r="S34" s="20"/>
-      <c r="T34" s="20"/>
-      <c r="U34" s="20"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+      <c r="AB34" s="27" t="s">
+        <v>94</v>
+      </c>
       <c r="AF34" s="16"/>
       <c r="AG34" s="16"/>
       <c r="AH34" s="16"/>
@@ -2559,6 +2922,9 @@
       <c r="W35" s="15"/>
       <c r="X35" s="15"/>
       <c r="Y35" s="15"/>
+      <c r="AB35" s="27" t="s">
+        <v>95</v>
+      </c>
       <c r="AF35" s="16"/>
       <c r="AG35" s="16"/>
       <c r="AH35" s="16"/>
@@ -2635,6 +3001,9 @@
       </c>
       <c r="X36" s="15"/>
       <c r="Y36" s="15"/>
+      <c r="AB36" s="27" t="s">
+        <v>96</v>
+      </c>
       <c r="AF36" s="16"/>
       <c r="AG36" s="16"/>
       <c r="AH36" s="16"/>
@@ -2701,6 +3070,9 @@
       <c r="W37" s="15"/>
       <c r="X37" s="15"/>
       <c r="Y37" s="15"/>
+      <c r="AB37" s="27" t="s">
+        <v>97</v>
+      </c>
       <c r="AF37" s="16"/>
       <c r="AG37" s="16"/>
       <c r="AH37" s="16"/>
@@ -2757,6 +3129,9 @@
       <c r="W38" s="15"/>
       <c r="X38" s="15"/>
       <c r="Y38" s="15"/>
+      <c r="AB38" s="27" t="s">
+        <v>98</v>
+      </c>
       <c r="AF38" s="16"/>
       <c r="AG38" s="16"/>
       <c r="AH38" s="16"/>
@@ -2828,6 +3203,9 @@
       <c r="W39" s="15"/>
       <c r="X39" s="15"/>
       <c r="Y39" s="15"/>
+      <c r="AB39" s="27" t="s">
+        <v>99</v>
+      </c>
       <c r="AF39" s="16"/>
       <c r="AG39" s="16"/>
       <c r="AH39" s="16"/>
@@ -2836,6 +3214,9 @@
       <c r="AK39" s="16"/>
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AB40" s="27" t="s">
+        <v>100</v>
+      </c>
       <c r="AD40" s="16"/>
       <c r="AE40" s="16"/>
       <c r="AF40" s="16"/>
@@ -2846,30 +3227,32 @@
       <c r="AK40" s="16"/>
     </row>
     <row r="41" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-      <c r="M41" s="19"/>
-      <c r="N41" s="19"/>
-      <c r="O41" s="19"/>
-      <c r="P41" s="19"/>
-      <c r="Q41" s="19"/>
-      <c r="R41" s="19"/>
-      <c r="S41" s="19"/>
-      <c r="T41" s="19"/>
-      <c r="U41" s="19"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="18"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="18"/>
+      <c r="S41" s="18"/>
+      <c r="T41" s="18"/>
+      <c r="U41" s="18"/>
       <c r="AA41" s="10"/>
-      <c r="AB41" s="10"/>
+      <c r="AB41" s="27" t="s">
+        <v>101</v>
+      </c>
       <c r="AC41" s="10"/>
       <c r="AD41" s="16"/>
       <c r="AE41" s="16"/>
@@ -2881,26 +3264,26 @@
       <c r="AK41" s="16"/>
     </row>
     <row r="42" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="20"/>
-      <c r="N42" s="20"/>
-      <c r="O42" s="20"/>
-      <c r="P42" s="20"/>
-      <c r="Q42" s="20"/>
-      <c r="R42" s="20"/>
-      <c r="S42" s="20"/>
-      <c r="T42" s="20"/>
-      <c r="U42" s="20"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="19"/>
+      <c r="O42" s="19"/>
+      <c r="P42" s="19"/>
+      <c r="Q42" s="19"/>
+      <c r="R42" s="19"/>
+      <c r="S42" s="19"/>
+      <c r="T42" s="19"/>
+      <c r="U42" s="19"/>
       <c r="AA42" s="10"/>
       <c r="AB42" s="10"/>
       <c r="AC42" s="10"/>
@@ -3491,26 +3874,26 @@
     </row>
     <row r="73" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A73" s="10"/>
-      <c r="B73" s="18"/>
-      <c r="C73" s="18"/>
-      <c r="D73" s="18"/>
-      <c r="E73" s="18"/>
-      <c r="F73" s="18"/>
-      <c r="G73" s="18"/>
-      <c r="H73" s="18"/>
-      <c r="I73" s="18"/>
-      <c r="J73" s="18"/>
-      <c r="K73" s="18"/>
-      <c r="L73" s="18"/>
-      <c r="M73" s="18"/>
-      <c r="N73" s="18"/>
-      <c r="O73" s="18"/>
-      <c r="P73" s="18"/>
-      <c r="Q73" s="18"/>
-      <c r="R73" s="18"/>
-      <c r="S73" s="18"/>
-      <c r="T73" s="18"/>
-      <c r="U73" s="18"/>
+      <c r="B73" s="26"/>
+      <c r="C73" s="26"/>
+      <c r="D73" s="26"/>
+      <c r="E73" s="26"/>
+      <c r="F73" s="26"/>
+      <c r="G73" s="26"/>
+      <c r="H73" s="26"/>
+      <c r="I73" s="26"/>
+      <c r="J73" s="26"/>
+      <c r="K73" s="26"/>
+      <c r="L73" s="26"/>
+      <c r="M73" s="26"/>
+      <c r="N73" s="26"/>
+      <c r="O73" s="26"/>
+      <c r="P73" s="26"/>
+      <c r="Q73" s="26"/>
+      <c r="R73" s="26"/>
+      <c r="S73" s="26"/>
+      <c r="T73" s="26"/>
+      <c r="U73" s="26"/>
       <c r="V73" s="10"/>
       <c r="W73" s="10"/>
       <c r="X73" s="10"/>
@@ -3519,26 +3902,26 @@
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A74" s="10"/>
-      <c r="B74" s="18"/>
-      <c r="C74" s="18"/>
-      <c r="D74" s="18"/>
-      <c r="E74" s="18"/>
-      <c r="F74" s="18"/>
-      <c r="G74" s="18"/>
-      <c r="H74" s="18"/>
-      <c r="I74" s="18"/>
-      <c r="J74" s="18"/>
-      <c r="K74" s="18"/>
-      <c r="L74" s="18"/>
-      <c r="M74" s="18"/>
-      <c r="N74" s="18"/>
-      <c r="O74" s="18"/>
-      <c r="P74" s="18"/>
-      <c r="Q74" s="18"/>
-      <c r="R74" s="18"/>
-      <c r="S74" s="18"/>
-      <c r="T74" s="18"/>
-      <c r="U74" s="18"/>
+      <c r="B74" s="26"/>
+      <c r="C74" s="26"/>
+      <c r="D74" s="26"/>
+      <c r="E74" s="26"/>
+      <c r="F74" s="26"/>
+      <c r="G74" s="26"/>
+      <c r="H74" s="26"/>
+      <c r="I74" s="26"/>
+      <c r="J74" s="26"/>
+      <c r="K74" s="26"/>
+      <c r="L74" s="26"/>
+      <c r="M74" s="26"/>
+      <c r="N74" s="26"/>
+      <c r="O74" s="26"/>
+      <c r="P74" s="26"/>
+      <c r="Q74" s="26"/>
+      <c r="R74" s="26"/>
+      <c r="S74" s="26"/>
+      <c r="T74" s="26"/>
+      <c r="U74" s="26"/>
       <c r="V74" s="10"/>
       <c r="W74" s="10"/>
       <c r="X74" s="10"/>
@@ -3743,26 +4126,26 @@
     </row>
     <row r="89" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A89" s="10"/>
-      <c r="B89" s="18"/>
-      <c r="C89" s="18"/>
-      <c r="D89" s="18"/>
-      <c r="E89" s="18"/>
-      <c r="F89" s="18"/>
-      <c r="G89" s="18"/>
-      <c r="H89" s="18"/>
-      <c r="I89" s="18"/>
-      <c r="J89" s="18"/>
-      <c r="K89" s="18"/>
-      <c r="L89" s="18"/>
-      <c r="M89" s="18"/>
-      <c r="N89" s="18"/>
-      <c r="O89" s="18"/>
-      <c r="P89" s="18"/>
-      <c r="Q89" s="18"/>
-      <c r="R89" s="18"/>
-      <c r="S89" s="18"/>
-      <c r="T89" s="18"/>
-      <c r="U89" s="18"/>
+      <c r="B89" s="26"/>
+      <c r="C89" s="26"/>
+      <c r="D89" s="26"/>
+      <c r="E89" s="26"/>
+      <c r="F89" s="26"/>
+      <c r="G89" s="26"/>
+      <c r="H89" s="26"/>
+      <c r="I89" s="26"/>
+      <c r="J89" s="26"/>
+      <c r="K89" s="26"/>
+      <c r="L89" s="26"/>
+      <c r="M89" s="26"/>
+      <c r="N89" s="26"/>
+      <c r="O89" s="26"/>
+      <c r="P89" s="26"/>
+      <c r="Q89" s="26"/>
+      <c r="R89" s="26"/>
+      <c r="S89" s="26"/>
+      <c r="T89" s="26"/>
+      <c r="U89" s="26"/>
       <c r="V89" s="10"/>
       <c r="W89" s="10"/>
       <c r="X89" s="10"/>
@@ -3773,26 +4156,26 @@
     </row>
     <row r="90" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A90" s="10"/>
-      <c r="B90" s="18"/>
-      <c r="C90" s="18"/>
-      <c r="D90" s="18"/>
-      <c r="E90" s="18"/>
-      <c r="F90" s="18"/>
-      <c r="G90" s="18"/>
-      <c r="H90" s="18"/>
-      <c r="I90" s="18"/>
-      <c r="J90" s="18"/>
-      <c r="K90" s="18"/>
-      <c r="L90" s="18"/>
-      <c r="M90" s="18"/>
-      <c r="N90" s="18"/>
-      <c r="O90" s="18"/>
-      <c r="P90" s="18"/>
-      <c r="Q90" s="18"/>
-      <c r="R90" s="18"/>
-      <c r="S90" s="18"/>
-      <c r="T90" s="18"/>
-      <c r="U90" s="18"/>
+      <c r="B90" s="26"/>
+      <c r="C90" s="26"/>
+      <c r="D90" s="26"/>
+      <c r="E90" s="26"/>
+      <c r="F90" s="26"/>
+      <c r="G90" s="26"/>
+      <c r="H90" s="26"/>
+      <c r="I90" s="26"/>
+      <c r="J90" s="26"/>
+      <c r="K90" s="26"/>
+      <c r="L90" s="26"/>
+      <c r="M90" s="26"/>
+      <c r="N90" s="26"/>
+      <c r="O90" s="26"/>
+      <c r="P90" s="26"/>
+      <c r="Q90" s="26"/>
+      <c r="R90" s="26"/>
+      <c r="S90" s="26"/>
+      <c r="T90" s="26"/>
+      <c r="U90" s="26"/>
       <c r="V90" s="10"/>
       <c r="W90" s="10"/>
       <c r="X90" s="10"/>
@@ -3983,26 +4366,26 @@
     </row>
     <row r="97" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A97" s="10"/>
-      <c r="B97" s="18"/>
-      <c r="C97" s="18"/>
-      <c r="D97" s="18"/>
-      <c r="E97" s="18"/>
-      <c r="F97" s="18"/>
-      <c r="G97" s="18"/>
-      <c r="H97" s="18"/>
-      <c r="I97" s="18"/>
-      <c r="J97" s="18"/>
-      <c r="K97" s="18"/>
-      <c r="L97" s="18"/>
-      <c r="M97" s="18"/>
-      <c r="N97" s="18"/>
-      <c r="O97" s="18"/>
-      <c r="P97" s="18"/>
-      <c r="Q97" s="18"/>
-      <c r="R97" s="18"/>
-      <c r="S97" s="18"/>
-      <c r="T97" s="18"/>
-      <c r="U97" s="18"/>
+      <c r="B97" s="26"/>
+      <c r="C97" s="26"/>
+      <c r="D97" s="26"/>
+      <c r="E97" s="26"/>
+      <c r="F97" s="26"/>
+      <c r="G97" s="26"/>
+      <c r="H97" s="26"/>
+      <c r="I97" s="26"/>
+      <c r="J97" s="26"/>
+      <c r="K97" s="26"/>
+      <c r="L97" s="26"/>
+      <c r="M97" s="26"/>
+      <c r="N97" s="26"/>
+      <c r="O97" s="26"/>
+      <c r="P97" s="26"/>
+      <c r="Q97" s="26"/>
+      <c r="R97" s="26"/>
+      <c r="S97" s="26"/>
+      <c r="T97" s="26"/>
+      <c r="U97" s="26"/>
       <c r="V97" s="10"/>
       <c r="W97" s="10"/>
       <c r="X97" s="10"/>
@@ -4013,26 +4396,26 @@
     </row>
     <row r="98" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A98" s="10"/>
-      <c r="B98" s="18"/>
-      <c r="C98" s="18"/>
-      <c r="D98" s="18"/>
-      <c r="E98" s="18"/>
-      <c r="F98" s="18"/>
-      <c r="G98" s="18"/>
-      <c r="H98" s="18"/>
-      <c r="I98" s="18"/>
-      <c r="J98" s="18"/>
-      <c r="K98" s="18"/>
-      <c r="L98" s="18"/>
-      <c r="M98" s="18"/>
-      <c r="N98" s="18"/>
-      <c r="O98" s="18"/>
-      <c r="P98" s="18"/>
-      <c r="Q98" s="18"/>
-      <c r="R98" s="18"/>
-      <c r="S98" s="18"/>
-      <c r="T98" s="18"/>
-      <c r="U98" s="18"/>
+      <c r="B98" s="26"/>
+      <c r="C98" s="26"/>
+      <c r="D98" s="26"/>
+      <c r="E98" s="26"/>
+      <c r="F98" s="26"/>
+      <c r="G98" s="26"/>
+      <c r="H98" s="26"/>
+      <c r="I98" s="26"/>
+      <c r="J98" s="26"/>
+      <c r="K98" s="26"/>
+      <c r="L98" s="26"/>
+      <c r="M98" s="26"/>
+      <c r="N98" s="26"/>
+      <c r="O98" s="26"/>
+      <c r="P98" s="26"/>
+      <c r="Q98" s="26"/>
+      <c r="R98" s="26"/>
+      <c r="S98" s="26"/>
+      <c r="T98" s="26"/>
+      <c r="U98" s="26"/>
       <c r="V98" s="10"/>
       <c r="W98" s="10"/>
       <c r="X98" s="10"/>
@@ -4223,26 +4606,26 @@
     </row>
     <row r="105" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A105" s="10"/>
-      <c r="B105" s="18"/>
-      <c r="C105" s="18"/>
-      <c r="D105" s="18"/>
-      <c r="E105" s="18"/>
-      <c r="F105" s="18"/>
-      <c r="G105" s="18"/>
-      <c r="H105" s="18"/>
-      <c r="I105" s="18"/>
-      <c r="J105" s="18"/>
-      <c r="K105" s="18"/>
-      <c r="L105" s="18"/>
-      <c r="M105" s="18"/>
-      <c r="N105" s="18"/>
-      <c r="O105" s="18"/>
-      <c r="P105" s="18"/>
-      <c r="Q105" s="18"/>
-      <c r="R105" s="18"/>
-      <c r="S105" s="18"/>
-      <c r="T105" s="18"/>
-      <c r="U105" s="18"/>
+      <c r="B105" s="26"/>
+      <c r="C105" s="26"/>
+      <c r="D105" s="26"/>
+      <c r="E105" s="26"/>
+      <c r="F105" s="26"/>
+      <c r="G105" s="26"/>
+      <c r="H105" s="26"/>
+      <c r="I105" s="26"/>
+      <c r="J105" s="26"/>
+      <c r="K105" s="26"/>
+      <c r="L105" s="26"/>
+      <c r="M105" s="26"/>
+      <c r="N105" s="26"/>
+      <c r="O105" s="26"/>
+      <c r="P105" s="26"/>
+      <c r="Q105" s="26"/>
+      <c r="R105" s="26"/>
+      <c r="S105" s="26"/>
+      <c r="T105" s="26"/>
+      <c r="U105" s="26"/>
       <c r="V105" s="10"/>
       <c r="W105" s="10"/>
       <c r="X105" s="10"/>
@@ -4253,26 +4636,26 @@
     </row>
     <row r="106" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A106" s="10"/>
-      <c r="B106" s="18"/>
-      <c r="C106" s="18"/>
-      <c r="D106" s="18"/>
-      <c r="E106" s="18"/>
-      <c r="F106" s="18"/>
-      <c r="G106" s="18"/>
-      <c r="H106" s="18"/>
-      <c r="I106" s="18"/>
-      <c r="J106" s="18"/>
-      <c r="K106" s="18"/>
-      <c r="L106" s="18"/>
-      <c r="M106" s="18"/>
-      <c r="N106" s="18"/>
-      <c r="O106" s="18"/>
-      <c r="P106" s="18"/>
-      <c r="Q106" s="18"/>
-      <c r="R106" s="18"/>
-      <c r="S106" s="18"/>
-      <c r="T106" s="18"/>
-      <c r="U106" s="18"/>
+      <c r="B106" s="26"/>
+      <c r="C106" s="26"/>
+      <c r="D106" s="26"/>
+      <c r="E106" s="26"/>
+      <c r="F106" s="26"/>
+      <c r="G106" s="26"/>
+      <c r="H106" s="26"/>
+      <c r="I106" s="26"/>
+      <c r="J106" s="26"/>
+      <c r="K106" s="26"/>
+      <c r="L106" s="26"/>
+      <c r="M106" s="26"/>
+      <c r="N106" s="26"/>
+      <c r="O106" s="26"/>
+      <c r="P106" s="26"/>
+      <c r="Q106" s="26"/>
+      <c r="R106" s="26"/>
+      <c r="S106" s="26"/>
+      <c r="T106" s="26"/>
+      <c r="U106" s="26"/>
       <c r="V106" s="10"/>
       <c r="W106" s="10"/>
       <c r="X106" s="10"/>
@@ -4463,26 +4846,26 @@
     </row>
     <row r="113" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A113" s="10"/>
-      <c r="B113" s="18"/>
-      <c r="C113" s="18"/>
-      <c r="D113" s="18"/>
-      <c r="E113" s="18"/>
-      <c r="F113" s="18"/>
-      <c r="G113" s="18"/>
-      <c r="H113" s="18"/>
-      <c r="I113" s="18"/>
-      <c r="J113" s="18"/>
-      <c r="K113" s="18"/>
-      <c r="L113" s="18"/>
-      <c r="M113" s="18"/>
-      <c r="N113" s="18"/>
-      <c r="O113" s="18"/>
-      <c r="P113" s="18"/>
-      <c r="Q113" s="18"/>
-      <c r="R113" s="18"/>
-      <c r="S113" s="18"/>
-      <c r="T113" s="18"/>
-      <c r="U113" s="18"/>
+      <c r="B113" s="26"/>
+      <c r="C113" s="26"/>
+      <c r="D113" s="26"/>
+      <c r="E113" s="26"/>
+      <c r="F113" s="26"/>
+      <c r="G113" s="26"/>
+      <c r="H113" s="26"/>
+      <c r="I113" s="26"/>
+      <c r="J113" s="26"/>
+      <c r="K113" s="26"/>
+      <c r="L113" s="26"/>
+      <c r="M113" s="26"/>
+      <c r="N113" s="26"/>
+      <c r="O113" s="26"/>
+      <c r="P113" s="26"/>
+      <c r="Q113" s="26"/>
+      <c r="R113" s="26"/>
+      <c r="S113" s="26"/>
+      <c r="T113" s="26"/>
+      <c r="U113" s="26"/>
       <c r="V113" s="10"/>
       <c r="W113" s="10"/>
       <c r="X113" s="10"/>
@@ -4493,26 +4876,26 @@
     </row>
     <row r="114" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A114" s="10"/>
-      <c r="B114" s="18"/>
-      <c r="C114" s="18"/>
-      <c r="D114" s="18"/>
-      <c r="E114" s="18"/>
-      <c r="F114" s="18"/>
-      <c r="G114" s="18"/>
-      <c r="H114" s="18"/>
-      <c r="I114" s="18"/>
-      <c r="J114" s="18"/>
-      <c r="K114" s="18"/>
-      <c r="L114" s="18"/>
-      <c r="M114" s="18"/>
-      <c r="N114" s="18"/>
-      <c r="O114" s="18"/>
-      <c r="P114" s="18"/>
-      <c r="Q114" s="18"/>
-      <c r="R114" s="18"/>
-      <c r="S114" s="18"/>
-      <c r="T114" s="18"/>
-      <c r="U114" s="18"/>
+      <c r="B114" s="26"/>
+      <c r="C114" s="26"/>
+      <c r="D114" s="26"/>
+      <c r="E114" s="26"/>
+      <c r="F114" s="26"/>
+      <c r="G114" s="26"/>
+      <c r="H114" s="26"/>
+      <c r="I114" s="26"/>
+      <c r="J114" s="26"/>
+      <c r="K114" s="26"/>
+      <c r="L114" s="26"/>
+      <c r="M114" s="26"/>
+      <c r="N114" s="26"/>
+      <c r="O114" s="26"/>
+      <c r="P114" s="26"/>
+      <c r="Q114" s="26"/>
+      <c r="R114" s="26"/>
+      <c r="S114" s="26"/>
+      <c r="T114" s="26"/>
+      <c r="U114" s="26"/>
       <c r="V114" s="10"/>
       <c r="W114" s="10"/>
       <c r="X114" s="10"/>
@@ -4528,9 +4911,9 @@
       <c r="D115" s="10"/>
       <c r="E115" s="10"/>
       <c r="F115" s="10"/>
-      <c r="G115" s="18"/>
-      <c r="H115" s="18"/>
-      <c r="I115" s="18"/>
+      <c r="G115" s="26"/>
+      <c r="H115" s="26"/>
+      <c r="I115" s="26"/>
       <c r="J115" s="10"/>
       <c r="K115" s="10"/>
       <c r="L115" s="10"/>
@@ -4558,9 +4941,9 @@
       <c r="D116" s="10"/>
       <c r="E116" s="10"/>
       <c r="F116" s="10"/>
-      <c r="G116" s="18"/>
-      <c r="H116" s="18"/>
-      <c r="I116" s="18"/>
+      <c r="G116" s="26"/>
+      <c r="H116" s="26"/>
+      <c r="I116" s="26"/>
       <c r="J116" s="10"/>
       <c r="K116" s="10"/>
       <c r="L116" s="10"/>
@@ -4597,10 +4980,10 @@
       <c r="M117" s="10"/>
       <c r="N117" s="10"/>
       <c r="O117" s="10"/>
-      <c r="P117" s="18"/>
-      <c r="Q117" s="18"/>
-      <c r="R117" s="18"/>
-      <c r="S117" s="18"/>
+      <c r="P117" s="26"/>
+      <c r="Q117" s="26"/>
+      <c r="R117" s="26"/>
+      <c r="S117" s="26"/>
       <c r="T117" s="10"/>
       <c r="U117" s="10"/>
       <c r="V117" s="10"/>
@@ -4627,10 +5010,10 @@
       <c r="M118" s="10"/>
       <c r="N118" s="10"/>
       <c r="O118" s="10"/>
-      <c r="P118" s="18"/>
-      <c r="Q118" s="18"/>
-      <c r="R118" s="18"/>
-      <c r="S118" s="18"/>
+      <c r="P118" s="26"/>
+      <c r="Q118" s="26"/>
+      <c r="R118" s="26"/>
+      <c r="S118" s="26"/>
       <c r="T118" s="10"/>
       <c r="U118" s="10"/>
       <c r="V118" s="10"/>
@@ -4703,26 +5086,26 @@
     </row>
     <row r="121" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A121" s="10"/>
-      <c r="B121" s="18"/>
-      <c r="C121" s="18"/>
-      <c r="D121" s="18"/>
-      <c r="E121" s="18"/>
-      <c r="F121" s="18"/>
-      <c r="G121" s="18"/>
-      <c r="H121" s="18"/>
-      <c r="I121" s="18"/>
-      <c r="J121" s="18"/>
-      <c r="K121" s="18"/>
-      <c r="L121" s="18"/>
-      <c r="M121" s="18"/>
-      <c r="N121" s="18"/>
-      <c r="O121" s="18"/>
-      <c r="P121" s="18"/>
-      <c r="Q121" s="18"/>
-      <c r="R121" s="18"/>
-      <c r="S121" s="18"/>
-      <c r="T121" s="18"/>
-      <c r="U121" s="18"/>
+      <c r="B121" s="26"/>
+      <c r="C121" s="26"/>
+      <c r="D121" s="26"/>
+      <c r="E121" s="26"/>
+      <c r="F121" s="26"/>
+      <c r="G121" s="26"/>
+      <c r="H121" s="26"/>
+      <c r="I121" s="26"/>
+      <c r="J121" s="26"/>
+      <c r="K121" s="26"/>
+      <c r="L121" s="26"/>
+      <c r="M121" s="26"/>
+      <c r="N121" s="26"/>
+      <c r="O121" s="26"/>
+      <c r="P121" s="26"/>
+      <c r="Q121" s="26"/>
+      <c r="R121" s="26"/>
+      <c r="S121" s="26"/>
+      <c r="T121" s="26"/>
+      <c r="U121" s="26"/>
       <c r="V121" s="10"/>
       <c r="W121" s="10"/>
       <c r="X121" s="10"/>
@@ -4733,26 +5116,26 @@
     </row>
     <row r="122" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A122" s="10"/>
-      <c r="B122" s="18"/>
-      <c r="C122" s="18"/>
-      <c r="D122" s="18"/>
-      <c r="E122" s="18"/>
-      <c r="F122" s="18"/>
-      <c r="G122" s="18"/>
-      <c r="H122" s="18"/>
-      <c r="I122" s="18"/>
-      <c r="J122" s="18"/>
-      <c r="K122" s="18"/>
-      <c r="L122" s="18"/>
-      <c r="M122" s="18"/>
-      <c r="N122" s="18"/>
-      <c r="O122" s="18"/>
-      <c r="P122" s="18"/>
-      <c r="Q122" s="18"/>
-      <c r="R122" s="18"/>
-      <c r="S122" s="18"/>
-      <c r="T122" s="18"/>
-      <c r="U122" s="18"/>
+      <c r="B122" s="26"/>
+      <c r="C122" s="26"/>
+      <c r="D122" s="26"/>
+      <c r="E122" s="26"/>
+      <c r="F122" s="26"/>
+      <c r="G122" s="26"/>
+      <c r="H122" s="26"/>
+      <c r="I122" s="26"/>
+      <c r="J122" s="26"/>
+      <c r="K122" s="26"/>
+      <c r="L122" s="26"/>
+      <c r="M122" s="26"/>
+      <c r="N122" s="26"/>
+      <c r="O122" s="26"/>
+      <c r="P122" s="26"/>
+      <c r="Q122" s="26"/>
+      <c r="R122" s="26"/>
+      <c r="S122" s="26"/>
+      <c r="T122" s="26"/>
+      <c r="U122" s="26"/>
       <c r="V122" s="10"/>
       <c r="W122" s="10"/>
       <c r="X122" s="10"/>
@@ -4943,26 +5326,26 @@
     </row>
     <row r="129" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A129" s="10"/>
-      <c r="B129" s="18"/>
-      <c r="C129" s="18"/>
-      <c r="D129" s="18"/>
-      <c r="E129" s="18"/>
-      <c r="F129" s="18"/>
-      <c r="G129" s="18"/>
-      <c r="H129" s="18"/>
-      <c r="I129" s="18"/>
-      <c r="J129" s="18"/>
-      <c r="K129" s="18"/>
-      <c r="L129" s="18"/>
-      <c r="M129" s="18"/>
-      <c r="N129" s="18"/>
-      <c r="O129" s="18"/>
-      <c r="P129" s="18"/>
-      <c r="Q129" s="18"/>
-      <c r="R129" s="18"/>
-      <c r="S129" s="18"/>
-      <c r="T129" s="18"/>
-      <c r="U129" s="18"/>
+      <c r="B129" s="26"/>
+      <c r="C129" s="26"/>
+      <c r="D129" s="26"/>
+      <c r="E129" s="26"/>
+      <c r="F129" s="26"/>
+      <c r="G129" s="26"/>
+      <c r="H129" s="26"/>
+      <c r="I129" s="26"/>
+      <c r="J129" s="26"/>
+      <c r="K129" s="26"/>
+      <c r="L129" s="26"/>
+      <c r="M129" s="26"/>
+      <c r="N129" s="26"/>
+      <c r="O129" s="26"/>
+      <c r="P129" s="26"/>
+      <c r="Q129" s="26"/>
+      <c r="R129" s="26"/>
+      <c r="S129" s="26"/>
+      <c r="T129" s="26"/>
+      <c r="U129" s="26"/>
       <c r="V129" s="10"/>
       <c r="W129" s="10"/>
       <c r="X129" s="10"/>
@@ -4973,26 +5356,26 @@
     </row>
     <row r="130" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A130" s="10"/>
-      <c r="B130" s="18"/>
-      <c r="C130" s="18"/>
-      <c r="D130" s="18"/>
-      <c r="E130" s="18"/>
-      <c r="F130" s="18"/>
-      <c r="G130" s="18"/>
-      <c r="H130" s="18"/>
-      <c r="I130" s="18"/>
-      <c r="J130" s="18"/>
-      <c r="K130" s="18"/>
-      <c r="L130" s="18"/>
-      <c r="M130" s="18"/>
-      <c r="N130" s="18"/>
-      <c r="O130" s="18"/>
-      <c r="P130" s="18"/>
-      <c r="Q130" s="18"/>
-      <c r="R130" s="18"/>
-      <c r="S130" s="18"/>
-      <c r="T130" s="18"/>
-      <c r="U130" s="18"/>
+      <c r="B130" s="26"/>
+      <c r="C130" s="26"/>
+      <c r="D130" s="26"/>
+      <c r="E130" s="26"/>
+      <c r="F130" s="26"/>
+      <c r="G130" s="26"/>
+      <c r="H130" s="26"/>
+      <c r="I130" s="26"/>
+      <c r="J130" s="26"/>
+      <c r="K130" s="26"/>
+      <c r="L130" s="26"/>
+      <c r="M130" s="26"/>
+      <c r="N130" s="26"/>
+      <c r="O130" s="26"/>
+      <c r="P130" s="26"/>
+      <c r="Q130" s="26"/>
+      <c r="R130" s="26"/>
+      <c r="S130" s="26"/>
+      <c r="T130" s="26"/>
+      <c r="U130" s="26"/>
       <c r="V130" s="10"/>
       <c r="W130" s="10"/>
       <c r="X130" s="10"/>
@@ -5301,15 +5684,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B1:U2"/>
-    <mergeCell ref="B9:U10"/>
-    <mergeCell ref="B17:U18"/>
-    <mergeCell ref="B25:U26"/>
-    <mergeCell ref="B33:U34"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="C28:J28"/>
     <mergeCell ref="B73:U74"/>
     <mergeCell ref="B89:U90"/>
     <mergeCell ref="B97:U98"/>
@@ -5322,6 +5696,15 @@
     <mergeCell ref="P117:S117"/>
     <mergeCell ref="P118:S118"/>
     <mergeCell ref="B121:U122"/>
+    <mergeCell ref="B1:U2"/>
+    <mergeCell ref="B9:U10"/>
+    <mergeCell ref="B17:U18"/>
+    <mergeCell ref="B25:U26"/>
+    <mergeCell ref="B33:U34"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="C28:J28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed watchdog time out to 6s Changed i2c refresh interval to 30m I2C refresh now reset watchdog timer aswell Added ADC reading timeout counter and measure Added LCD debug screen
</commit_message>
<xml_diff>
--- a/LCD User Interface.xlsx
+++ b/LCD User Interface.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Stromvy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DD2289-3362-4755-993D-FE5F719D4676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AF8C3D-D767-422C-A317-9C92748A05BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="105">
   <si>
     <t>x</t>
   </si>
@@ -611,6 +611,15 @@
       </rPr>
       <t>0.0001</t>
     </r>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>SCREEN_DEBUG</t>
+  </si>
+  <si>
+    <t>%d</t>
   </si>
 </sst>
 </file>
@@ -781,7 +790,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -837,6 +846,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -858,11 +876,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1146,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45:H45"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1158,50 +1173,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
@@ -1251,11 +1266,11 @@
         <v>65</v>
       </c>
       <c r="Q3" s="1"/>
-      <c r="R3" s="20" t="s">
+      <c r="R3" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="S3" s="22"/>
-      <c r="T3" s="21"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="24"/>
       <c r="U3" s="1"/>
       <c r="W3" s="15"/>
       <c r="X3" s="15"/>
@@ -1316,10 +1331,10 @@
         <v>2</v>
       </c>
       <c r="Q4" s="1"/>
-      <c r="R4" s="20" t="s">
+      <c r="R4" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="S4" s="21"/>
+      <c r="S4" s="24"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="W4" s="15"/>
@@ -1448,11 +1463,11 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="20" t="s">
+      <c r="R6" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="S6" s="22"/>
-      <c r="T6" s="21"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="24"/>
       <c r="U6" s="12"/>
       <c r="W6" s="15"/>
       <c r="X6" s="15"/>
@@ -1544,28 +1559,28 @@
       <c r="AD8" s="15"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="21"/>
+      <c r="U9" s="21"/>
       <c r="W9" s="15"/>
       <c r="X9" s="15"/>
       <c r="Y9" s="15"/>
@@ -1576,26 +1591,26 @@
       <c r="AD9" s="15"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22"/>
+      <c r="U10" s="22"/>
       <c r="W10" s="15"/>
       <c r="X10" s="15"/>
       <c r="Y10" s="15"/>
@@ -1846,10 +1861,18 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
+      <c r="R14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="W14" s="15"/>
       <c r="X14" s="15"/>
       <c r="Y14" s="15"/>
@@ -1969,28 +1992,28 @@
       <c r="AK16" s="16"/>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="18"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="21"/>
+      <c r="U17" s="21"/>
       <c r="W17" s="15"/>
       <c r="X17" s="15"/>
       <c r="Y17" s="15"/>
@@ -2008,26 +2031,26 @@
       <c r="AK17" s="16"/>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="19"/>
-      <c r="S18" s="19"/>
-      <c r="T18" s="19"/>
-      <c r="U18" s="19"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22"/>
+      <c r="U18" s="22"/>
       <c r="W18" s="15"/>
       <c r="X18" s="15"/>
       <c r="Y18" s="15"/>
@@ -2386,28 +2409,28 @@
       <c r="AK24" s="16"/>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="18"/>
-      <c r="P25" s="18"/>
-      <c r="Q25" s="18"/>
-      <c r="R25" s="18"/>
-      <c r="S25" s="18"/>
-      <c r="T25" s="18"/>
-      <c r="U25" s="18"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="21"/>
+      <c r="U25" s="21"/>
       <c r="AE25" s="16"/>
       <c r="AF25" s="16"/>
       <c r="AG25" s="16"/>
@@ -2417,26 +2440,26 @@
       <c r="AK25" s="16"/>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19"/>
-      <c r="O26" s="19"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="19"/>
-      <c r="S26" s="19"/>
-      <c r="T26" s="19"/>
-      <c r="U26" s="19"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="22"/>
+      <c r="U26" s="22"/>
       <c r="AE26" s="16"/>
       <c r="AF26" s="16"/>
       <c r="AG26" s="16"/>
@@ -2521,16 +2544,16 @@
       <c r="B28" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="25"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="28"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
@@ -2545,7 +2568,7 @@
       <c r="W28" s="15"/>
       <c r="X28" s="15"/>
       <c r="Y28" s="15"/>
-      <c r="AB28" s="27" t="s">
+      <c r="AB28" s="19" t="s">
         <v>88</v>
       </c>
       <c r="AE28" s="16"/>
@@ -2617,7 +2640,7 @@
       <c r="W29" s="15"/>
       <c r="X29" s="15"/>
       <c r="Y29" s="15"/>
-      <c r="AB29" s="27" t="s">
+      <c r="AB29" s="19" t="s">
         <v>89</v>
       </c>
       <c r="AE29" s="16"/>
@@ -2665,7 +2688,7 @@
       <c r="W30" s="15"/>
       <c r="X30" s="15"/>
       <c r="Y30" s="15"/>
-      <c r="AB30" s="27" t="s">
+      <c r="AB30" s="19" t="s">
         <v>90</v>
       </c>
       <c r="AE30" s="16"/>
@@ -2740,7 +2763,7 @@
       <c r="W31" s="15"/>
       <c r="X31" s="15"/>
       <c r="Y31" s="15"/>
-      <c r="AB31" s="27" t="s">
+      <c r="AB31" s="19" t="s">
         <v>91</v>
       </c>
       <c r="AE31" s="16"/>
@@ -2779,7 +2802,7 @@
       <c r="Y32" s="10"/>
       <c r="Z32" s="10"/>
       <c r="AA32" s="10"/>
-      <c r="AB32" s="27" t="s">
+      <c r="AB32" s="19" t="s">
         <v>92</v>
       </c>
       <c r="AD32" s="16"/>
@@ -2792,29 +2815,29 @@
       <c r="AK32" s="16"/>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18"/>
-      <c r="O33" s="18"/>
-      <c r="P33" s="18"/>
-      <c r="Q33" s="18"/>
-      <c r="R33" s="18"/>
-      <c r="S33" s="18"/>
-      <c r="T33" s="18"/>
-      <c r="U33" s="18"/>
-      <c r="AB33" s="27" t="s">
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="21"/>
+      <c r="O33" s="21"/>
+      <c r="P33" s="21"/>
+      <c r="Q33" s="21"/>
+      <c r="R33" s="21"/>
+      <c r="S33" s="21"/>
+      <c r="T33" s="21"/>
+      <c r="U33" s="21"/>
+      <c r="AB33" s="19" t="s">
         <v>93</v>
       </c>
       <c r="AF33" s="16"/>
@@ -2825,27 +2848,27 @@
       <c r="AK33" s="16"/>
     </row>
     <row r="34" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
-      <c r="O34" s="19"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="19"/>
-      <c r="R34" s="19"/>
-      <c r="S34" s="19"/>
-      <c r="T34" s="19"/>
-      <c r="U34" s="19"/>
-      <c r="AB34" s="27" t="s">
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="22"/>
+      <c r="N34" s="22"/>
+      <c r="O34" s="22"/>
+      <c r="P34" s="22"/>
+      <c r="Q34" s="22"/>
+      <c r="R34" s="22"/>
+      <c r="S34" s="22"/>
+      <c r="T34" s="22"/>
+      <c r="U34" s="22"/>
+      <c r="AB34" s="19" t="s">
         <v>94</v>
       </c>
       <c r="AF34" s="16"/>
@@ -2922,7 +2945,7 @@
       <c r="W35" s="15"/>
       <c r="X35" s="15"/>
       <c r="Y35" s="15"/>
-      <c r="AB35" s="27" t="s">
+      <c r="AB35" s="19" t="s">
         <v>95</v>
       </c>
       <c r="AF35" s="16"/>
@@ -3001,7 +3024,7 @@
       </c>
       <c r="X36" s="15"/>
       <c r="Y36" s="15"/>
-      <c r="AB36" s="27" t="s">
+      <c r="AB36" s="19" t="s">
         <v>96</v>
       </c>
       <c r="AF36" s="16"/>
@@ -3070,7 +3093,7 @@
       <c r="W37" s="15"/>
       <c r="X37" s="15"/>
       <c r="Y37" s="15"/>
-      <c r="AB37" s="27" t="s">
+      <c r="AB37" s="19" t="s">
         <v>97</v>
       </c>
       <c r="AF37" s="16"/>
@@ -3129,7 +3152,7 @@
       <c r="W38" s="15"/>
       <c r="X38" s="15"/>
       <c r="Y38" s="15"/>
-      <c r="AB38" s="27" t="s">
+      <c r="AB38" s="19" t="s">
         <v>98</v>
       </c>
       <c r="AF38" s="16"/>
@@ -3203,7 +3226,7 @@
       <c r="W39" s="15"/>
       <c r="X39" s="15"/>
       <c r="Y39" s="15"/>
-      <c r="AB39" s="27" t="s">
+      <c r="AB39" s="19" t="s">
         <v>99</v>
       </c>
       <c r="AF39" s="16"/>
@@ -3214,7 +3237,7 @@
       <c r="AK39" s="16"/>
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="AB40" s="27" t="s">
+      <c r="AB40" s="19" t="s">
         <v>100</v>
       </c>
       <c r="AD40" s="16"/>
@@ -3227,30 +3250,30 @@
       <c r="AK40" s="16"/>
     </row>
     <row r="41" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-      <c r="N41" s="18"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="18"/>
-      <c r="Q41" s="18"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="18"/>
-      <c r="T41" s="18"/>
-      <c r="U41" s="18"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="21"/>
+      <c r="P41" s="21"/>
+      <c r="Q41" s="21"/>
+      <c r="R41" s="21"/>
+      <c r="S41" s="21"/>
+      <c r="T41" s="21"/>
+      <c r="U41" s="21"/>
       <c r="AA41" s="10"/>
-      <c r="AB41" s="27" t="s">
+      <c r="AB41" s="19" t="s">
         <v>101</v>
       </c>
       <c r="AC41" s="10"/>
@@ -3264,26 +3287,26 @@
       <c r="AK41" s="16"/>
     </row>
     <row r="42" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="19"/>
-      <c r="M42" s="19"/>
-      <c r="N42" s="19"/>
-      <c r="O42" s="19"/>
-      <c r="P42" s="19"/>
-      <c r="Q42" s="19"/>
-      <c r="R42" s="19"/>
-      <c r="S42" s="19"/>
-      <c r="T42" s="19"/>
-      <c r="U42" s="19"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="22"/>
+      <c r="L42" s="22"/>
+      <c r="M42" s="22"/>
+      <c r="N42" s="22"/>
+      <c r="O42" s="22"/>
+      <c r="P42" s="22"/>
+      <c r="Q42" s="22"/>
+      <c r="R42" s="22"/>
+      <c r="S42" s="22"/>
+      <c r="T42" s="22"/>
+      <c r="U42" s="22"/>
       <c r="AA42" s="10"/>
       <c r="AB42" s="10"/>
       <c r="AC42" s="10"/>
@@ -3656,7 +3679,29 @@
       <c r="AJ48" s="16"/>
       <c r="AK48" s="16"/>
     </row>
-    <row r="49" spans="30:37" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B49" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
+      <c r="K49" s="21"/>
+      <c r="L49" s="21"/>
+      <c r="M49" s="21"/>
+      <c r="N49" s="21"/>
+      <c r="O49" s="21"/>
+      <c r="P49" s="21"/>
+      <c r="Q49" s="21"/>
+      <c r="R49" s="21"/>
+      <c r="S49" s="21"/>
+      <c r="T49" s="21"/>
+      <c r="U49" s="21"/>
       <c r="AD49" s="16"/>
       <c r="AE49" s="16"/>
       <c r="AF49" s="16"/>
@@ -3666,7 +3711,27 @@
       <c r="AJ49" s="16"/>
       <c r="AK49" s="16"/>
     </row>
-    <row r="50" spans="30:37" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="22"/>
+      <c r="L50" s="22"/>
+      <c r="M50" s="22"/>
+      <c r="N50" s="22"/>
+      <c r="O50" s="22"/>
+      <c r="P50" s="22"/>
+      <c r="Q50" s="22"/>
+      <c r="R50" s="22"/>
+      <c r="S50" s="22"/>
+      <c r="T50" s="22"/>
+      <c r="U50" s="22"/>
       <c r="AD50" s="16"/>
       <c r="AE50" s="16"/>
       <c r="AF50" s="16"/>
@@ -3676,7 +3741,54 @@
       <c r="AJ50" s="16"/>
       <c r="AK50" s="16"/>
     </row>
-    <row r="51" spans="30:37" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A51" s="18">
+        <v>0</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K51" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="L51" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M51" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="N51" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="O51" s="12"/>
+      <c r="P51" s="12"/>
+      <c r="Q51" s="29"/>
+      <c r="R51" s="7"/>
+      <c r="S51" s="2"/>
+      <c r="T51" s="2"/>
+      <c r="U51" s="2"/>
       <c r="AD51" s="16"/>
       <c r="AE51" s="16"/>
       <c r="AF51" s="16"/>
@@ -3686,7 +3798,56 @@
       <c r="AJ51" s="16"/>
       <c r="AK51" s="16"/>
     </row>
-    <row r="52" spans="30:37" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A52" s="18">
+        <v>1</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L52" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M52" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N52" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O52" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="P52" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="2"/>
+      <c r="S52" s="7"/>
+      <c r="T52" s="7"/>
+      <c r="U52" s="7"/>
       <c r="AD52" s="16"/>
       <c r="AE52" s="16"/>
       <c r="AF52" s="16"/>
@@ -3696,7 +3857,30 @@
       <c r="AJ52" s="16"/>
       <c r="AK52" s="16"/>
     </row>
-    <row r="53" spans="30:37" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A53" s="18">
+        <v>2</v>
+      </c>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="12"/>
+      <c r="L53" s="12"/>
+      <c r="M53" s="12"/>
+      <c r="N53" s="12"/>
+      <c r="O53" s="12"/>
+      <c r="P53" s="2"/>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="2"/>
+      <c r="S53" s="2"/>
+      <c r="T53" s="2"/>
+      <c r="U53" s="2"/>
       <c r="AD53" s="16"/>
       <c r="AE53" s="16"/>
       <c r="AF53" s="16"/>
@@ -3706,7 +3890,40 @@
       <c r="AJ53" s="16"/>
       <c r="AK53" s="16"/>
     </row>
-    <row r="54" spans="30:37" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A54" s="18">
+        <v>3</v>
+      </c>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="12"/>
+      <c r="P54" s="12"/>
+      <c r="Q54" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="R54" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S54" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T54" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U54" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="AD54" s="16"/>
       <c r="AE54" s="16"/>
       <c r="AF54" s="16"/>
@@ -3716,7 +3933,68 @@
       <c r="AJ54" s="16"/>
       <c r="AK54" s="16"/>
     </row>
-    <row r="55" spans="30:37" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A55" s="18"/>
+      <c r="B55" s="18">
+        <v>0</v>
+      </c>
+      <c r="C55" s="18">
+        <v>1</v>
+      </c>
+      <c r="D55" s="18">
+        <v>2</v>
+      </c>
+      <c r="E55" s="18">
+        <v>3</v>
+      </c>
+      <c r="F55" s="18">
+        <v>4</v>
+      </c>
+      <c r="G55" s="18">
+        <v>5</v>
+      </c>
+      <c r="H55" s="18">
+        <v>6</v>
+      </c>
+      <c r="I55" s="18">
+        <v>7</v>
+      </c>
+      <c r="J55" s="18">
+        <v>8</v>
+      </c>
+      <c r="K55" s="18">
+        <v>9</v>
+      </c>
+      <c r="L55" s="18">
+        <v>10</v>
+      </c>
+      <c r="M55" s="18">
+        <v>11</v>
+      </c>
+      <c r="N55" s="18">
+        <v>12</v>
+      </c>
+      <c r="O55" s="18">
+        <v>13</v>
+      </c>
+      <c r="P55" s="18">
+        <v>14</v>
+      </c>
+      <c r="Q55" s="18">
+        <v>15</v>
+      </c>
+      <c r="R55" s="18">
+        <v>16</v>
+      </c>
+      <c r="S55" s="18">
+        <v>17</v>
+      </c>
+      <c r="T55" s="18">
+        <v>18</v>
+      </c>
+      <c r="U55" s="18">
+        <v>19</v>
+      </c>
       <c r="AD55" s="16"/>
       <c r="AE55" s="16"/>
       <c r="AF55" s="16"/>
@@ -3726,7 +4004,7 @@
       <c r="AJ55" s="16"/>
       <c r="AK55" s="16"/>
     </row>
-    <row r="56" spans="30:37" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AD56" s="16"/>
       <c r="AE56" s="16"/>
       <c r="AF56" s="16"/>
@@ -3736,7 +4014,7 @@
       <c r="AJ56" s="16"/>
       <c r="AK56" s="16"/>
     </row>
-    <row r="57" spans="30:37" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AD57" s="16"/>
       <c r="AE57" s="16"/>
       <c r="AF57" s="16"/>
@@ -3746,7 +4024,7 @@
       <c r="AJ57" s="16"/>
       <c r="AK57" s="16"/>
     </row>
-    <row r="58" spans="30:37" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AD58" s="16"/>
       <c r="AE58" s="16"/>
       <c r="AF58" s="16"/>
@@ -3756,7 +4034,7 @@
       <c r="AJ58" s="16"/>
       <c r="AK58" s="16"/>
     </row>
-    <row r="59" spans="30:37" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AD59" s="16"/>
       <c r="AE59" s="16"/>
       <c r="AF59" s="16"/>
@@ -3766,7 +4044,7 @@
       <c r="AJ59" s="16"/>
       <c r="AK59" s="16"/>
     </row>
-    <row r="60" spans="30:37" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AD60" s="16"/>
       <c r="AE60" s="16"/>
       <c r="AF60" s="16"/>
@@ -3776,7 +4054,7 @@
       <c r="AJ60" s="16"/>
       <c r="AK60" s="16"/>
     </row>
-    <row r="61" spans="30:37" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AD61" s="16"/>
       <c r="AE61" s="16"/>
       <c r="AF61" s="16"/>
@@ -3786,7 +4064,7 @@
       <c r="AJ61" s="16"/>
       <c r="AK61" s="16"/>
     </row>
-    <row r="62" spans="30:37" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AD62" s="16"/>
       <c r="AE62" s="16"/>
       <c r="AF62" s="16"/>
@@ -3796,7 +4074,7 @@
       <c r="AJ62" s="16"/>
       <c r="AK62" s="16"/>
     </row>
-    <row r="63" spans="30:37" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AD63" s="16"/>
       <c r="AE63" s="16"/>
       <c r="AF63" s="16"/>
@@ -3806,7 +4084,7 @@
       <c r="AJ63" s="16"/>
       <c r="AK63" s="16"/>
     </row>
-    <row r="64" spans="30:37" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AD64" s="15"/>
       <c r="AE64" s="15"/>
       <c r="AF64" s="15"/>
@@ -3874,26 +4152,26 @@
     </row>
     <row r="73" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A73" s="10"/>
-      <c r="B73" s="26"/>
-      <c r="C73" s="26"/>
-      <c r="D73" s="26"/>
-      <c r="E73" s="26"/>
-      <c r="F73" s="26"/>
-      <c r="G73" s="26"/>
-      <c r="H73" s="26"/>
-      <c r="I73" s="26"/>
-      <c r="J73" s="26"/>
-      <c r="K73" s="26"/>
-      <c r="L73" s="26"/>
-      <c r="M73" s="26"/>
-      <c r="N73" s="26"/>
-      <c r="O73" s="26"/>
-      <c r="P73" s="26"/>
-      <c r="Q73" s="26"/>
-      <c r="R73" s="26"/>
-      <c r="S73" s="26"/>
-      <c r="T73" s="26"/>
-      <c r="U73" s="26"/>
+      <c r="B73" s="20"/>
+      <c r="C73" s="20"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="20"/>
+      <c r="F73" s="20"/>
+      <c r="G73" s="20"/>
+      <c r="H73" s="20"/>
+      <c r="I73" s="20"/>
+      <c r="J73" s="20"/>
+      <c r="K73" s="20"/>
+      <c r="L73" s="20"/>
+      <c r="M73" s="20"/>
+      <c r="N73" s="20"/>
+      <c r="O73" s="20"/>
+      <c r="P73" s="20"/>
+      <c r="Q73" s="20"/>
+      <c r="R73" s="20"/>
+      <c r="S73" s="20"/>
+      <c r="T73" s="20"/>
+      <c r="U73" s="20"/>
       <c r="V73" s="10"/>
       <c r="W73" s="10"/>
       <c r="X73" s="10"/>
@@ -3902,26 +4180,26 @@
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A74" s="10"/>
-      <c r="B74" s="26"/>
-      <c r="C74" s="26"/>
-      <c r="D74" s="26"/>
-      <c r="E74" s="26"/>
-      <c r="F74" s="26"/>
-      <c r="G74" s="26"/>
-      <c r="H74" s="26"/>
-      <c r="I74" s="26"/>
-      <c r="J74" s="26"/>
-      <c r="K74" s="26"/>
-      <c r="L74" s="26"/>
-      <c r="M74" s="26"/>
-      <c r="N74" s="26"/>
-      <c r="O74" s="26"/>
-      <c r="P74" s="26"/>
-      <c r="Q74" s="26"/>
-      <c r="R74" s="26"/>
-      <c r="S74" s="26"/>
-      <c r="T74" s="26"/>
-      <c r="U74" s="26"/>
+      <c r="B74" s="20"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="20"/>
+      <c r="F74" s="20"/>
+      <c r="G74" s="20"/>
+      <c r="H74" s="20"/>
+      <c r="I74" s="20"/>
+      <c r="J74" s="20"/>
+      <c r="K74" s="20"/>
+      <c r="L74" s="20"/>
+      <c r="M74" s="20"/>
+      <c r="N74" s="20"/>
+      <c r="O74" s="20"/>
+      <c r="P74" s="20"/>
+      <c r="Q74" s="20"/>
+      <c r="R74" s="20"/>
+      <c r="S74" s="20"/>
+      <c r="T74" s="20"/>
+      <c r="U74" s="20"/>
       <c r="V74" s="10"/>
       <c r="W74" s="10"/>
       <c r="X74" s="10"/>
@@ -4126,26 +4404,26 @@
     </row>
     <row r="89" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A89" s="10"/>
-      <c r="B89" s="26"/>
-      <c r="C89" s="26"/>
-      <c r="D89" s="26"/>
-      <c r="E89" s="26"/>
-      <c r="F89" s="26"/>
-      <c r="G89" s="26"/>
-      <c r="H89" s="26"/>
-      <c r="I89" s="26"/>
-      <c r="J89" s="26"/>
-      <c r="K89" s="26"/>
-      <c r="L89" s="26"/>
-      <c r="M89" s="26"/>
-      <c r="N89" s="26"/>
-      <c r="O89" s="26"/>
-      <c r="P89" s="26"/>
-      <c r="Q89" s="26"/>
-      <c r="R89" s="26"/>
-      <c r="S89" s="26"/>
-      <c r="T89" s="26"/>
-      <c r="U89" s="26"/>
+      <c r="B89" s="20"/>
+      <c r="C89" s="20"/>
+      <c r="D89" s="20"/>
+      <c r="E89" s="20"/>
+      <c r="F89" s="20"/>
+      <c r="G89" s="20"/>
+      <c r="H89" s="20"/>
+      <c r="I89" s="20"/>
+      <c r="J89" s="20"/>
+      <c r="K89" s="20"/>
+      <c r="L89" s="20"/>
+      <c r="M89" s="20"/>
+      <c r="N89" s="20"/>
+      <c r="O89" s="20"/>
+      <c r="P89" s="20"/>
+      <c r="Q89" s="20"/>
+      <c r="R89" s="20"/>
+      <c r="S89" s="20"/>
+      <c r="T89" s="20"/>
+      <c r="U89" s="20"/>
       <c r="V89" s="10"/>
       <c r="W89" s="10"/>
       <c r="X89" s="10"/>
@@ -4156,26 +4434,26 @@
     </row>
     <row r="90" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A90" s="10"/>
-      <c r="B90" s="26"/>
-      <c r="C90" s="26"/>
-      <c r="D90" s="26"/>
-      <c r="E90" s="26"/>
-      <c r="F90" s="26"/>
-      <c r="G90" s="26"/>
-      <c r="H90" s="26"/>
-      <c r="I90" s="26"/>
-      <c r="J90" s="26"/>
-      <c r="K90" s="26"/>
-      <c r="L90" s="26"/>
-      <c r="M90" s="26"/>
-      <c r="N90" s="26"/>
-      <c r="O90" s="26"/>
-      <c r="P90" s="26"/>
-      <c r="Q90" s="26"/>
-      <c r="R90" s="26"/>
-      <c r="S90" s="26"/>
-      <c r="T90" s="26"/>
-      <c r="U90" s="26"/>
+      <c r="B90" s="20"/>
+      <c r="C90" s="20"/>
+      <c r="D90" s="20"/>
+      <c r="E90" s="20"/>
+      <c r="F90" s="20"/>
+      <c r="G90" s="20"/>
+      <c r="H90" s="20"/>
+      <c r="I90" s="20"/>
+      <c r="J90" s="20"/>
+      <c r="K90" s="20"/>
+      <c r="L90" s="20"/>
+      <c r="M90" s="20"/>
+      <c r="N90" s="20"/>
+      <c r="O90" s="20"/>
+      <c r="P90" s="20"/>
+      <c r="Q90" s="20"/>
+      <c r="R90" s="20"/>
+      <c r="S90" s="20"/>
+      <c r="T90" s="20"/>
+      <c r="U90" s="20"/>
       <c r="V90" s="10"/>
       <c r="W90" s="10"/>
       <c r="X90" s="10"/>
@@ -4366,26 +4644,26 @@
     </row>
     <row r="97" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A97" s="10"/>
-      <c r="B97" s="26"/>
-      <c r="C97" s="26"/>
-      <c r="D97" s="26"/>
-      <c r="E97" s="26"/>
-      <c r="F97" s="26"/>
-      <c r="G97" s="26"/>
-      <c r="H97" s="26"/>
-      <c r="I97" s="26"/>
-      <c r="J97" s="26"/>
-      <c r="K97" s="26"/>
-      <c r="L97" s="26"/>
-      <c r="M97" s="26"/>
-      <c r="N97" s="26"/>
-      <c r="O97" s="26"/>
-      <c r="P97" s="26"/>
-      <c r="Q97" s="26"/>
-      <c r="R97" s="26"/>
-      <c r="S97" s="26"/>
-      <c r="T97" s="26"/>
-      <c r="U97" s="26"/>
+      <c r="B97" s="20"/>
+      <c r="C97" s="20"/>
+      <c r="D97" s="20"/>
+      <c r="E97" s="20"/>
+      <c r="F97" s="20"/>
+      <c r="G97" s="20"/>
+      <c r="H97" s="20"/>
+      <c r="I97" s="20"/>
+      <c r="J97" s="20"/>
+      <c r="K97" s="20"/>
+      <c r="L97" s="20"/>
+      <c r="M97" s="20"/>
+      <c r="N97" s="20"/>
+      <c r="O97" s="20"/>
+      <c r="P97" s="20"/>
+      <c r="Q97" s="20"/>
+      <c r="R97" s="20"/>
+      <c r="S97" s="20"/>
+      <c r="T97" s="20"/>
+      <c r="U97" s="20"/>
       <c r="V97" s="10"/>
       <c r="W97" s="10"/>
       <c r="X97" s="10"/>
@@ -4396,26 +4674,26 @@
     </row>
     <row r="98" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A98" s="10"/>
-      <c r="B98" s="26"/>
-      <c r="C98" s="26"/>
-      <c r="D98" s="26"/>
-      <c r="E98" s="26"/>
-      <c r="F98" s="26"/>
-      <c r="G98" s="26"/>
-      <c r="H98" s="26"/>
-      <c r="I98" s="26"/>
-      <c r="J98" s="26"/>
-      <c r="K98" s="26"/>
-      <c r="L98" s="26"/>
-      <c r="M98" s="26"/>
-      <c r="N98" s="26"/>
-      <c r="O98" s="26"/>
-      <c r="P98" s="26"/>
-      <c r="Q98" s="26"/>
-      <c r="R98" s="26"/>
-      <c r="S98" s="26"/>
-      <c r="T98" s="26"/>
-      <c r="U98" s="26"/>
+      <c r="B98" s="20"/>
+      <c r="C98" s="20"/>
+      <c r="D98" s="20"/>
+      <c r="E98" s="20"/>
+      <c r="F98" s="20"/>
+      <c r="G98" s="20"/>
+      <c r="H98" s="20"/>
+      <c r="I98" s="20"/>
+      <c r="J98" s="20"/>
+      <c r="K98" s="20"/>
+      <c r="L98" s="20"/>
+      <c r="M98" s="20"/>
+      <c r="N98" s="20"/>
+      <c r="O98" s="20"/>
+      <c r="P98" s="20"/>
+      <c r="Q98" s="20"/>
+      <c r="R98" s="20"/>
+      <c r="S98" s="20"/>
+      <c r="T98" s="20"/>
+      <c r="U98" s="20"/>
       <c r="V98" s="10"/>
       <c r="W98" s="10"/>
       <c r="X98" s="10"/>
@@ -4606,26 +4884,26 @@
     </row>
     <row r="105" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A105" s="10"/>
-      <c r="B105" s="26"/>
-      <c r="C105" s="26"/>
-      <c r="D105" s="26"/>
-      <c r="E105" s="26"/>
-      <c r="F105" s="26"/>
-      <c r="G105" s="26"/>
-      <c r="H105" s="26"/>
-      <c r="I105" s="26"/>
-      <c r="J105" s="26"/>
-      <c r="K105" s="26"/>
-      <c r="L105" s="26"/>
-      <c r="M105" s="26"/>
-      <c r="N105" s="26"/>
-      <c r="O105" s="26"/>
-      <c r="P105" s="26"/>
-      <c r="Q105" s="26"/>
-      <c r="R105" s="26"/>
-      <c r="S105" s="26"/>
-      <c r="T105" s="26"/>
-      <c r="U105" s="26"/>
+      <c r="B105" s="20"/>
+      <c r="C105" s="20"/>
+      <c r="D105" s="20"/>
+      <c r="E105" s="20"/>
+      <c r="F105" s="20"/>
+      <c r="G105" s="20"/>
+      <c r="H105" s="20"/>
+      <c r="I105" s="20"/>
+      <c r="J105" s="20"/>
+      <c r="K105" s="20"/>
+      <c r="L105" s="20"/>
+      <c r="M105" s="20"/>
+      <c r="N105" s="20"/>
+      <c r="O105" s="20"/>
+      <c r="P105" s="20"/>
+      <c r="Q105" s="20"/>
+      <c r="R105" s="20"/>
+      <c r="S105" s="20"/>
+      <c r="T105" s="20"/>
+      <c r="U105" s="20"/>
       <c r="V105" s="10"/>
       <c r="W105" s="10"/>
       <c r="X105" s="10"/>
@@ -4636,26 +4914,26 @@
     </row>
     <row r="106" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A106" s="10"/>
-      <c r="B106" s="26"/>
-      <c r="C106" s="26"/>
-      <c r="D106" s="26"/>
-      <c r="E106" s="26"/>
-      <c r="F106" s="26"/>
-      <c r="G106" s="26"/>
-      <c r="H106" s="26"/>
-      <c r="I106" s="26"/>
-      <c r="J106" s="26"/>
-      <c r="K106" s="26"/>
-      <c r="L106" s="26"/>
-      <c r="M106" s="26"/>
-      <c r="N106" s="26"/>
-      <c r="O106" s="26"/>
-      <c r="P106" s="26"/>
-      <c r="Q106" s="26"/>
-      <c r="R106" s="26"/>
-      <c r="S106" s="26"/>
-      <c r="T106" s="26"/>
-      <c r="U106" s="26"/>
+      <c r="B106" s="20"/>
+      <c r="C106" s="20"/>
+      <c r="D106" s="20"/>
+      <c r="E106" s="20"/>
+      <c r="F106" s="20"/>
+      <c r="G106" s="20"/>
+      <c r="H106" s="20"/>
+      <c r="I106" s="20"/>
+      <c r="J106" s="20"/>
+      <c r="K106" s="20"/>
+      <c r="L106" s="20"/>
+      <c r="M106" s="20"/>
+      <c r="N106" s="20"/>
+      <c r="O106" s="20"/>
+      <c r="P106" s="20"/>
+      <c r="Q106" s="20"/>
+      <c r="R106" s="20"/>
+      <c r="S106" s="20"/>
+      <c r="T106" s="20"/>
+      <c r="U106" s="20"/>
       <c r="V106" s="10"/>
       <c r="W106" s="10"/>
       <c r="X106" s="10"/>
@@ -4846,26 +5124,26 @@
     </row>
     <row r="113" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A113" s="10"/>
-      <c r="B113" s="26"/>
-      <c r="C113" s="26"/>
-      <c r="D113" s="26"/>
-      <c r="E113" s="26"/>
-      <c r="F113" s="26"/>
-      <c r="G113" s="26"/>
-      <c r="H113" s="26"/>
-      <c r="I113" s="26"/>
-      <c r="J113" s="26"/>
-      <c r="K113" s="26"/>
-      <c r="L113" s="26"/>
-      <c r="M113" s="26"/>
-      <c r="N113" s="26"/>
-      <c r="O113" s="26"/>
-      <c r="P113" s="26"/>
-      <c r="Q113" s="26"/>
-      <c r="R113" s="26"/>
-      <c r="S113" s="26"/>
-      <c r="T113" s="26"/>
-      <c r="U113" s="26"/>
+      <c r="B113" s="20"/>
+      <c r="C113" s="20"/>
+      <c r="D113" s="20"/>
+      <c r="E113" s="20"/>
+      <c r="F113" s="20"/>
+      <c r="G113" s="20"/>
+      <c r="H113" s="20"/>
+      <c r="I113" s="20"/>
+      <c r="J113" s="20"/>
+      <c r="K113" s="20"/>
+      <c r="L113" s="20"/>
+      <c r="M113" s="20"/>
+      <c r="N113" s="20"/>
+      <c r="O113" s="20"/>
+      <c r="P113" s="20"/>
+      <c r="Q113" s="20"/>
+      <c r="R113" s="20"/>
+      <c r="S113" s="20"/>
+      <c r="T113" s="20"/>
+      <c r="U113" s="20"/>
       <c r="V113" s="10"/>
       <c r="W113" s="10"/>
       <c r="X113" s="10"/>
@@ -4876,26 +5154,26 @@
     </row>
     <row r="114" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A114" s="10"/>
-      <c r="B114" s="26"/>
-      <c r="C114" s="26"/>
-      <c r="D114" s="26"/>
-      <c r="E114" s="26"/>
-      <c r="F114" s="26"/>
-      <c r="G114" s="26"/>
-      <c r="H114" s="26"/>
-      <c r="I114" s="26"/>
-      <c r="J114" s="26"/>
-      <c r="K114" s="26"/>
-      <c r="L114" s="26"/>
-      <c r="M114" s="26"/>
-      <c r="N114" s="26"/>
-      <c r="O114" s="26"/>
-      <c r="P114" s="26"/>
-      <c r="Q114" s="26"/>
-      <c r="R114" s="26"/>
-      <c r="S114" s="26"/>
-      <c r="T114" s="26"/>
-      <c r="U114" s="26"/>
+      <c r="B114" s="20"/>
+      <c r="C114" s="20"/>
+      <c r="D114" s="20"/>
+      <c r="E114" s="20"/>
+      <c r="F114" s="20"/>
+      <c r="G114" s="20"/>
+      <c r="H114" s="20"/>
+      <c r="I114" s="20"/>
+      <c r="J114" s="20"/>
+      <c r="K114" s="20"/>
+      <c r="L114" s="20"/>
+      <c r="M114" s="20"/>
+      <c r="N114" s="20"/>
+      <c r="O114" s="20"/>
+      <c r="P114" s="20"/>
+      <c r="Q114" s="20"/>
+      <c r="R114" s="20"/>
+      <c r="S114" s="20"/>
+      <c r="T114" s="20"/>
+      <c r="U114" s="20"/>
       <c r="V114" s="10"/>
       <c r="W114" s="10"/>
       <c r="X114" s="10"/>
@@ -4911,9 +5189,9 @@
       <c r="D115" s="10"/>
       <c r="E115" s="10"/>
       <c r="F115" s="10"/>
-      <c r="G115" s="26"/>
-      <c r="H115" s="26"/>
-      <c r="I115" s="26"/>
+      <c r="G115" s="20"/>
+      <c r="H115" s="20"/>
+      <c r="I115" s="20"/>
       <c r="J115" s="10"/>
       <c r="K115" s="10"/>
       <c r="L115" s="10"/>
@@ -4941,9 +5219,9 @@
       <c r="D116" s="10"/>
       <c r="E116" s="10"/>
       <c r="F116" s="10"/>
-      <c r="G116" s="26"/>
-      <c r="H116" s="26"/>
-      <c r="I116" s="26"/>
+      <c r="G116" s="20"/>
+      <c r="H116" s="20"/>
+      <c r="I116" s="20"/>
       <c r="J116" s="10"/>
       <c r="K116" s="10"/>
       <c r="L116" s="10"/>
@@ -4980,10 +5258,10 @@
       <c r="M117" s="10"/>
       <c r="N117" s="10"/>
       <c r="O117" s="10"/>
-      <c r="P117" s="26"/>
-      <c r="Q117" s="26"/>
-      <c r="R117" s="26"/>
-      <c r="S117" s="26"/>
+      <c r="P117" s="20"/>
+      <c r="Q117" s="20"/>
+      <c r="R117" s="20"/>
+      <c r="S117" s="20"/>
       <c r="T117" s="10"/>
       <c r="U117" s="10"/>
       <c r="V117" s="10"/>
@@ -5010,10 +5288,10 @@
       <c r="M118" s="10"/>
       <c r="N118" s="10"/>
       <c r="O118" s="10"/>
-      <c r="P118" s="26"/>
-      <c r="Q118" s="26"/>
-      <c r="R118" s="26"/>
-      <c r="S118" s="26"/>
+      <c r="P118" s="20"/>
+      <c r="Q118" s="20"/>
+      <c r="R118" s="20"/>
+      <c r="S118" s="20"/>
       <c r="T118" s="10"/>
       <c r="U118" s="10"/>
       <c r="V118" s="10"/>
@@ -5086,26 +5364,26 @@
     </row>
     <row r="121" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A121" s="10"/>
-      <c r="B121" s="26"/>
-      <c r="C121" s="26"/>
-      <c r="D121" s="26"/>
-      <c r="E121" s="26"/>
-      <c r="F121" s="26"/>
-      <c r="G121" s="26"/>
-      <c r="H121" s="26"/>
-      <c r="I121" s="26"/>
-      <c r="J121" s="26"/>
-      <c r="K121" s="26"/>
-      <c r="L121" s="26"/>
-      <c r="M121" s="26"/>
-      <c r="N121" s="26"/>
-      <c r="O121" s="26"/>
-      <c r="P121" s="26"/>
-      <c r="Q121" s="26"/>
-      <c r="R121" s="26"/>
-      <c r="S121" s="26"/>
-      <c r="T121" s="26"/>
-      <c r="U121" s="26"/>
+      <c r="B121" s="20"/>
+      <c r="C121" s="20"/>
+      <c r="D121" s="20"/>
+      <c r="E121" s="20"/>
+      <c r="F121" s="20"/>
+      <c r="G121" s="20"/>
+      <c r="H121" s="20"/>
+      <c r="I121" s="20"/>
+      <c r="J121" s="20"/>
+      <c r="K121" s="20"/>
+      <c r="L121" s="20"/>
+      <c r="M121" s="20"/>
+      <c r="N121" s="20"/>
+      <c r="O121" s="20"/>
+      <c r="P121" s="20"/>
+      <c r="Q121" s="20"/>
+      <c r="R121" s="20"/>
+      <c r="S121" s="20"/>
+      <c r="T121" s="20"/>
+      <c r="U121" s="20"/>
       <c r="V121" s="10"/>
       <c r="W121" s="10"/>
       <c r="X121" s="10"/>
@@ -5116,26 +5394,26 @@
     </row>
     <row r="122" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A122" s="10"/>
-      <c r="B122" s="26"/>
-      <c r="C122" s="26"/>
-      <c r="D122" s="26"/>
-      <c r="E122" s="26"/>
-      <c r="F122" s="26"/>
-      <c r="G122" s="26"/>
-      <c r="H122" s="26"/>
-      <c r="I122" s="26"/>
-      <c r="J122" s="26"/>
-      <c r="K122" s="26"/>
-      <c r="L122" s="26"/>
-      <c r="M122" s="26"/>
-      <c r="N122" s="26"/>
-      <c r="O122" s="26"/>
-      <c r="P122" s="26"/>
-      <c r="Q122" s="26"/>
-      <c r="R122" s="26"/>
-      <c r="S122" s="26"/>
-      <c r="T122" s="26"/>
-      <c r="U122" s="26"/>
+      <c r="B122" s="20"/>
+      <c r="C122" s="20"/>
+      <c r="D122" s="20"/>
+      <c r="E122" s="20"/>
+      <c r="F122" s="20"/>
+      <c r="G122" s="20"/>
+      <c r="H122" s="20"/>
+      <c r="I122" s="20"/>
+      <c r="J122" s="20"/>
+      <c r="K122" s="20"/>
+      <c r="L122" s="20"/>
+      <c r="M122" s="20"/>
+      <c r="N122" s="20"/>
+      <c r="O122" s="20"/>
+      <c r="P122" s="20"/>
+      <c r="Q122" s="20"/>
+      <c r="R122" s="20"/>
+      <c r="S122" s="20"/>
+      <c r="T122" s="20"/>
+      <c r="U122" s="20"/>
       <c r="V122" s="10"/>
       <c r="W122" s="10"/>
       <c r="X122" s="10"/>
@@ -5326,26 +5604,26 @@
     </row>
     <row r="129" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A129" s="10"/>
-      <c r="B129" s="26"/>
-      <c r="C129" s="26"/>
-      <c r="D129" s="26"/>
-      <c r="E129" s="26"/>
-      <c r="F129" s="26"/>
-      <c r="G129" s="26"/>
-      <c r="H129" s="26"/>
-      <c r="I129" s="26"/>
-      <c r="J129" s="26"/>
-      <c r="K129" s="26"/>
-      <c r="L129" s="26"/>
-      <c r="M129" s="26"/>
-      <c r="N129" s="26"/>
-      <c r="O129" s="26"/>
-      <c r="P129" s="26"/>
-      <c r="Q129" s="26"/>
-      <c r="R129" s="26"/>
-      <c r="S129" s="26"/>
-      <c r="T129" s="26"/>
-      <c r="U129" s="26"/>
+      <c r="B129" s="20"/>
+      <c r="C129" s="20"/>
+      <c r="D129" s="20"/>
+      <c r="E129" s="20"/>
+      <c r="F129" s="20"/>
+      <c r="G129" s="20"/>
+      <c r="H129" s="20"/>
+      <c r="I129" s="20"/>
+      <c r="J129" s="20"/>
+      <c r="K129" s="20"/>
+      <c r="L129" s="20"/>
+      <c r="M129" s="20"/>
+      <c r="N129" s="20"/>
+      <c r="O129" s="20"/>
+      <c r="P129" s="20"/>
+      <c r="Q129" s="20"/>
+      <c r="R129" s="20"/>
+      <c r="S129" s="20"/>
+      <c r="T129" s="20"/>
+      <c r="U129" s="20"/>
       <c r="V129" s="10"/>
       <c r="W129" s="10"/>
       <c r="X129" s="10"/>
@@ -5356,26 +5634,26 @@
     </row>
     <row r="130" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A130" s="10"/>
-      <c r="B130" s="26"/>
-      <c r="C130" s="26"/>
-      <c r="D130" s="26"/>
-      <c r="E130" s="26"/>
-      <c r="F130" s="26"/>
-      <c r="G130" s="26"/>
-      <c r="H130" s="26"/>
-      <c r="I130" s="26"/>
-      <c r="J130" s="26"/>
-      <c r="K130" s="26"/>
-      <c r="L130" s="26"/>
-      <c r="M130" s="26"/>
-      <c r="N130" s="26"/>
-      <c r="O130" s="26"/>
-      <c r="P130" s="26"/>
-      <c r="Q130" s="26"/>
-      <c r="R130" s="26"/>
-      <c r="S130" s="26"/>
-      <c r="T130" s="26"/>
-      <c r="U130" s="26"/>
+      <c r="B130" s="20"/>
+      <c r="C130" s="20"/>
+      <c r="D130" s="20"/>
+      <c r="E130" s="20"/>
+      <c r="F130" s="20"/>
+      <c r="G130" s="20"/>
+      <c r="H130" s="20"/>
+      <c r="I130" s="20"/>
+      <c r="J130" s="20"/>
+      <c r="K130" s="20"/>
+      <c r="L130" s="20"/>
+      <c r="M130" s="20"/>
+      <c r="N130" s="20"/>
+      <c r="O130" s="20"/>
+      <c r="P130" s="20"/>
+      <c r="Q130" s="20"/>
+      <c r="R130" s="20"/>
+      <c r="S130" s="20"/>
+      <c r="T130" s="20"/>
+      <c r="U130" s="20"/>
       <c r="V130" s="10"/>
       <c r="W130" s="10"/>
       <c r="X130" s="10"/>
@@ -5683,7 +5961,16 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="22">
+    <mergeCell ref="B1:U2"/>
+    <mergeCell ref="B9:U10"/>
+    <mergeCell ref="B17:U18"/>
+    <mergeCell ref="B25:U26"/>
+    <mergeCell ref="B33:U34"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="R6:T6"/>
+    <mergeCell ref="C28:J28"/>
     <mergeCell ref="B73:U74"/>
     <mergeCell ref="B89:U90"/>
     <mergeCell ref="B97:U98"/>
@@ -5696,15 +5983,7 @@
     <mergeCell ref="P117:S117"/>
     <mergeCell ref="P118:S118"/>
     <mergeCell ref="B121:U122"/>
-    <mergeCell ref="B1:U2"/>
-    <mergeCell ref="B9:U10"/>
-    <mergeCell ref="B17:U18"/>
-    <mergeCell ref="B25:U26"/>
-    <mergeCell ref="B33:U34"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="R6:T6"/>
-    <mergeCell ref="C28:J28"/>
+    <mergeCell ref="B49:U50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>